<commit_message>
first attempt at refactor and repair
</commit_message>
<xml_diff>
--- a/blackjack.xlsx
+++ b/blackjack.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seanwo/projects/ti994a/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F063DB7A-AECB-3240-9162-11D7B12D275C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2A82851-207F-6549-833A-7614D8E5E506}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1700" yWindow="500" windowWidth="49500" windowHeight="28300" xr2:uid="{F2DCDACA-2E8A-E041-BEAE-FEED980AFD9D}"/>
   </bookViews>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="986" uniqueCount="813">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="992" uniqueCount="819">
   <si>
     <t>1</t>
   </si>
@@ -2393,12 +2393,6 @@
     <t>HANDS(1,0,0)=5 :: HANDS(1,1,0)=11 :: HANDS(1,2,0)=3 :: HANDS(1,3,0)=13 :: HANDS(1,4,0)=14</t>
   </si>
   <si>
-    <t>DISPLAY AT (1,26): PSCORE</t>
-  </si>
-  <si>
-    <t>DISPLAY AT (2,26):DSCORE</t>
-  </si>
-  <si>
     <t>IF PSCORE=SCORE THEN DISPLAY AT (12,10): "TIE GAME"</t>
   </si>
   <si>
@@ -2450,54 +2444,18 @@
     <t>DISPLAY AT (1, 1): "HOW TO PLAY:"</t>
   </si>
   <si>
-    <t>DISPLAY AT (1, 1): "RULES:"</t>
-  </si>
-  <si>
     <t>DISPLAY AT (3, 1): "BOTH YOU AND THE DEALER WILL"</t>
   </si>
   <si>
     <t>DISPLAY AT (4, 1): "BE GIVEN TWO CARDS TO START."</t>
   </si>
   <si>
-    <t>DISPLAY AT (5, 1): "THEN TAKE AS MANY CARDS AS"</t>
-  </si>
-  <si>
-    <t>DISPLAY AT (6, 1): "YOU WISH. IF YOUR HAND IS"</t>
-  </si>
-  <si>
-    <t>DISPLAY AT (7, 1): "OVER 21 YOU LOSE."</t>
-  </si>
-  <si>
     <t>DISPLAY AT (3, 1): "THIS IS A GAME BETWEEN YOU"</t>
   </si>
   <si>
     <t>DISPLAY AT (4, 1): "AND THE DEALER (COMPUTER)."</t>
   </si>
   <si>
-    <t>DISPLAY AT (6, 1): "OBJECT OF GAME:"</t>
-  </si>
-  <si>
-    <t>DISPLAY AT (8, 1): "THE OBJECT OF THIS GAME IS"</t>
-  </si>
-  <si>
-    <t>DISPLAY AT (9, 1): "TO COLLECT A SET OF CARDS"</t>
-  </si>
-  <si>
-    <t>DISPLAY AT (10, 1): "THAT IS LESS THAN OR EQUAL"</t>
-  </si>
-  <si>
-    <t>DISPLAY AT (11, 1): "TO 21. IF YOUR SET OF CARDS"</t>
-  </si>
-  <si>
-    <t>DISPLAY AT (12, 1): "IS HIGHER THAN THE DEALER'S"</t>
-  </si>
-  <si>
-    <t>DISPLAY AT (13, 1): "AND NOT OVER 21 THEN YOU WIN"</t>
-  </si>
-  <si>
-    <t>DISPLAY AT (15, 1): "VALUES:"</t>
-  </si>
-  <si>
     <t>DISPLAY AT (17, 1): "NUMBER CARDS = FACE VALUE"</t>
   </si>
   <si>
@@ -2511,6 +2469,66 @@
   </si>
   <si>
     <t>DISPLAY AT (24,1): "PRESS ENTER TO BEGIN:"</t>
+  </si>
+  <si>
+    <t>DISPLAY AT (8, 1): "THE OBJECT OF THE GAME IS TO"</t>
+  </si>
+  <si>
+    <t>DISPLAY AT (9, 1): "COLLECT A SET OF CARDS LESS"</t>
+  </si>
+  <si>
+    <t>DISPLAY AT (10, 1): "THAN OR EQUAL TO 21. IF YOUR"</t>
+  </si>
+  <si>
+    <t>DISPLAY AT (11, 1): "SET OF CARDS IS HIGHER THAN"</t>
+  </si>
+  <si>
+    <t>DISPLAY AT (12, 1): "THE DEALER'S AND NOT OVER 21"</t>
+  </si>
+  <si>
+    <t>DISPLAY AT (13, 1): "THEN YOU WIN."</t>
+  </si>
+  <si>
+    <t>DISPLAY AT (15, 1): "CARD VALUES:"</t>
+  </si>
+  <si>
+    <t>DISPLAY AT (6, 1): "OBJECT OF THE GAME:"</t>
+  </si>
+  <si>
+    <t>DISPLAY AT (1, 1): "PREFACE:"</t>
+  </si>
+  <si>
+    <t>DISPLAY AT (5, 1): "TAKE AS MANY CARDS AS YOU"</t>
+  </si>
+  <si>
+    <t>DISPLAY AT (6, 1): "WISH (UP TO 5 CARDS). IF"</t>
+  </si>
+  <si>
+    <t>DISPLAY AT (7, 1): "THE VALUE OF YOUR HAND"</t>
+  </si>
+  <si>
+    <t>DISPLAY AT (8, 1): "EXCEEDS 21 YOU BUST. ONCE"</t>
+  </si>
+  <si>
+    <t>DISPLAY AT (9, 1): "YOU STOP TAKING CARDS, THE"</t>
+  </si>
+  <si>
+    <t>DISPLAY AT (10, 1): "DEALER WILL TAKE CARDS"</t>
+  </si>
+  <si>
+    <t>DISPLAY AT (11, 1): "TRYING NOT TO BUST AS WELL."</t>
+  </si>
+  <si>
+    <t>DISPLAY AT (12, 1): "THE PLAYER WITH THE HIGHEST"</t>
+  </si>
+  <si>
+    <t>DISPLAY AT (13, 1): "HAND VALUE WINS."</t>
+  </si>
+  <si>
+    <t>DISPLAY AT (1,24): "P:"&amp;STR$(PSCORE)</t>
+  </si>
+  <si>
+    <t>DISPLAY AT (2,24):"D:"&amp;STR$(DSCORE)</t>
   </si>
 </sst>
 </file>
@@ -2697,7 +2715,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -2724,8 +2742,6 @@
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -3062,7 +3078,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AB3D0CF-00CA-1047-A168-192C0697CE9E}">
-  <dimension ref="A1:D284"/>
+  <dimension ref="A1:D290"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -3089,7 +3105,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="28"/>
+      <c r="A2" s="26"/>
       <c r="B2">
         <v>100</v>
       </c>
@@ -3102,7 +3118,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="28"/>
+      <c r="A3" s="26"/>
       <c r="B3">
         <v>110</v>
       </c>
@@ -3116,7 +3132,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="28"/>
+      <c r="A4" s="26"/>
       <c r="B4">
         <v>120</v>
       </c>
@@ -3125,7 +3141,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="28"/>
+      <c r="A5" s="26"/>
       <c r="B5">
         <v>130</v>
       </c>
@@ -3134,7 +3150,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="28"/>
+      <c r="A6" s="26"/>
       <c r="B6">
         <v>140</v>
       </c>
@@ -3143,7 +3159,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="28"/>
+      <c r="A7" s="26"/>
       <c r="B7">
         <v>150</v>
       </c>
@@ -3152,35 +3168,35 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="28"/>
+      <c r="A8" s="26"/>
       <c r="B8">
         <v>160</v>
       </c>
       <c r="C8" t="str">
         <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D8,A:A,0),0)," :: REM CALL ",D8,"")</f>
-        <v>GOSUB 540 :: REM CALL SETCHARS</v>
+        <v>GOSUB 600 :: REM CALL SETCHARS</v>
       </c>
       <c r="D8" t="str">
-        <f>A46</f>
+        <f>A52</f>
         <v>SETCHARS</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="28"/>
+      <c r="A9" s="26"/>
       <c r="B9">
         <v>170</v>
       </c>
       <c r="C9" t="str">
         <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D9,A:A,0),0)," :: REM CALL ",D9,"")</f>
-        <v>GOSUB 990 :: REM CALL SETCOLORSCHEME</v>
+        <v>GOSUB 1050 :: REM CALL SETCOLORSCHEME</v>
       </c>
       <c r="D9" t="str">
-        <f>A91</f>
+        <f>A97</f>
         <v>SETCOLORSCHEME</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="29" t="s">
+      <c r="A10" s="27" t="s">
         <v>763</v>
       </c>
       <c r="B10">
@@ -3192,53 +3208,53 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="28"/>
+      <c r="A11" s="26"/>
       <c r="B11">
         <v>190</v>
       </c>
       <c r="C11" t="str">
         <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D11,A:A,0),0)," :: REM CALL ",D11,"")</f>
-        <v>GOSUB 2260 :: REM CALL PLAY</v>
+        <v>GOSUB 2320 :: REM CALL PLAY</v>
       </c>
       <c r="D11" t="str">
-        <f>A218</f>
+        <f>A224</f>
         <v>PLAY</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="28"/>
+      <c r="A12" s="26"/>
       <c r="B12">
         <v>200</v>
       </c>
-      <c r="C12" s="26" t="s">
+      <c r="C12" t="s">
         <v>430</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="28"/>
+      <c r="A13" s="26"/>
       <c r="B13">
         <v>210</v>
       </c>
-      <c r="C13" s="26" t="s">
+      <c r="C13" t="s">
         <v>432</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="28"/>
+      <c r="A14" s="26"/>
       <c r="B14">
         <v>220</v>
       </c>
-      <c r="C14" s="26" t="str" cm="1">
+      <c r="C14" t="str" cm="1">
         <f t="array" ref="C14">CONCATENATE("IF A$=""N"" THEN GOSUB ",INDEX(B:B,MATCH(D14,A:A,0),0)," :: REM CALL ",D14,"")</f>
-        <v>IF A$="N" THEN GOSUB 2880 :: REM CALL TERMINATE</v>
+        <v>IF A$="N" THEN GOSUB 2940 :: REM CALL TERMINATE</v>
       </c>
       <c r="D14" t="str">
-        <f>A280</f>
+        <f>A286</f>
         <v>TERMINATE</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="28"/>
+      <c r="A15" s="26"/>
       <c r="B15">
         <v>230</v>
       </c>
@@ -3252,7 +3268,7 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="28" t="s">
+      <c r="A16" s="26" t="s">
         <v>501</v>
       </c>
       <c r="B16">
@@ -3264,7 +3280,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="28"/>
+      <c r="A17" s="26"/>
       <c r="B17">
         <v>250</v>
       </c>
@@ -3273,7 +3289,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="28"/>
+      <c r="A18" s="26"/>
       <c r="B18">
         <v>260</v>
       </c>
@@ -3282,7 +3298,7 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="28"/>
+      <c r="A19" s="26"/>
       <c r="B19">
         <v>270</v>
       </c>
@@ -3291,151 +3307,151 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="28"/>
+      <c r="A20" s="26"/>
       <c r="B20">
         <v>280</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>792</v>
+        <v>807</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="28"/>
+      <c r="A21" s="26"/>
       <c r="B21">
         <v>290</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>798</v>
+        <v>792</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="28"/>
+      <c r="A22" s="26"/>
       <c r="B22">
         <v>300</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>799</v>
+        <v>793</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="28"/>
+      <c r="A23" s="26"/>
       <c r="B23">
         <v>310</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>800</v>
+        <v>806</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="28"/>
+      <c r="A24" s="26"/>
       <c r="B24">
         <v>320</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="28"/>
+      <c r="A25" s="26"/>
       <c r="B25">
         <v>330</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="28"/>
+      <c r="A26" s="26"/>
       <c r="B26">
         <v>340</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="28"/>
+      <c r="A27" s="26"/>
       <c r="B27">
         <v>350</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="28"/>
+      <c r="A28" s="26"/>
       <c r="B28">
         <v>360</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="28"/>
+      <c r="A29" s="26"/>
       <c r="B29">
         <v>370</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" s="28"/>
+      <c r="A30" s="26"/>
       <c r="B30">
         <v>380</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" s="28"/>
+      <c r="A31" s="26"/>
       <c r="B31">
         <v>390</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>808</v>
+        <v>794</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" s="28"/>
+      <c r="A32" s="26"/>
       <c r="B32">
         <v>400</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>809</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="28"/>
+        <v>795</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="26"/>
       <c r="B33">
         <v>410</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>810</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" s="28"/>
+        <v>796</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="26"/>
       <c r="B34">
         <v>420</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>811</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="28"/>
+        <v>797</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="26"/>
       <c r="B35">
         <v>430</v>
       </c>
       <c r="C35" s="11" t="s">
-        <v>790</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="28"/>
+        <v>788</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="26"/>
       <c r="B36">
         <v>440</v>
       </c>
@@ -3443,330 +3459,322 @@
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="28"/>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="26"/>
       <c r="B37">
         <v>450</v>
       </c>
       <c r="C37" s="11" t="s">
-        <v>791</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="28"/>
+        <v>789</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="26"/>
       <c r="B38">
         <v>460</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>793</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" s="28"/>
+        <v>790</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" s="26"/>
       <c r="B39">
         <v>470</v>
       </c>
       <c r="C39" s="11" t="s">
-        <v>794</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" s="28"/>
+        <v>791</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" s="26"/>
       <c r="B40">
         <v>480</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>795</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" s="28"/>
+        <v>808</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" s="26"/>
       <c r="B41">
         <v>490</v>
       </c>
       <c r="C41" s="11" t="s">
-        <v>796</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" s="28"/>
+        <v>809</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" s="26"/>
       <c r="B42">
         <v>500</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>797</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" s="28"/>
+        <v>810</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" s="26"/>
       <c r="B43">
         <v>510</v>
       </c>
       <c r="C43" s="11" t="s">
-        <v>812</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" s="28"/>
+        <v>811</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" s="26"/>
       <c r="B44">
         <v>520</v>
       </c>
       <c r="C44" s="11" t="s">
-        <v>790</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="28"/>
+        <v>812</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" s="26"/>
       <c r="B45">
         <v>530</v>
       </c>
       <c r="C45" s="11" t="s">
-        <v>662</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" s="28" t="s">
-        <v>663</v>
-      </c>
+        <v>813</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" s="26"/>
       <c r="B46">
         <v>540</v>
       </c>
-      <c r="C46" s="11" t="str">
-        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A46,"***")</f>
-        <v>REM SUBROUTINE ***SETCHARS***</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" s="28"/>
+      <c r="C46" s="11" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" s="26"/>
       <c r="B47">
         <v>550</v>
       </c>
       <c r="C47" s="11" t="s">
-        <v>701</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A48" s="28"/>
+        <v>815</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" s="26"/>
       <c r="B48">
         <v>560</v>
       </c>
-      <c r="C48" t="str">
-        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D48,A:A,0),0)," :: REM CALL ",D48,"")</f>
-        <v>GOSUB 640 :: REM CALL SETCHARSREDSUIT</v>
-      </c>
-      <c r="D48" t="str">
-        <f>A56</f>
-        <v>SETCHARSREDSUIT</v>
+      <c r="C48" s="11" t="s">
+        <v>816</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" s="28"/>
+      <c r="A49" s="26"/>
       <c r="B49">
         <v>570</v>
       </c>
       <c r="C49" s="11" t="s">
-        <v>702</v>
+        <v>798</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" s="28"/>
+      <c r="A50" s="26"/>
       <c r="B50">
         <v>580</v>
       </c>
-      <c r="C50" t="str">
-        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D50,A:A,0),0)," :: REM CALL ",D50,"")</f>
-        <v>GOSUB 720 :: REM CALL SETCHARSBLACKSUIT</v>
-      </c>
-      <c r="D50" t="str">
-        <f>A64</f>
-        <v>SETCHARSBLACKSUIT</v>
+      <c r="C50" s="11" t="s">
+        <v>788</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" s="28"/>
+      <c r="A51" s="26"/>
       <c r="B51">
         <v>590</v>
       </c>
       <c r="C51" s="11" t="s">
-        <v>703</v>
+        <v>662</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A52" s="28"/>
+      <c r="A52" s="26" t="s">
+        <v>663</v>
+      </c>
       <c r="B52">
         <v>600</v>
       </c>
-      <c r="C52" t="str">
-        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D52,A:A,0),0)," :: REM CALL ",D52,"")</f>
-        <v>GOSUB 940 :: REM CALL SETCHARSEDGES</v>
-      </c>
-      <c r="D52" t="str">
-        <f>A86</f>
-        <v>SETCHARSEDGES</v>
+      <c r="C52" s="11" t="str">
+        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A52,"***")</f>
+        <v>REM SUBROUTINE ***SETCHARS***</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53" s="28"/>
+      <c r="A53" s="26"/>
       <c r="B53">
         <v>610</v>
       </c>
       <c r="C53" s="11" t="s">
-        <v>704</v>
+        <v>701</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A54" s="28"/>
+      <c r="A54" s="26"/>
       <c r="B54">
         <v>620</v>
       </c>
-      <c r="C54" t="s">
-        <v>692</v>
+      <c r="C54" t="str">
+        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D54,A:A,0),0)," :: REM CALL ",D54,"")</f>
+        <v>GOSUB 700 :: REM CALL SETCHARSREDSUIT</v>
+      </c>
+      <c r="D54" t="str">
+        <f>A62</f>
+        <v>SETCHARSREDSUIT</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A55" s="28"/>
+      <c r="A55" s="26"/>
       <c r="B55">
         <v>630</v>
       </c>
       <c r="C55" s="11" t="s">
-        <v>662</v>
+        <v>702</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56" s="28" t="s">
-        <v>689</v>
-      </c>
+      <c r="A56" s="26"/>
       <c r="B56">
         <v>640</v>
       </c>
-      <c r="C56" s="11" t="str">
-        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A56,"***")</f>
-        <v>REM SUBROUTINE ***SETCHARSREDSUIT***</v>
+      <c r="C56" t="str">
+        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D56,A:A,0),0)," :: REM CALL ",D56,"")</f>
+        <v>GOSUB 780 :: REM CALL SETCHARSBLACKSUIT</v>
+      </c>
+      <c r="D56" t="str">
+        <f>A70</f>
+        <v>SETCHARSBLACKSUIT</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57" s="28"/>
+      <c r="A57" s="26"/>
       <c r="B57">
         <v>650</v>
       </c>
       <c r="C57" s="11" t="s">
-        <v>666</v>
+        <v>703</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58" s="28"/>
+      <c r="A58" s="26"/>
       <c r="B58">
         <v>660</v>
       </c>
-      <c r="C58" t="s">
-        <v>680</v>
+      <c r="C58" t="str">
+        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D58,A:A,0),0)," :: REM CALL ",D58,"")</f>
+        <v>GOSUB 1000 :: REM CALL SETCHARSEDGES</v>
+      </c>
+      <c r="D58" t="str">
+        <f>A92</f>
+        <v>SETCHARSEDGES</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" s="28"/>
+      <c r="A59" s="26"/>
       <c r="B59">
         <v>670</v>
       </c>
-      <c r="C59" t="s">
-        <v>710</v>
+      <c r="C59" s="11" t="s">
+        <v>704</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A60" s="28"/>
+      <c r="A60" s="26"/>
       <c r="B60">
         <v>680</v>
       </c>
-      <c r="C60" t="str">
-        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D60,A:A,0),0)," :: REM CALL ",D60,"")</f>
-        <v>GOSUB 780 :: REM CALL SETCHARSVALS</v>
-      </c>
-      <c r="D60" t="str">
-        <f>A70</f>
-        <v>SETCHARSVALS</v>
+      <c r="C60" t="s">
+        <v>692</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A61" s="28"/>
+      <c r="A61" s="26"/>
       <c r="B61">
         <v>690</v>
       </c>
-      <c r="C61" t="s">
-        <v>686</v>
+      <c r="C61" s="11" t="s">
+        <v>662</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A62" s="28"/>
+      <c r="A62" s="26" t="s">
+        <v>689</v>
+      </c>
       <c r="B62">
         <v>700</v>
       </c>
-      <c r="C62" t="s">
-        <v>683</v>
+      <c r="C62" s="11" t="str">
+        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A62,"***")</f>
+        <v>REM SUBROUTINE ***SETCHARSREDSUIT***</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A63" s="28"/>
+      <c r="A63" s="26"/>
       <c r="B63">
         <v>710</v>
       </c>
-      <c r="C63" t="s">
-        <v>662</v>
+      <c r="C63" s="11" t="s">
+        <v>666</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A64" s="28" t="s">
-        <v>690</v>
-      </c>
+      <c r="A64" s="26"/>
       <c r="B64">
         <v>720</v>
       </c>
-      <c r="C64" s="11" t="str">
-        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A64,"***")</f>
-        <v>REM SUBROUTINE ***SETCHARSBLACKSUIT***</v>
+      <c r="C64" t="s">
+        <v>680</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A65" s="28"/>
+      <c r="A65" s="26"/>
       <c r="B65">
         <v>730</v>
       </c>
-      <c r="C65" s="11" t="s">
-        <v>682</v>
+      <c r="C65" t="s">
+        <v>710</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A66" s="28"/>
+      <c r="A66" s="26"/>
       <c r="B66">
         <v>740</v>
       </c>
-      <c r="C66" t="s">
-        <v>681</v>
+      <c r="C66" t="str">
+        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D66,A:A,0),0)," :: REM CALL ",D66,"")</f>
+        <v>GOSUB 840 :: REM CALL SETCHARSVALS</v>
+      </c>
+      <c r="D66" t="str">
+        <f>A76</f>
+        <v>SETCHARSVALS</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A67" s="28"/>
+      <c r="A67" s="26"/>
       <c r="B67">
         <v>750</v>
       </c>
       <c r="C67" t="s">
-        <v>711</v>
+        <v>686</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A68" s="28"/>
+      <c r="A68" s="26"/>
       <c r="B68">
         <v>760</v>
       </c>
-      <c r="C68" t="str">
-        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D68,A:A,0),0)," :: REM CALL ",D68,"")</f>
-        <v>GOSUB 780 :: REM CALL SETCHARSVALS</v>
-      </c>
-      <c r="D68" t="str">
-        <f>A70</f>
-        <v>SETCHARSVALS</v>
+      <c r="C68" t="s">
+        <v>683</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A69" s="28"/>
+      <c r="A69" s="26"/>
       <c r="B69">
         <v>770</v>
       </c>
@@ -3775,632 +3783,637 @@
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A70" s="28" t="s">
-        <v>665</v>
+      <c r="A70" s="26" t="s">
+        <v>690</v>
       </c>
       <c r="B70">
         <v>780</v>
       </c>
       <c r="C70" s="11" t="str">
         <f>_xlfn.CONCAT("REM SUBROUTINE ***",A70,"***")</f>
-        <v>REM SUBROUTINE ***SETCHARSVALS***</v>
+        <v>REM SUBROUTINE ***SETCHARSBLACKSUIT***</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A71" s="28"/>
+      <c r="A71" s="26"/>
       <c r="B71">
         <v>790</v>
       </c>
       <c r="C71" s="11" t="s">
-        <v>664</v>
+        <v>682</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A72" s="28"/>
+      <c r="A72" s="26"/>
       <c r="B72">
         <v>800</v>
       </c>
       <c r="C72" t="s">
-        <v>667</v>
+        <v>681</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A73" s="28"/>
+      <c r="A73" s="26"/>
       <c r="B73">
         <v>810</v>
       </c>
       <c r="C73" t="s">
-        <v>668</v>
+        <v>711</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A74" s="28"/>
+      <c r="A74" s="26"/>
       <c r="B74">
         <v>820</v>
       </c>
-      <c r="C74" t="s">
-        <v>669</v>
+      <c r="C74" t="str">
+        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D74,A:A,0),0)," :: REM CALL ",D74,"")</f>
+        <v>GOSUB 840 :: REM CALL SETCHARSVALS</v>
+      </c>
+      <c r="D74" t="str">
+        <f>A76</f>
+        <v>SETCHARSVALS</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A75" s="28"/>
+      <c r="A75" s="26"/>
       <c r="B75">
         <v>830</v>
       </c>
       <c r="C75" t="s">
-        <v>670</v>
+        <v>662</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A76" s="28"/>
+      <c r="A76" s="26" t="s">
+        <v>665</v>
+      </c>
       <c r="B76">
         <v>840</v>
       </c>
-      <c r="C76" t="s">
-        <v>671</v>
+      <c r="C76" s="11" t="str">
+        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A76,"***")</f>
+        <v>REM SUBROUTINE ***SETCHARSVALS***</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A77" s="28"/>
+      <c r="A77" s="26"/>
       <c r="B77">
         <v>850</v>
       </c>
-      <c r="C77" t="s">
-        <v>672</v>
+      <c r="C77" s="11" t="s">
+        <v>664</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A78" s="28"/>
+      <c r="A78" s="26"/>
       <c r="B78">
         <v>860</v>
       </c>
       <c r="C78" t="s">
-        <v>673</v>
+        <v>667</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A79" s="28"/>
+      <c r="A79" s="26"/>
       <c r="B79">
         <v>870</v>
       </c>
       <c r="C79" t="s">
-        <v>674</v>
+        <v>668</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A80" s="28"/>
+      <c r="A80" s="26"/>
       <c r="B80">
         <v>880</v>
       </c>
       <c r="C80" t="s">
-        <v>675</v>
+        <v>669</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A81" s="28"/>
+      <c r="A81" s="26"/>
       <c r="B81">
         <v>890</v>
       </c>
       <c r="C81" t="s">
-        <v>676</v>
+        <v>670</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A82" s="28"/>
+      <c r="A82" s="26"/>
       <c r="B82">
         <v>900</v>
       </c>
       <c r="C82" t="s">
-        <v>677</v>
+        <v>671</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A83" s="28"/>
+      <c r="A83" s="26"/>
       <c r="B83">
         <v>910</v>
       </c>
       <c r="C83" t="s">
-        <v>678</v>
+        <v>672</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A84" s="28"/>
+      <c r="A84" s="26"/>
       <c r="B84">
         <v>920</v>
       </c>
       <c r="C84" t="s">
-        <v>679</v>
+        <v>673</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A85" s="28"/>
+      <c r="A85" s="26"/>
       <c r="B85">
         <v>930</v>
       </c>
       <c r="C85" t="s">
-        <v>662</v>
+        <v>674</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A86" s="28" t="s">
-        <v>684</v>
-      </c>
+      <c r="A86" s="26"/>
       <c r="B86">
         <v>940</v>
       </c>
-      <c r="C86" s="11" t="str">
-        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A86,"***")</f>
-        <v>REM SUBROUTINE ***SETCHARSEDGES***</v>
+      <c r="C86" t="s">
+        <v>675</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A87" s="28"/>
+      <c r="A87" s="26"/>
       <c r="B87">
         <v>950</v>
       </c>
-      <c r="C87" s="11" t="s">
-        <v>685</v>
+      <c r="C87" t="s">
+        <v>676</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A88" s="28"/>
+      <c r="A88" s="26"/>
       <c r="B88">
         <v>960</v>
       </c>
       <c r="C88" t="s">
-        <v>687</v>
+        <v>677</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A89" s="28"/>
+      <c r="A89" s="26"/>
       <c r="B89">
         <v>970</v>
       </c>
       <c r="C89" t="s">
-        <v>688</v>
+        <v>678</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A90" s="28"/>
+      <c r="A90" s="26"/>
       <c r="B90">
         <v>980</v>
       </c>
       <c r="C90" t="s">
-        <v>662</v>
+        <v>679</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A91" s="28" t="s">
-        <v>694</v>
-      </c>
+      <c r="A91" s="26"/>
       <c r="B91">
         <v>990</v>
       </c>
-      <c r="C91" s="11" t="str">
-        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A91,"***")</f>
-        <v>REM SUBROUTINE ***SETCOLORSCHEME***</v>
+      <c r="C91" t="s">
+        <v>662</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A92" s="28"/>
+      <c r="A92" s="26" t="s">
+        <v>684</v>
+      </c>
       <c r="B92">
         <v>1000</v>
       </c>
-      <c r="C92" s="11" t="s">
-        <v>696</v>
+      <c r="C92" s="11" t="str">
+        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A92,"***")</f>
+        <v>REM SUBROUTINE ***SETCHARSEDGES***</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A93" s="28"/>
+      <c r="A93" s="26"/>
       <c r="B93">
         <v>1010</v>
       </c>
       <c r="C93" s="11" t="s">
-        <v>697</v>
+        <v>685</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A94" s="28"/>
+      <c r="A94" s="26"/>
       <c r="B94">
         <v>1020</v>
       </c>
-      <c r="C94" s="11" t="s">
-        <v>698</v>
+      <c r="C94" t="s">
+        <v>687</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A95" s="28"/>
+      <c r="A95" s="26"/>
       <c r="B95">
         <v>1030</v>
       </c>
-      <c r="C95" s="11" t="s">
-        <v>699</v>
+      <c r="C95" t="s">
+        <v>688</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A96" s="28"/>
+      <c r="A96" s="26"/>
       <c r="B96">
         <v>1040</v>
       </c>
-      <c r="C96" s="11" t="s">
-        <v>700</v>
+      <c r="C96" t="s">
+        <v>662</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A97" s="28"/>
+      <c r="A97" s="26" t="s">
+        <v>694</v>
+      </c>
       <c r="B97">
         <v>1050</v>
       </c>
-      <c r="C97" s="11" t="s">
-        <v>705</v>
+      <c r="C97" s="11" t="str">
+        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A97,"***")</f>
+        <v>REM SUBROUTINE ***SETCOLORSCHEME***</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A98" s="28"/>
+      <c r="A98" s="26"/>
       <c r="B98">
         <v>1060</v>
       </c>
       <c r="C98" s="11" t="s">
-        <v>706</v>
+        <v>696</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A99" s="28"/>
+      <c r="A99" s="26"/>
       <c r="B99">
         <v>1070</v>
       </c>
       <c r="C99" s="11" t="s">
-        <v>662</v>
+        <v>697</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A100" s="28" t="s">
-        <v>577</v>
-      </c>
+      <c r="A100" s="26"/>
       <c r="B100">
         <v>1080</v>
       </c>
-      <c r="C100" s="11" t="str">
-        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A100,"***")</f>
-        <v>REM SUBROUTINE ***RENDERCARD***</v>
+      <c r="C100" s="11" t="s">
+        <v>698</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A101" s="28"/>
+      <c r="A101" s="26"/>
       <c r="B101">
         <v>1090</v>
       </c>
       <c r="C101" s="11" t="s">
-        <v>723</v>
+        <v>699</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A102" s="28"/>
+      <c r="A102" s="26"/>
       <c r="B102">
         <v>1100</v>
       </c>
       <c r="C102" s="11" t="s">
-        <v>709</v>
+        <v>700</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A103" s="28"/>
+      <c r="A103" s="26"/>
       <c r="B103">
         <v>1110</v>
       </c>
       <c r="C103" s="11" t="s">
-        <v>712</v>
+        <v>705</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A104" s="28"/>
+      <c r="A104" s="26"/>
       <c r="B104">
         <v>1120</v>
       </c>
-      <c r="C104" t="s">
-        <v>130</v>
+      <c r="C104" s="11" t="s">
+        <v>706</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A105" s="28"/>
+      <c r="A105" s="26"/>
       <c r="B105">
         <v>1130</v>
       </c>
-      <c r="C105" t="s">
-        <v>132</v>
+      <c r="C105" s="11" t="s">
+        <v>662</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A106" s="28"/>
+      <c r="A106" s="26" t="s">
+        <v>577</v>
+      </c>
       <c r="B106">
         <v>1140</v>
       </c>
-      <c r="C106" t="s">
-        <v>57</v>
+      <c r="C106" s="11" t="str">
+        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A106,"***")</f>
+        <v>REM SUBROUTINE ***RENDERCARD***</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A107" s="28"/>
+      <c r="A107" s="26"/>
       <c r="B107">
         <v>1150</v>
       </c>
-      <c r="C107" t="s">
-        <v>707</v>
+      <c r="C107" s="11" t="s">
+        <v>723</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A108" s="28"/>
+      <c r="A108" s="26"/>
       <c r="B108">
         <v>1160</v>
       </c>
-      <c r="C108" t="s">
-        <v>708</v>
+      <c r="C108" s="11" t="s">
+        <v>709</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A109" s="28"/>
+      <c r="A109" s="26"/>
       <c r="B109">
         <v>1170</v>
       </c>
-      <c r="C109" t="s">
-        <v>724</v>
+      <c r="C109" s="11" t="s">
+        <v>712</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A110" s="28"/>
+      <c r="A110" s="26"/>
       <c r="B110">
         <v>1180</v>
       </c>
       <c r="C110" t="s">
-        <v>714</v>
+        <v>130</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A111" s="28"/>
+      <c r="A111" s="26"/>
       <c r="B111">
         <v>1190</v>
       </c>
       <c r="C111" t="s">
-        <v>740</v>
+        <v>132</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A112" s="28"/>
+      <c r="A112" s="26"/>
       <c r="B112">
         <v>1200</v>
       </c>
       <c r="C112" t="s">
-        <v>741</v>
+        <v>57</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A113" s="28"/>
+      <c r="A113" s="26"/>
       <c r="B113">
         <v>1210</v>
       </c>
       <c r="C113" t="s">
-        <v>742</v>
+        <v>707</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A114" s="28"/>
+      <c r="A114" s="26"/>
       <c r="B114">
         <v>1220</v>
       </c>
       <c r="C114" t="s">
-        <v>743</v>
+        <v>708</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A115" s="28"/>
+      <c r="A115" s="26"/>
       <c r="B115">
         <v>1230</v>
       </c>
       <c r="C115" t="s">
-        <v>713</v>
+        <v>724</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A116" s="28"/>
+      <c r="A116" s="26"/>
       <c r="B116">
         <v>1240</v>
       </c>
       <c r="C116" t="s">
-        <v>744</v>
+        <v>714</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A117" s="28"/>
+      <c r="A117" s="26"/>
       <c r="B117">
         <v>1250</v>
       </c>
       <c r="C117" t="s">
-        <v>745</v>
+        <v>740</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A118" s="28"/>
+      <c r="A118" s="26"/>
       <c r="B118">
         <v>1260</v>
       </c>
       <c r="C118" t="s">
-        <v>746</v>
+        <v>741</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A119" s="28"/>
+      <c r="A119" s="26"/>
       <c r="B119">
         <v>1270</v>
       </c>
       <c r="C119" t="s">
-        <v>719</v>
+        <v>742</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A120" s="28"/>
+      <c r="A120" s="26"/>
       <c r="B120">
         <v>1280</v>
       </c>
       <c r="C120" t="s">
-        <v>717</v>
+        <v>743</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A121" s="28"/>
+      <c r="A121" s="26"/>
       <c r="B121">
         <v>1290</v>
       </c>
       <c r="C121" t="s">
-        <v>718</v>
+        <v>713</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A122" s="28"/>
+      <c r="A122" s="26"/>
       <c r="B122">
         <v>1300</v>
       </c>
       <c r="C122" t="s">
-        <v>716</v>
+        <v>744</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A123" s="28"/>
+      <c r="A123" s="26"/>
       <c r="B123">
         <v>1310</v>
       </c>
-      <c r="C123" t="str">
-        <f>_xlfn.CONCAT("ON CARDVAL-1 GOSUB ",B125,",",B129,",",B132,",",B138,",",B142,",",B146,",",B150,",",B160,",",B167,",",B171,",",B176,",",B182,",",B188," :: REM CALL RENDERX")</f>
-        <v>ON CARDVAL-1 GOSUB 1330,1370,1400,1460,1500,1540,1580,1680,1750,1790,1840,1900,1960 :: REM CALL RENDERX</v>
+      <c r="C123" t="s">
+        <v>745</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A124" s="28"/>
+      <c r="A124" s="26"/>
       <c r="B124">
         <v>1320</v>
       </c>
-      <c r="C124" s="11" t="s">
-        <v>662</v>
+      <c r="C124" t="s">
+        <v>746</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A125" s="28" t="s">
-        <v>715</v>
-      </c>
+      <c r="A125" s="26"/>
       <c r="B125">
         <v>1330</v>
       </c>
-      <c r="C125" s="11" t="str">
-        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A125,"***")</f>
-        <v>REM SUBROUTINE ***RENDER2***</v>
+      <c r="C125" t="s">
+        <v>719</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A126" s="28"/>
+      <c r="A126" s="26"/>
       <c r="B126">
         <v>1340</v>
       </c>
       <c r="C126" t="s">
-        <v>163</v>
+        <v>717</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A127" s="28"/>
+      <c r="A127" s="26"/>
       <c r="B127">
         <v>1350</v>
       </c>
       <c r="C127" t="s">
-        <v>165</v>
+        <v>718</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A128" s="28"/>
+      <c r="A128" s="26"/>
       <c r="B128">
         <v>1360</v>
       </c>
       <c r="C128" t="s">
-        <v>662</v>
-      </c>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A129" s="28" t="s">
-        <v>578</v>
-      </c>
+        <v>716</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A129" s="26"/>
       <c r="B129">
         <v>1370</v>
       </c>
-      <c r="C129" s="11" t="str">
-        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A129,"***")</f>
-        <v>REM SUBROUTINE ***RENDER3***</v>
-      </c>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A130" s="28"/>
+      <c r="C129" t="str">
+        <f>_xlfn.CONCAT("ON CARDVAL-1 GOSUB ",B131,",",B135,",",B138,",",B144,",",B148,",",B152,",",B156,",",B166,",",B173,",",B177,",",B182,",",B188,",",B194," :: REM CALL RENDERX")</f>
+        <v>ON CARDVAL-1 GOSUB 1390,1430,1460,1520,1560,1600,1640,1740,1810,1850,1900,1960,2020 :: REM CALL RENDERX</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A130" s="26"/>
       <c r="B130">
         <v>1380</v>
       </c>
-      <c r="C130" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A131" s="28"/>
+      <c r="C130" s="11" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A131" s="26" t="s">
+        <v>715</v>
+      </c>
       <c r="B131">
         <v>1390</v>
       </c>
-      <c r="C131" t="s">
-        <v>662</v>
-      </c>
-    </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A132" s="28" t="s">
-        <v>579</v>
-      </c>
+      <c r="C131" s="11" t="str">
+        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A131,"***")</f>
+        <v>REM SUBROUTINE ***RENDER2***</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A132" s="26"/>
       <c r="B132">
         <v>1400</v>
       </c>
-      <c r="C132" s="11" t="str">
-        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A132,"***")</f>
-        <v>REM SUBROUTINE ***RENDER4***</v>
-      </c>
-    </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A133" s="28"/>
+      <c r="C132" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A133" s="26"/>
       <c r="B133">
         <v>1410</v>
       </c>
       <c r="C133" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A134" s="28"/>
+        <v>165</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A134" s="26"/>
       <c r="B134">
         <v>1420</v>
       </c>
       <c r="C134" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A135" s="28"/>
+        <v>662</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A135" s="26" t="s">
+        <v>578</v>
+      </c>
       <c r="B135">
         <v>1430</v>
       </c>
-      <c r="C135" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A136" s="28"/>
+      <c r="C135" s="11" t="str">
+        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A135,"***")</f>
+        <v>REM SUBROUTINE ***RENDER3***</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A136" s="26"/>
       <c r="B136">
         <v>1440</v>
       </c>
       <c r="C136" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A137" s="28"/>
+        <v>173</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A137" s="26"/>
       <c r="B137">
         <v>1450</v>
       </c>
@@ -4408,402 +4421,402 @@
         <v>662</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A138" s="28" t="s">
-        <v>580</v>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A138" s="26" t="s">
+        <v>579</v>
       </c>
       <c r="B138">
         <v>1460</v>
       </c>
       <c r="C138" s="11" t="str">
         <f>_xlfn.CONCAT("REM SUBROUTINE ***",A138,"***")</f>
-        <v>REM SUBROUTINE ***RENDER5***</v>
-      </c>
-    </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A139" s="28"/>
+        <v>REM SUBROUTINE ***RENDER4***</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A139" s="26"/>
       <c r="B139">
         <v>1470</v>
       </c>
-      <c r="C139" t="str">
-        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D139,A:A,0),0)," :: REM CALL ",D139,"")</f>
-        <v>GOSUB 1400 :: REM CALL RENDER4</v>
-      </c>
-      <c r="D139" t="str">
-        <f>A132</f>
-        <v>RENDER4</v>
-      </c>
-    </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A140" s="28"/>
+      <c r="C139" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A140" s="26"/>
       <c r="B140">
         <v>1480</v>
       </c>
       <c r="C140" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A141" s="28"/>
+        <v>182</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A141" s="26"/>
       <c r="B141">
         <v>1490</v>
       </c>
       <c r="C141" t="s">
-        <v>662</v>
-      </c>
-    </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A142" s="28" t="s">
-        <v>581</v>
-      </c>
+        <v>184</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A142" s="26"/>
       <c r="B142">
         <v>1500</v>
       </c>
-      <c r="C142" s="11" t="str">
-        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A142,"***")</f>
-        <v>REM SUBROUTINE ***RENDER6***</v>
-      </c>
-    </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A143" s="28"/>
+      <c r="C142" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A143" s="26"/>
       <c r="B143">
         <v>1510</v>
       </c>
       <c r="C143" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A144" s="28"/>
+        <v>662</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A144" s="26" t="s">
+        <v>580</v>
+      </c>
       <c r="B144">
         <v>1520</v>
       </c>
-      <c r="C144" t="s">
-        <v>201</v>
+      <c r="C144" s="11" t="str">
+        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A144,"***")</f>
+        <v>REM SUBROUTINE ***RENDER5***</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A145" s="28"/>
+      <c r="A145" s="26"/>
       <c r="B145">
         <v>1530</v>
       </c>
-      <c r="C145" t="s">
-        <v>662</v>
+      <c r="C145" t="str">
+        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D145,A:A,0),0)," :: REM CALL ",D145,"")</f>
+        <v>GOSUB 1460 :: REM CALL RENDER4</v>
+      </c>
+      <c r="D145" t="str">
+        <f>A138</f>
+        <v>RENDER4</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A146" s="28" t="s">
-        <v>582</v>
-      </c>
+      <c r="A146" s="26"/>
       <c r="B146">
         <v>1540</v>
       </c>
-      <c r="C146" s="11" t="str">
-        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A146,"***")</f>
-        <v>REM SUBROUTINE ***RENDER7***</v>
+      <c r="C146" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A147" s="28"/>
+      <c r="A147" s="26"/>
       <c r="B147">
         <v>1550</v>
       </c>
-      <c r="C147" t="str">
-        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D147,A:A,0),0)," :: REM CALL ",D147,"")</f>
-        <v>GOSUB 1500 :: REM CALL RENDER6</v>
-      </c>
-      <c r="D147" t="str">
-        <f>A142</f>
-        <v>RENDER6</v>
+      <c r="C147" t="s">
+        <v>662</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A148" s="28"/>
+      <c r="A148" s="26" t="s">
+        <v>581</v>
+      </c>
       <c r="B148">
         <v>1560</v>
       </c>
-      <c r="C148" t="s">
-        <v>207</v>
+      <c r="C148" s="11" t="str">
+        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A148,"***")</f>
+        <v>REM SUBROUTINE ***RENDER6***</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A149" s="28"/>
+      <c r="A149" s="26"/>
       <c r="B149">
         <v>1570</v>
       </c>
       <c r="C149" t="s">
-        <v>662</v>
+        <v>199</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A150" s="28" t="s">
-        <v>583</v>
-      </c>
+      <c r="A150" s="26"/>
       <c r="B150">
         <v>1580</v>
       </c>
-      <c r="C150" s="11" t="str">
-        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A150,"***")</f>
-        <v>REM SUBROUTINE ***RENDER8***</v>
+      <c r="C150" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A151" s="28"/>
+      <c r="A151" s="26"/>
       <c r="B151">
         <v>1590</v>
       </c>
       <c r="C151" t="s">
-        <v>214</v>
+        <v>662</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A152" s="28"/>
+      <c r="A152" s="26" t="s">
+        <v>582</v>
+      </c>
       <c r="B152">
         <v>1600</v>
       </c>
-      <c r="C152" t="s">
-        <v>216</v>
+      <c r="C152" s="11" t="str">
+        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A152,"***")</f>
+        <v>REM SUBROUTINE ***RENDER7***</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A153" s="28"/>
+      <c r="A153" s="26"/>
       <c r="B153">
         <v>1610</v>
       </c>
-      <c r="C153" t="s">
-        <v>163</v>
+      <c r="C153" t="str">
+        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D153,A:A,0),0)," :: REM CALL ",D153,"")</f>
+        <v>GOSUB 1560 :: REM CALL RENDER6</v>
+      </c>
+      <c r="D153" t="str">
+        <f>A148</f>
+        <v>RENDER6</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A154" s="28"/>
+      <c r="A154" s="26"/>
       <c r="B154">
         <v>1620</v>
       </c>
       <c r="C154" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A155" s="28"/>
+      <c r="A155" s="26"/>
       <c r="B155">
         <v>1630</v>
       </c>
       <c r="C155" t="s">
-        <v>221</v>
+        <v>662</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A156" s="28"/>
+      <c r="A156" s="26" t="s">
+        <v>583</v>
+      </c>
       <c r="B156">
         <v>1640</v>
       </c>
-      <c r="C156" t="s">
-        <v>165</v>
+      <c r="C156" s="11" t="str">
+        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A156,"***")</f>
+        <v>REM SUBROUTINE ***RENDER8***</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A157" s="28"/>
+      <c r="A157" s="26"/>
       <c r="B157">
         <v>1650</v>
       </c>
       <c r="C157" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A158" s="28"/>
+      <c r="A158" s="26"/>
       <c r="B158">
         <v>1660</v>
       </c>
       <c r="C158" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A159" s="28"/>
+      <c r="A159" s="26"/>
       <c r="B159">
         <v>1670</v>
       </c>
       <c r="C159" t="s">
-        <v>662</v>
+        <v>163</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A160" s="28" t="s">
-        <v>584</v>
-      </c>
+      <c r="A160" s="26"/>
       <c r="B160">
         <v>1680</v>
       </c>
-      <c r="C160" s="11" t="str">
-        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A160,"***")</f>
-        <v>REM SUBROUTINE ***RENDER9***</v>
+      <c r="C160" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A161" s="28"/>
+      <c r="A161" s="26"/>
       <c r="B161">
         <v>1690</v>
       </c>
       <c r="C161" t="s">
-        <v>233</v>
+        <v>221</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A162" s="28"/>
+      <c r="A162" s="26"/>
       <c r="B162">
         <v>1700</v>
       </c>
       <c r="C162" t="s">
-        <v>235</v>
+        <v>165</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A163" s="28"/>
+      <c r="A163" s="26"/>
       <c r="B163">
         <v>1710</v>
       </c>
       <c r="C163" t="s">
-        <v>237</v>
+        <v>224</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A164" s="28"/>
+      <c r="A164" s="26"/>
       <c r="B164">
         <v>1720</v>
       </c>
       <c r="C164" t="s">
-        <v>239</v>
+        <v>226</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A165" s="28"/>
+      <c r="A165" s="26"/>
       <c r="B165">
         <v>1730</v>
       </c>
       <c r="C165" t="s">
-        <v>192</v>
+        <v>662</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A166" s="28"/>
+      <c r="A166" s="26" t="s">
+        <v>584</v>
+      </c>
       <c r="B166">
         <v>1740</v>
       </c>
-      <c r="C166" t="s">
-        <v>662</v>
+      <c r="C166" s="11" t="str">
+        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A166,"***")</f>
+        <v>REM SUBROUTINE ***RENDER9***</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A167" s="28" t="s">
-        <v>585</v>
-      </c>
+      <c r="A167" s="26"/>
       <c r="B167">
         <v>1750</v>
       </c>
-      <c r="C167" s="11" t="str">
-        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A167,"***")</f>
-        <v>REM SUBROUTINE ***RENDER10***</v>
+      <c r="C167" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A168" s="28"/>
+      <c r="A168" s="26"/>
       <c r="B168">
         <v>1760</v>
       </c>
       <c r="C168" t="s">
-        <v>247</v>
+        <v>235</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A169" s="28"/>
+      <c r="A169" s="26"/>
       <c r="B169">
         <v>1770</v>
       </c>
       <c r="C169" t="s">
-        <v>249</v>
+        <v>237</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A170" s="28"/>
+      <c r="A170" s="26"/>
       <c r="B170">
         <v>1780</v>
       </c>
       <c r="C170" t="s">
-        <v>662</v>
+        <v>239</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A171" s="28" t="s">
-        <v>586</v>
-      </c>
+      <c r="A171" s="26"/>
       <c r="B171">
         <v>1790</v>
       </c>
-      <c r="C171" s="11" t="str">
-        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A171,"***")</f>
-        <v>REM SUBROUTINE ***RENDERJACK***</v>
+      <c r="C171" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A172" s="28"/>
+      <c r="A172" s="26"/>
       <c r="B172">
         <v>1800</v>
       </c>
       <c r="C172" t="s">
-        <v>249</v>
+        <v>662</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A173" s="28"/>
+      <c r="A173" s="26" t="s">
+        <v>585</v>
+      </c>
       <c r="B173">
         <v>1810</v>
       </c>
-      <c r="C173" t="s">
-        <v>257</v>
+      <c r="C173" s="11" t="str">
+        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A173,"***")</f>
+        <v>REM SUBROUTINE ***RENDER10***</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A174" s="28"/>
+      <c r="A174" s="26"/>
       <c r="B174">
         <v>1820</v>
       </c>
       <c r="C174" t="s">
-        <v>182</v>
+        <v>247</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A175" s="28"/>
+      <c r="A175" s="26"/>
       <c r="B175">
         <v>1830</v>
       </c>
       <c r="C175" t="s">
-        <v>662</v>
+        <v>249</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A176" s="28" t="s">
-        <v>587</v>
-      </c>
+      <c r="A176" s="26"/>
       <c r="B176">
         <v>1840</v>
       </c>
-      <c r="C176" s="11" t="str">
-        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A176,"***")</f>
-        <v>REM SUBROUTINE ***RENDERQUEEN***</v>
+      <c r="C176" t="s">
+        <v>662</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A177" s="28"/>
+      <c r="A177" s="26" t="s">
+        <v>586</v>
+      </c>
       <c r="B177">
         <v>1850</v>
       </c>
-      <c r="C177" t="s">
-        <v>247</v>
+      <c r="C177" s="11" t="str">
+        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A177,"***")</f>
+        <v>REM SUBROUTINE ***RENDERJACK***</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A178" s="28"/>
+      <c r="A178" s="26"/>
       <c r="B178">
         <v>1860</v>
       </c>
@@ -4812,25 +4825,25 @@
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A179" s="28"/>
+      <c r="A179" s="26"/>
       <c r="B179">
         <v>1870</v>
       </c>
       <c r="C179" t="s">
-        <v>267</v>
+        <v>257</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A180" s="28"/>
+      <c r="A180" s="26"/>
       <c r="B180">
         <v>1880</v>
       </c>
       <c r="C180" t="s">
-        <v>269</v>
+        <v>182</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A181" s="28"/>
+      <c r="A181" s="26"/>
       <c r="B181">
         <v>1890</v>
       </c>
@@ -4839,19 +4852,19 @@
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A182" s="28" t="s">
-        <v>588</v>
+      <c r="A182" s="26" t="s">
+        <v>587</v>
       </c>
       <c r="B182">
         <v>1900</v>
       </c>
       <c r="C182" s="11" t="str">
         <f>_xlfn.CONCAT("REM SUBROUTINE ***",A182,"***")</f>
-        <v>REM SUBROUTINE ***RENDERKING***</v>
+        <v>REM SUBROUTINE ***RENDERQUEEN***</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A183" s="28"/>
+      <c r="A183" s="26"/>
       <c r="B183">
         <v>1910</v>
       </c>
@@ -4860,34 +4873,34 @@
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A184" s="28"/>
+      <c r="A184" s="26"/>
       <c r="B184">
         <v>1920</v>
       </c>
       <c r="C184" t="s">
-        <v>235</v>
+        <v>249</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A185" s="28"/>
+      <c r="A185" s="26"/>
       <c r="B185">
         <v>1930</v>
       </c>
       <c r="C185" t="s">
-        <v>239</v>
+        <v>267</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A186" s="28"/>
+      <c r="A186" s="26"/>
       <c r="B186">
         <v>1940</v>
       </c>
       <c r="C186" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A187" s="28"/>
+      <c r="A187" s="26"/>
       <c r="B187">
         <v>1950</v>
       </c>
@@ -4896,1009 +4909,1066 @@
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A188" s="28" t="s">
-        <v>589</v>
+      <c r="A188" s="26" t="s">
+        <v>588</v>
       </c>
       <c r="B188">
         <v>1960</v>
       </c>
-      <c r="C188" t="s">
-        <v>192</v>
+      <c r="C188" s="11" t="str">
+        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A188,"***")</f>
+        <v>REM SUBROUTINE ***RENDERKING***</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A189" s="28"/>
+      <c r="A189" s="26"/>
       <c r="B189">
         <v>1970</v>
       </c>
       <c r="C189" t="s">
-        <v>662</v>
+        <v>247</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A190" s="28" t="s">
-        <v>751</v>
-      </c>
+      <c r="A190" s="26"/>
       <c r="B190">
         <v>1980</v>
       </c>
-      <c r="C190" s="11" t="str">
-        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A190,"***")</f>
-        <v>REM SUBROUTINE ***DRAWHANDS***</v>
+      <c r="C190" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A191" s="28"/>
+      <c r="A191" s="26"/>
       <c r="B191">
         <v>1990</v>
       </c>
-      <c r="C191" s="11" t="s">
-        <v>747</v>
+      <c r="C191" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A192" s="28"/>
+      <c r="A192" s="26"/>
       <c r="B192">
         <v>2000</v>
       </c>
-      <c r="C192" s="11" t="s">
-        <v>748</v>
+      <c r="C192" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A193" s="28"/>
+      <c r="A193" s="26"/>
       <c r="B193">
         <v>2010</v>
       </c>
-      <c r="C193" s="11" t="s">
-        <v>772</v>
+      <c r="C193" t="s">
+        <v>662</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A194" s="28"/>
+      <c r="A194" s="26" t="s">
+        <v>589</v>
+      </c>
       <c r="B194">
         <v>2020</v>
       </c>
-      <c r="C194" s="11" t="s">
-        <v>749</v>
+      <c r="C194" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A195" s="28"/>
+      <c r="A195" s="26"/>
       <c r="B195">
         <v>2030</v>
       </c>
-      <c r="C195" s="11" t="s">
-        <v>783</v>
+      <c r="C195" t="s">
+        <v>662</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A196" s="28"/>
+      <c r="A196" s="26" t="s">
+        <v>751</v>
+      </c>
       <c r="B196">
         <v>2040</v>
       </c>
-      <c r="C196" s="26" t="s">
-        <v>96</v>
+      <c r="C196" s="11" t="str">
+        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A196,"***")</f>
+        <v>REM SUBROUTINE ***DRAWHANDS***</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A197" s="28"/>
+      <c r="A197" s="26"/>
       <c r="B197">
         <v>2050</v>
       </c>
       <c r="C197" s="11" t="s">
-        <v>787</v>
+        <v>747</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A198" s="28"/>
+      <c r="A198" s="26"/>
       <c r="B198">
         <v>2060</v>
       </c>
       <c r="C198" s="11" t="s">
-        <v>782</v>
+        <v>748</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A199" s="28"/>
+      <c r="A199" s="26"/>
       <c r="B199">
         <v>2070</v>
       </c>
       <c r="C199" s="11" t="s">
-        <v>784</v>
+        <v>772</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A200" s="28"/>
+      <c r="A200" s="26"/>
       <c r="B200">
         <v>2080</v>
       </c>
       <c r="C200" s="11" t="s">
-        <v>785</v>
+        <v>749</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A201" s="28"/>
+      <c r="A201" s="26"/>
       <c r="B201">
         <v>2090</v>
       </c>
       <c r="C201" s="11" t="s">
-        <v>786</v>
+        <v>781</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A202" s="28"/>
+      <c r="A202" s="26"/>
       <c r="B202">
         <v>2100</v>
       </c>
-      <c r="C202" s="26" t="s">
-        <v>57</v>
+      <c r="C202" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A203" s="28"/>
+      <c r="A203" s="26"/>
       <c r="B203">
         <v>2110</v>
       </c>
       <c r="C203" s="11" t="s">
-        <v>662</v>
+        <v>785</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A204" s="28" t="s">
-        <v>720</v>
-      </c>
+      <c r="A204" s="26"/>
       <c r="B204">
         <v>2120</v>
       </c>
-      <c r="C204" s="11" t="str">
-        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A204,"***")</f>
-        <v>REM SUBROUTINE ***CLEARTABLE***</v>
+      <c r="C204" s="11" t="s">
+        <v>780</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A205" s="28"/>
+      <c r="A205" s="26"/>
       <c r="B205">
         <v>2130</v>
       </c>
-      <c r="C205" t="s">
-        <v>7</v>
+      <c r="C205" s="11" t="s">
+        <v>782</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A206" s="28"/>
+      <c r="A206" s="26"/>
       <c r="B206">
         <v>2140</v>
       </c>
-      <c r="C206" t="s">
-        <v>788</v>
+      <c r="C206" s="11" t="s">
+        <v>783</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A207" s="28"/>
+      <c r="A207" s="26"/>
       <c r="B207">
         <v>2150</v>
       </c>
-      <c r="C207" t="s">
-        <v>755</v>
+      <c r="C207" s="11" t="s">
+        <v>784</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A208" s="28"/>
+      <c r="A208" s="26"/>
       <c r="B208">
         <v>2160</v>
       </c>
       <c r="C208" t="s">
-        <v>662</v>
+        <v>57</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A209" s="28" t="s">
-        <v>721</v>
-      </c>
+      <c r="A209" s="26"/>
       <c r="B209">
         <v>2170</v>
       </c>
-      <c r="C209" s="11" t="str">
-        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A209,"***")</f>
-        <v>REM SUBROUTINE ***DEAL***</v>
+      <c r="C209" s="11" t="s">
+        <v>662</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A210" s="28"/>
+      <c r="A210" s="26" t="s">
+        <v>720</v>
+      </c>
       <c r="B210">
         <v>2180</v>
       </c>
-      <c r="C210" s="11" t="s">
-        <v>756</v>
+      <c r="C210" s="11" t="str">
+        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A210,"***")</f>
+        <v>REM SUBROUTINE ***CLEARTABLE***</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A211" s="28"/>
+      <c r="A211" s="26"/>
       <c r="B211">
         <v>2190</v>
       </c>
-      <c r="C211" s="11" t="s">
-        <v>757</v>
+      <c r="C211" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A212" s="28"/>
+      <c r="A212" s="26"/>
       <c r="B212">
         <v>2200</v>
       </c>
-      <c r="C212" s="11" t="s">
-        <v>750</v>
+      <c r="C212" t="s">
+        <v>786</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A213" s="28"/>
+      <c r="A213" s="26"/>
       <c r="B213">
         <v>2210</v>
       </c>
-      <c r="C213" s="11" t="str">
-        <f>_xlfn.CONCAT("IF CVAL&lt;10 THEN ",B215)</f>
-        <v>IF CVAL&lt;10 THEN 2230</v>
+      <c r="C213" t="s">
+        <v>755</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A214" s="28"/>
+      <c r="A214" s="26"/>
       <c r="B214">
         <v>2220</v>
       </c>
-      <c r="C214" s="11" t="s">
-        <v>734</v>
+      <c r="C214" t="s">
+        <v>662</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A215" s="28"/>
+      <c r="A215" s="26" t="s">
+        <v>721</v>
+      </c>
       <c r="B215">
         <v>2230</v>
       </c>
-      <c r="C215" s="11" t="s">
-        <v>758</v>
+      <c r="C215" s="11" t="str">
+        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A215,"***")</f>
+        <v>REM SUBROUTINE ***DEAL***</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A216" s="28"/>
+      <c r="A216" s="26"/>
       <c r="B216">
         <v>2240</v>
       </c>
-      <c r="C216" t="str">
-        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D216,A:A,0),0)," :: REM CALL ",D216,"")</f>
-        <v>GOSUB 1080 :: REM CALL RENDERCARD</v>
-      </c>
-      <c r="D216" t="str">
-        <f>A100</f>
-        <v>RENDERCARD</v>
+      <c r="C216" s="11" t="s">
+        <v>756</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A217" s="28"/>
+      <c r="A217" s="26"/>
       <c r="B217">
         <v>2250</v>
       </c>
       <c r="C217" s="11" t="s">
-        <v>662</v>
+        <v>757</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A218" s="28" t="s">
-        <v>722</v>
-      </c>
+      <c r="A218" s="26"/>
       <c r="B218">
         <v>2260</v>
       </c>
-      <c r="C218" s="11" t="str">
-        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A218,"***")</f>
-        <v>REM SUBROUTINE ***PLAY***</v>
+      <c r="C218" s="11" t="s">
+        <v>750</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A219" s="28"/>
+      <c r="A219" s="26"/>
       <c r="B219">
         <v>2270</v>
       </c>
-      <c r="C219" t="str">
-        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D219,A:A,0),0)," :: REM CALL ",D219,"")</f>
-        <v>GOSUB 2120 :: REM CALL CLEARTABLE</v>
-      </c>
-      <c r="D219" t="str">
-        <f>A204</f>
-        <v>CLEARTABLE</v>
+      <c r="C219" s="11" t="str">
+        <f>_xlfn.CONCAT("IF CVAL&lt;10 THEN ",B221)</f>
+        <v>IF CVAL&lt;10 THEN 2290</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A220" s="28"/>
+      <c r="A220" s="26"/>
       <c r="B220">
         <v>2280</v>
       </c>
-      <c r="C220" t="str">
-        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D220,A:A,0),0)," :: REM CALL ",D220,"")</f>
-        <v>GOSUB 1980 :: REM CALL DRAWHANDS</v>
-      </c>
-      <c r="D220" t="str">
-        <f>A190</f>
-        <v>DRAWHANDS</v>
+      <c r="C220" s="11" t="s">
+        <v>734</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A221" s="28"/>
+      <c r="A221" s="26"/>
       <c r="B221">
         <v>2290</v>
       </c>
-      <c r="C221" t="s">
-        <v>725</v>
+      <c r="C221" s="11" t="s">
+        <v>758</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A222" s="28"/>
+      <c r="A222" s="26"/>
       <c r="B222">
         <v>2300</v>
       </c>
       <c r="C222" t="str">
         <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D222,A:A,0),0)," :: REM CALL ",D222,"")</f>
-        <v>GOSUB 2170 :: REM CALL DEAL</v>
+        <v>GOSUB 1140 :: REM CALL RENDERCARD</v>
       </c>
       <c r="D222" t="str">
-        <f>A209</f>
-        <v>DEAL</v>
+        <f>A106</f>
+        <v>RENDERCARD</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A223" s="28"/>
+      <c r="A223" s="26"/>
       <c r="B223">
         <v>2310</v>
       </c>
-      <c r="C223" t="str">
-        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D223,A:A,0),0)," :: REM CALL ",D223,"")</f>
-        <v>GOSUB 2170 :: REM CALL DEAL</v>
-      </c>
-      <c r="D223" t="str">
-        <f>A209</f>
-        <v>DEAL</v>
+      <c r="C223" s="11" t="s">
+        <v>662</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A224" s="28"/>
+      <c r="A224" s="26" t="s">
+        <v>722</v>
+      </c>
       <c r="B224">
         <v>2320</v>
       </c>
-      <c r="C224" t="s">
-        <v>726</v>
+      <c r="C224" s="11" t="str">
+        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A224,"***")</f>
+        <v>REM SUBROUTINE ***PLAY***</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A225" s="28"/>
+      <c r="A225" s="26"/>
       <c r="B225">
         <v>2330</v>
       </c>
       <c r="C225" t="str">
         <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D225,A:A,0),0)," :: REM CALL ",D225,"")</f>
-        <v>GOSUB 2170 :: REM CALL DEAL</v>
+        <v>GOSUB 2180 :: REM CALL CLEARTABLE</v>
       </c>
       <c r="D225" t="str">
-        <f>A209</f>
-        <v>DEAL</v>
+        <f>A210</f>
+        <v>CLEARTABLE</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A226" s="28"/>
+      <c r="A226" s="26"/>
       <c r="B226">
         <v>2340</v>
       </c>
-      <c r="C226" t="s">
-        <v>727</v>
+      <c r="C226" t="str">
+        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D226,A:A,0),0)," :: REM CALL ",D226,"")</f>
+        <v>GOSUB 2040 :: REM CALL DRAWHANDS</v>
+      </c>
+      <c r="D226" t="str">
+        <f>A196</f>
+        <v>DRAWHANDS</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A227" s="28"/>
+      <c r="A227" s="26"/>
       <c r="B227">
         <v>2350</v>
       </c>
-      <c r="C227" t="str">
-        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D227,A:A,0),0)," :: REM CALL ",D227,"")</f>
-        <v>GOSUB 2170 :: REM CALL DEAL</v>
-      </c>
-      <c r="D227" t="str">
-        <f>A209</f>
-        <v>DEAL</v>
+      <c r="C227" t="s">
+        <v>725</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A228" s="28" t="s">
-        <v>770</v>
-      </c>
+      <c r="A228" s="26"/>
       <c r="B228">
         <v>2360</v>
       </c>
       <c r="C228" t="str">
-        <f>_xlfn.CONCAT("REM ***",A228,"***")</f>
-        <v>REM ***PLAYER***</v>
+        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D228,A:A,0),0)," :: REM CALL ",D228,"")</f>
+        <v>GOSUB 2230 :: REM CALL DEAL</v>
+      </c>
+      <c r="D228" t="str">
+        <f>A215</f>
+        <v>DEAL</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A229" s="28"/>
+      <c r="A229" s="26"/>
       <c r="B229">
         <v>2370</v>
       </c>
-      <c r="C229" t="s">
-        <v>739</v>
+      <c r="C229" t="str">
+        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D229,A:A,0),0)," :: REM CALL ",D229,"")</f>
+        <v>GOSUB 2230 :: REM CALL DEAL</v>
+      </c>
+      <c r="D229" t="str">
+        <f>A215</f>
+        <v>DEAL</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A230" s="28"/>
+      <c r="A230" s="26"/>
       <c r="B230">
         <v>2380</v>
       </c>
       <c r="C230" t="s">
-        <v>729</v>
+        <v>726</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A231" s="28"/>
+      <c r="A231" s="26"/>
       <c r="B231">
         <v>2390</v>
       </c>
-      <c r="C231" s="1" t="s">
-        <v>769</v>
+      <c r="C231" t="str">
+        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D231,A:A,0),0)," :: REM CALL ",D231,"")</f>
+        <v>GOSUB 2230 :: REM CALL DEAL</v>
+      </c>
+      <c r="D231" t="str">
+        <f>A215</f>
+        <v>DEAL</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A232" s="28"/>
+      <c r="A232" s="26"/>
       <c r="B232">
         <v>2400</v>
       </c>
-      <c r="C232" s="1" t="s">
-        <v>334</v>
+      <c r="C232" t="s">
+        <v>727</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A233" s="28"/>
+      <c r="A233" s="26"/>
       <c r="B233">
         <v>2410</v>
       </c>
-      <c r="C233" s="1" t="s">
-        <v>780</v>
+      <c r="C233" t="str">
+        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D233,A:A,0),0)," :: REM CALL ",D233,"")</f>
+        <v>GOSUB 2230 :: REM CALL DEAL</v>
+      </c>
+      <c r="D233" t="str">
+        <f>A215</f>
+        <v>DEAL</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A234" s="28"/>
+      <c r="A234" s="26" t="s">
+        <v>770</v>
+      </c>
       <c r="B234">
         <v>2420</v>
       </c>
-      <c r="C234" s="1" t="str">
-        <f>_xlfn.CONCAT("IF A$=""N"" THEN ",INDEX(B:B,MATCH(D234,A:A,0),0)," :: REM GOTO ",D234,"")</f>
-        <v>IF A$="N" THEN 2490 :: REM GOTO REVEAL</v>
-      </c>
-      <c r="D234" t="str">
-        <f>A241</f>
-        <v>REVEAL</v>
+      <c r="C234" t="str">
+        <f>_xlfn.CONCAT("REM ***",A234,"***")</f>
+        <v>REM ***PLAYER***</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A235" s="28"/>
+      <c r="A235" s="26"/>
       <c r="B235">
         <v>2430</v>
       </c>
-      <c r="C235" s="1" t="s">
-        <v>725</v>
+      <c r="C235" t="s">
+        <v>739</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A236" s="28"/>
+      <c r="A236" s="26"/>
       <c r="B236">
         <v>2440</v>
       </c>
-      <c r="C236" t="str">
-        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D236,A:A,0),0)," :: REM CALL ",D236,"")</f>
-        <v>GOSUB 2170 :: REM CALL DEAL</v>
-      </c>
-      <c r="D236" t="str">
-        <f>A209</f>
-        <v>DEAL</v>
+      <c r="C236" t="s">
+        <v>729</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A237" s="28"/>
+      <c r="A237" s="26"/>
       <c r="B237">
         <v>2450</v>
       </c>
       <c r="C237" s="1" t="s">
-        <v>762</v>
+        <v>769</v>
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A238" s="28"/>
+      <c r="A238" s="26"/>
       <c r="B238">
         <v>2460</v>
       </c>
-      <c r="C238" s="26" t="s">
-        <v>779</v>
+      <c r="C238" s="1" t="s">
+        <v>334</v>
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A239" s="28"/>
+      <c r="A239" s="26"/>
       <c r="B239">
         <v>2470</v>
       </c>
-      <c r="C239" s="1" t="str">
-        <f>_xlfn.CONCAT("IF BUSTED=1 THEN ",INDEX(B:B,MATCH(D239,A:A,0),0)," :: REM GOTO ",D239,"")</f>
-        <v>IF BUSTED=1 THEN 2490 :: REM GOTO REVEAL</v>
-      </c>
-      <c r="D239" t="str">
-        <f>A241</f>
-        <v>REVEAL</v>
+      <c r="C239" s="1" t="s">
+        <v>778</v>
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A240" s="28"/>
+      <c r="A240" s="26"/>
       <c r="B240">
         <v>2480</v>
       </c>
-      <c r="C240" s="1" t="s">
-        <v>728</v>
+      <c r="C240" s="1" t="str">
+        <f>_xlfn.CONCAT("IF A$=""N"" THEN ",INDEX(B:B,MATCH(D240,A:A,0),0)," :: REM GOTO ",D240,"")</f>
+        <v>IF A$="N" THEN 2550 :: REM GOTO REVEAL</v>
+      </c>
+      <c r="D240" t="str">
+        <f>A247</f>
+        <v>REVEAL</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A241" s="29" t="s">
-        <v>732</v>
-      </c>
+      <c r="A241" s="26"/>
       <c r="B241">
         <v>2490</v>
       </c>
-      <c r="C241" t="str">
-        <f>_xlfn.CONCAT("REM ***",A241,"***")</f>
-        <v>REM ***REVEAL***</v>
+      <c r="C241" s="1" t="s">
+        <v>725</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A242" s="28"/>
+      <c r="A242" s="26"/>
       <c r="B242">
         <v>2500</v>
       </c>
-      <c r="C242" s="1" t="s">
-        <v>764</v>
+      <c r="C242" t="str">
+        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D242,A:A,0),0)," :: REM CALL ",D242,"")</f>
+        <v>GOSUB 2230 :: REM CALL DEAL</v>
+      </c>
+      <c r="D242" t="str">
+        <f>A215</f>
+        <v>DEAL</v>
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A243" s="28"/>
+      <c r="A243" s="26"/>
       <c r="B243">
         <v>2510</v>
       </c>
-      <c r="C243" t="str">
-        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D243,A:A,0),0)," :: REM CALL ",D243,"")</f>
-        <v>GOSUB 1080 :: REM CALL RENDERCARD</v>
-      </c>
-      <c r="D243" t="str">
-        <f>A100</f>
-        <v>RENDERCARD</v>
+      <c r="C243" s="1" t="s">
+        <v>762</v>
       </c>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A244" s="28"/>
+      <c r="A244" s="26"/>
       <c r="B244">
         <v>2520</v>
       </c>
-      <c r="C244" s="1" t="str">
-        <f>_xlfn.CONCAT("IF BUSTED=1 THEN ",INDEX(B:B,MATCH(D244,A:A,0),0)," :: REM GOTO ",D244,"")</f>
-        <v>IF BUSTED=1 THEN 2660 :: REM GOTO GAMEOVER</v>
-      </c>
-      <c r="D244" t="str">
-        <f>A258</f>
-        <v>GAMEOVER</v>
+      <c r="C244" t="s">
+        <v>777</v>
       </c>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A245" s="29" t="s">
-        <v>767</v>
-      </c>
+      <c r="A245" s="26"/>
       <c r="B245">
         <v>2530</v>
       </c>
-      <c r="C245" t="str">
-        <f>_xlfn.CONCAT("REM ***",A245,"***")</f>
-        <v>REM ***DEALER***</v>
+      <c r="C245" s="1" t="str">
+        <f>_xlfn.CONCAT("IF BUSTED=1 THEN ",INDEX(B:B,MATCH(D245,A:A,0),0)," :: REM GOTO ",D245,"")</f>
+        <v>IF BUSTED=1 THEN 2550 :: REM GOTO REVEAL</v>
+      </c>
+      <c r="D245" t="str">
+        <f>A247</f>
+        <v>REVEAL</v>
       </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A246" s="29"/>
+      <c r="A246" s="26"/>
       <c r="B246">
         <v>2540</v>
       </c>
-      <c r="C246" t="s">
-        <v>739</v>
+      <c r="C246" s="1" t="s">
+        <v>728</v>
       </c>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A247" s="29"/>
+      <c r="A247" s="27" t="s">
+        <v>732</v>
+      </c>
       <c r="B247">
         <v>2550</v>
       </c>
-      <c r="C247" t="s">
-        <v>729</v>
+      <c r="C247" t="str">
+        <f>_xlfn.CONCAT("REM ***",A247,"***")</f>
+        <v>REM ***REVEAL***</v>
       </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A248" s="29"/>
+      <c r="A248" s="26"/>
       <c r="B248">
         <v>2560</v>
       </c>
       <c r="C248" s="1" t="s">
-        <v>726</v>
+        <v>764</v>
       </c>
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A249" s="29"/>
+      <c r="A249" s="26"/>
       <c r="B249">
         <v>2570</v>
       </c>
       <c r="C249" t="str">
         <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D249,A:A,0),0)," :: REM CALL ",D249,"")</f>
-        <v>GOSUB 2810 :: REM CALL CALCSCORE</v>
+        <v>GOSUB 1140 :: REM CALL RENDERCARD</v>
       </c>
       <c r="D249" t="str">
-        <f>A273</f>
-        <v>CALCSCORE</v>
+        <f>A106</f>
+        <v>RENDERCARD</v>
       </c>
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A250" s="29"/>
+      <c r="A250" s="26"/>
       <c r="B250">
         <v>2580</v>
       </c>
-      <c r="C250" t="str">
-        <f>_xlfn.CONCAT("IF SCORE&gt;=17 THEN ",,INDEX(B:B,MATCH(D250,A:A,0),0)," :: REM GOTO ",D250,"")</f>
-        <v>IF SCORE&gt;=17 THEN 2640 :: REM GOTO TALLY</v>
+      <c r="C250" s="1" t="str">
+        <f>_xlfn.CONCAT("IF BUSTED=1 THEN ",INDEX(B:B,MATCH(D250,A:A,0),0)," :: REM GOTO ",D250,"")</f>
+        <v>IF BUSTED=1 THEN 2720 :: REM GOTO GAMEOVER</v>
       </c>
       <c r="D250" t="str">
-        <f>A256</f>
-        <v>TALLY</v>
+        <f>A264</f>
+        <v>GAMEOVER</v>
       </c>
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A251" s="29"/>
+      <c r="A251" s="27" t="s">
+        <v>767</v>
+      </c>
       <c r="B251">
         <v>2590</v>
       </c>
       <c r="C251" t="str">
-        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D251,A:A,0),0)," :: REM CALL ",D251,"")</f>
-        <v>GOSUB 2170 :: REM CALL DEAL</v>
-      </c>
-      <c r="D251" t="str">
-        <f>A209</f>
-        <v>DEAL</v>
+        <f>_xlfn.CONCAT("REM ***",A251,"***")</f>
+        <v>REM ***DEALER***</v>
       </c>
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A252" s="29"/>
+      <c r="A252" s="27"/>
       <c r="B252">
         <v>2600</v>
       </c>
-      <c r="C252" s="1" t="s">
-        <v>768</v>
+      <c r="C252" t="s">
+        <v>739</v>
       </c>
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A253" s="29"/>
+      <c r="A253" s="27"/>
       <c r="B253">
         <v>2610</v>
       </c>
-      <c r="C253" s="26" t="s">
-        <v>778</v>
+      <c r="C253" t="s">
+        <v>729</v>
       </c>
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A254" s="29"/>
+      <c r="A254" s="27"/>
       <c r="B254">
         <v>2620</v>
       </c>
-      <c r="C254" s="1" t="str">
-        <f>_xlfn.CONCAT("IF BUSTED=1 THEN ",INDEX(B:B,MATCH(D254,A:A,0),0)," :: REM GOTO ",D254,"")</f>
-        <v>IF BUSTED=1 THEN 2660 :: REM GOTO GAMEOVER</v>
-      </c>
-      <c r="D254" t="str">
-        <f>A258</f>
-        <v>GAMEOVER</v>
+      <c r="C254" s="1" t="s">
+        <v>726</v>
       </c>
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A255" s="29"/>
+      <c r="A255" s="27"/>
       <c r="B255">
         <v>2630</v>
       </c>
-      <c r="C255" s="1" t="s">
-        <v>728</v>
+      <c r="C255" t="str">
+        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D255,A:A,0),0)," :: REM CALL ",D255,"")</f>
+        <v>GOSUB 2870 :: REM CALL CALCSCORE</v>
+      </c>
+      <c r="D255" t="str">
+        <f>A279</f>
+        <v>CALCSCORE</v>
       </c>
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A256" s="29" t="s">
-        <v>771</v>
-      </c>
+      <c r="A256" s="27"/>
       <c r="B256">
         <v>2640</v>
       </c>
       <c r="C256" t="str">
-        <f>_xlfn.CONCAT("REM ***",A256,"***")</f>
-        <v>REM ***TALLY***</v>
+        <f>_xlfn.CONCAT("IF SCORE&gt;=17 THEN ",,INDEX(B:B,MATCH(D256,A:A,0),0)," :: REM GOTO ",D256,"")</f>
+        <v>IF SCORE&gt;=17 THEN 2700 :: REM GOTO TALLY</v>
+      </c>
+      <c r="D256" t="str">
+        <f>A262</f>
+        <v>TALLY</v>
       </c>
     </row>
     <row r="257" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A257" s="28"/>
+      <c r="A257" s="27"/>
       <c r="B257">
         <v>2650</v>
       </c>
       <c r="C257" t="str">
         <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D257,A:A,0),0)," :: REM CALL ",D257,"")</f>
-        <v>GOSUB 2680 :: REM CALL WHOWON</v>
+        <v>GOSUB 2230 :: REM CALL DEAL</v>
       </c>
       <c r="D257" t="str">
-        <f>A260</f>
-        <v>WHOWON</v>
+        <f>A215</f>
+        <v>DEAL</v>
       </c>
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A258" s="29" t="s">
-        <v>765</v>
-      </c>
+      <c r="A258" s="27"/>
       <c r="B258">
         <v>2660</v>
       </c>
-      <c r="C258" t="str">
-        <f>_xlfn.CONCAT("REM ***",A258,"***")</f>
-        <v>REM ***GAMEOVER***</v>
+      <c r="C258" s="1" t="s">
+        <v>768</v>
       </c>
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A259" s="28"/>
+      <c r="A259" s="27"/>
       <c r="B259">
         <v>2670</v>
       </c>
       <c r="C259" t="s">
-        <v>662</v>
+        <v>776</v>
       </c>
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A260" s="28" t="s">
-        <v>614</v>
-      </c>
+      <c r="A260" s="27"/>
       <c r="B260">
         <v>2680</v>
       </c>
-      <c r="C260" s="11" t="str">
-        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A260,"***")</f>
-        <v>REM SUBROUTINE ***WHOWON***</v>
+      <c r="C260" s="1" t="str">
+        <f>_xlfn.CONCAT("IF BUSTED=1 THEN ",INDEX(B:B,MATCH(D260,A:A,0),0)," :: REM GOTO ",D260,"")</f>
+        <v>IF BUSTED=1 THEN 2720 :: REM GOTO GAMEOVER</v>
+      </c>
+      <c r="D260" t="str">
+        <f>A264</f>
+        <v>GAMEOVER</v>
       </c>
     </row>
     <row r="261" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A261" s="28"/>
+      <c r="A261" s="27"/>
       <c r="B261">
         <v>2690</v>
       </c>
-      <c r="C261" t="s">
-        <v>736</v>
+      <c r="C261" s="1" t="s">
+        <v>728</v>
       </c>
     </row>
     <row r="262" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A262" s="28"/>
+      <c r="A262" s="27" t="s">
+        <v>771</v>
+      </c>
       <c r="B262">
         <v>2700</v>
       </c>
       <c r="C262" t="str">
-        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D262,A:A,0),0)," :: REM CALL ",D262,"")</f>
-        <v>GOSUB 2810 :: REM CALL CALCSCORE</v>
-      </c>
-      <c r="D262" t="str">
-        <f>A273</f>
-        <v>CALCSCORE</v>
+        <f>_xlfn.CONCAT("REM ***",A262,"***")</f>
+        <v>REM ***TALLY***</v>
       </c>
     </row>
     <row r="263" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A263" s="28"/>
+      <c r="A263" s="26"/>
       <c r="B263">
         <v>2710</v>
       </c>
-      <c r="C263" t="s">
-        <v>737</v>
+      <c r="C263" t="str">
+        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D263,A:A,0),0)," :: REM CALL ",D263,"")</f>
+        <v>GOSUB 2740 :: REM CALL WHOWON</v>
+      </c>
+      <c r="D263" t="str">
+        <f>A266</f>
+        <v>WHOWON</v>
       </c>
     </row>
     <row r="264" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A264" s="28"/>
+      <c r="A264" s="27" t="s">
+        <v>765</v>
+      </c>
       <c r="B264">
         <v>2720</v>
       </c>
-      <c r="C264" t="s">
-        <v>773</v>
+      <c r="C264" t="str">
+        <f>_xlfn.CONCAT("REM ***",A264,"***")</f>
+        <v>REM ***GAMEOVER***</v>
       </c>
     </row>
     <row r="265" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A265" s="28"/>
+      <c r="A265" s="26"/>
       <c r="B265">
         <v>2730</v>
       </c>
       <c r="C265" t="s">
-        <v>733</v>
+        <v>662</v>
       </c>
     </row>
     <row r="266" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A266" s="28"/>
+      <c r="A266" s="26" t="s">
+        <v>614</v>
+      </c>
       <c r="B266">
         <v>2740</v>
       </c>
-      <c r="C266" t="str">
-        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D266,A:A,0),0)," :: REM CALL ",D266,"")</f>
-        <v>GOSUB 2810 :: REM CALL CALCSCORE</v>
-      </c>
-      <c r="D266" t="str">
-        <f>A273</f>
-        <v>CALCSCORE</v>
+      <c r="C266" s="11" t="str">
+        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A266,"***")</f>
+        <v>REM SUBROUTINE ***WHOWON***</v>
       </c>
     </row>
     <row r="267" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A267" s="28"/>
+      <c r="A267" s="26"/>
       <c r="B267">
         <v>2750</v>
       </c>
       <c r="C267" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
     </row>
     <row r="268" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A268" s="28"/>
+      <c r="A268" s="26"/>
       <c r="B268">
         <v>2760</v>
       </c>
-      <c r="C268" t="s">
-        <v>774</v>
+      <c r="C268" t="str">
+        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D268,A:A,0),0)," :: REM CALL ",D268,"")</f>
+        <v>GOSUB 2870 :: REM CALL CALCSCORE</v>
+      </c>
+      <c r="D268" t="str">
+        <f>A279</f>
+        <v>CALCSCORE</v>
       </c>
     </row>
     <row r="269" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A269" s="28"/>
+      <c r="A269" s="26"/>
       <c r="B269">
         <v>2770</v>
       </c>
       <c r="C269" t="s">
-        <v>775</v>
+        <v>737</v>
       </c>
     </row>
     <row r="270" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A270" s="28"/>
+      <c r="A270" s="26"/>
       <c r="B270">
         <v>2780</v>
       </c>
       <c r="C270" t="s">
-        <v>776</v>
+        <v>817</v>
       </c>
     </row>
     <row r="271" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A271" s="28"/>
+      <c r="A271" s="26"/>
       <c r="B271">
         <v>2790</v>
       </c>
       <c r="C271" t="s">
-        <v>777</v>
+        <v>733</v>
       </c>
     </row>
     <row r="272" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A272" s="28"/>
+      <c r="A272" s="26"/>
       <c r="B272">
         <v>2800</v>
       </c>
-      <c r="C272" t="s">
-        <v>662</v>
+      <c r="C272" t="str">
+        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D272,A:A,0),0)," :: REM CALL ",D272,"")</f>
+        <v>GOSUB 2870 :: REM CALL CALCSCORE</v>
+      </c>
+      <c r="D272" t="str">
+        <f>A279</f>
+        <v>CALCSCORE</v>
       </c>
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A273" s="28" t="s">
-        <v>735</v>
-      </c>
+      <c r="A273" s="26"/>
       <c r="B273">
         <v>2810</v>
       </c>
-      <c r="C273" s="11" t="str">
-        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A273,"***")</f>
-        <v>REM SUBROUTINE ***CALCSCORE***</v>
+      <c r="C273" t="s">
+        <v>738</v>
       </c>
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A274" s="28"/>
+      <c r="A274" s="26"/>
       <c r="B274">
         <v>2820</v>
       </c>
       <c r="C274" t="s">
-        <v>759</v>
+        <v>818</v>
       </c>
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A275" s="28"/>
+      <c r="A275" s="26"/>
       <c r="B275">
         <v>2830</v>
       </c>
       <c r="C275" t="s">
-        <v>761</v>
+        <v>773</v>
       </c>
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A276" s="28"/>
+      <c r="A276" s="26"/>
       <c r="B276">
         <v>2840</v>
       </c>
       <c r="C276" t="s">
-        <v>760</v>
+        <v>774</v>
       </c>
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A277" s="28"/>
+      <c r="A277" s="26"/>
       <c r="B277">
         <v>2850</v>
       </c>
-      <c r="C277" s="11" t="s">
-        <v>781</v>
+      <c r="C277" t="s">
+        <v>775</v>
       </c>
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A278" s="28"/>
+      <c r="A278" s="26"/>
       <c r="B278">
         <v>2860</v>
       </c>
-      <c r="C278" s="11" t="s">
-        <v>57</v>
+      <c r="C278" t="s">
+        <v>662</v>
       </c>
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A279" s="28"/>
+      <c r="A279" s="26" t="s">
+        <v>735</v>
+      </c>
       <c r="B279">
         <v>2870</v>
       </c>
-      <c r="C279" s="11" t="s">
-        <v>662</v>
+      <c r="C279" s="11" t="str">
+        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A279,"***")</f>
+        <v>REM SUBROUTINE ***CALCSCORE***</v>
       </c>
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A280" s="28" t="s">
-        <v>730</v>
-      </c>
+      <c r="A280" s="26"/>
       <c r="B280">
         <v>2880</v>
       </c>
-      <c r="C280" s="11" t="str">
-        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A280,"***")</f>
-        <v>REM SUBROUTINE ***TERMINATE***</v>
+      <c r="C280" t="s">
+        <v>759</v>
       </c>
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A281" s="28"/>
+      <c r="A281" s="26"/>
       <c r="B281">
         <v>2890</v>
       </c>
-      <c r="C281" s="26" t="s">
-        <v>385</v>
+      <c r="C281" t="s">
+        <v>761</v>
       </c>
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A282" s="28"/>
+      <c r="A282" s="26"/>
       <c r="B282">
         <v>2900</v>
       </c>
-      <c r="C282" s="26" t="s">
-        <v>731</v>
+      <c r="C282" t="s">
+        <v>760</v>
       </c>
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A283" s="28"/>
+      <c r="A283" s="26"/>
       <c r="B283">
         <v>2910</v>
       </c>
-      <c r="C283" s="27" t="s">
-        <v>691</v>
+      <c r="C283" s="11" t="s">
+        <v>779</v>
       </c>
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A284" s="28"/>
+      <c r="A284" s="26"/>
       <c r="B284">
         <v>2920</v>
       </c>
-      <c r="C284" t="s">
+      <c r="C284" s="11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="285" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A285" s="26"/>
+      <c r="B285">
+        <v>2930</v>
+      </c>
+      <c r="C285" s="11" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="286" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A286" s="26" t="s">
+        <v>730</v>
+      </c>
+      <c r="B286">
+        <v>2940</v>
+      </c>
+      <c r="C286" s="11" t="str">
+        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A286,"***")</f>
+        <v>REM SUBROUTINE ***TERMINATE***</v>
+      </c>
+    </row>
+    <row r="287" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A287" s="26"/>
+      <c r="B287">
+        <v>2950</v>
+      </c>
+      <c r="C287" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="288" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A288" s="26"/>
+      <c r="B288">
+        <v>2960</v>
+      </c>
+      <c r="C288" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="289" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A289" s="26"/>
+      <c r="B289">
+        <v>2970</v>
+      </c>
+      <c r="C289" s="11" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="290" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A290" s="26"/>
+      <c r="B290">
+        <v>2980</v>
+      </c>
+      <c r="C290" t="s">
         <v>662</v>
       </c>
     </row>
@@ -5963,7 +6033,7 @@
         <v>551</v>
       </c>
       <c r="G2" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -10561,7 +10631,7 @@
         <v/>
       </c>
       <c r="E258" t="str">
-        <f t="shared" ref="E258:E321" si="9">IFERROR(INDEX($A:$A,MATCH(D258,$B:$B,0)),"")</f>
+        <f t="shared" ref="E258:E272" si="9">IFERROR(INDEX($A:$A,MATCH(D258,$B:$B,0)),"")</f>
         <v/>
       </c>
     </row>

</xml_diff>

<commit_message>
clean and changed game to use a single deck instead of just random numbers. also added tidisk for quick loading
</commit_message>
<xml_diff>
--- a/blackjack.xlsx
+++ b/blackjack.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seanwo/projects/ti994a/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2A82851-207F-6549-833A-7614D8E5E506}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC5FE0C4-6925-414E-9B62-8C1C426AB06F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1700" yWindow="500" windowWidth="49500" windowHeight="28300" xr2:uid="{F2DCDACA-2E8A-E041-BEAE-FEED980AFD9D}"/>
+    <workbookView xWindow="7620" yWindow="29560" windowWidth="34560" windowHeight="21580" xr2:uid="{F2DCDACA-2E8A-E041-BEAE-FEED980AFD9D}"/>
   </bookViews>
   <sheets>
     <sheet name="REFACTORED" sheetId="4" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="992" uniqueCount="819">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1005" uniqueCount="829">
   <si>
     <t>1</t>
   </si>
@@ -2222,9 +2222,6 @@
     <t>RENDER2</t>
   </si>
   <si>
-    <t>REM RENDER CENTERPIECE</t>
-  </si>
-  <si>
     <t>CALL HCHAR (4+ROW, 2+COL, CARDCHAR, 1)</t>
   </si>
   <si>
@@ -2261,9 +2258,6 @@
     <t>NEXT H</t>
   </si>
   <si>
-    <t>FOR H=3 TO 5</t>
-  </si>
-  <si>
     <t>TERMINATE</t>
   </si>
   <si>
@@ -2276,9 +2270,6 @@
     <t>PLAYER=1</t>
   </si>
   <si>
-    <t>IF CVAL&lt;14 THEN CVAL=10 ELSE CVAL=1</t>
-  </si>
-  <si>
     <t>CALCSCORE</t>
   </si>
   <si>
@@ -2315,21 +2306,9 @@
     <t>CARDVAL=HANDS(PLAYER,CARD,0)</t>
   </si>
   <si>
-    <t>HANDS(0,0,0)=10 :: HANDS(0,1,0)=14 :: HANDS(0,2,0)=11 :: HANDS(0,3,0)=2 :: HANDS(0,4,0)=3</t>
-  </si>
-  <si>
-    <t>HANDS(0,0,1)=1 :: HANDS(0,1,1)=2 :: HANDS(0,2,1)=3 :: HANDS(0,3,1)=4 :: HANDS(0,4,1)=1</t>
-  </si>
-  <si>
-    <t>HANDS(1,0,1)=1 :: HANDS(1,1,1)=2 :: HANDS(1,2,1)=3 :: HANDS(1,3,1)=4 :: HANDS(1,4,1)=1</t>
-  </si>
-  <si>
     <t>CVAL=HANDS(PLAYER,CARD,0)</t>
   </si>
   <si>
-    <t>DRAWHANDS</t>
-  </si>
-  <si>
     <t>DIM CARDS(1) :: REM CARDS[PLAYER]</t>
   </si>
   <si>
@@ -2375,66 +2354,15 @@
     <t>GOSUB/GOTO LABELS</t>
   </si>
   <si>
-    <t>DEALER</t>
-  </si>
-  <si>
     <t>IF SUMS(1)&gt;21 THEN BUSTED=1</t>
   </si>
   <si>
-    <t>DISPLAY AT (22,1): "DO YOU WANT ANOTHER CARD?"</t>
-  </si>
-  <si>
-    <t>PLAYER</t>
-  </si>
-  <si>
     <t>TALLY</t>
   </si>
   <si>
-    <t>HANDS(1,0,0)=5 :: HANDS(1,1,0)=11 :: HANDS(1,2,0)=3 :: HANDS(1,3,0)=13 :: HANDS(1,4,0)=14</t>
-  </si>
-  <si>
-    <t>IF PSCORE=SCORE THEN DISPLAY AT (12,10): "TIE GAME"</t>
-  </si>
-  <si>
-    <t>IF PSCORE&gt;SCORE THEN DISPLAY AT (12,10): "YOU WIN!"</t>
-  </si>
-  <si>
-    <t>IF PSCORE&lt;SCORE THEN DISPLAY AT (12,10): "YOU LOSE"</t>
-  </si>
-  <si>
-    <t>IF BUSTED=1 THEN DISPLAY AT (12,2) BEEP: "DEALER BUSTED. YOU WIN."</t>
-  </si>
-  <si>
-    <t>IF BUSTED=1 THEN DISPLAY AT (12,3) BEEP: "YOU BUSTED. YOU LOSE."</t>
-  </si>
-  <si>
-    <t>DISPLAY AT (22,1): "                         " :: DISPLAY AT (23,14): " "</t>
-  </si>
-  <si>
     <t>IF HANDS(PLAYER,I,0)=14 THEN SCORE=SCORE+10 :: RETURN</t>
   </si>
   <si>
-    <t>HANDS(0,I,0)=INT(RND*13)+2</t>
-  </si>
-  <si>
-    <t>REM RETURN</t>
-  </si>
-  <si>
-    <t>HANDS(1,I,0)=INT(RND*13)+2</t>
-  </si>
-  <si>
-    <t>HANDS(0,I,1)=INT(RND*4)+1</t>
-  </si>
-  <si>
-    <t>HANDS(1,I,1)=INT(RND*4)+1</t>
-  </si>
-  <si>
-    <t>FOR I=0 TO 4</t>
-  </si>
-  <si>
-    <t>DISPLAY AT (1, 9): "BLACK JACK"</t>
-  </si>
-  <si>
     <t>Dealer code missing!</t>
   </si>
   <si>
@@ -2525,10 +2453,112 @@
     <t>DISPLAY AT (13, 1): "HAND VALUE WINS."</t>
   </si>
   <si>
-    <t>DISPLAY AT (1,24): "P:"&amp;STR$(PSCORE)</t>
-  </si>
-  <si>
-    <t>DISPLAY AT (2,24):"D:"&amp;STR$(DSCORE)</t>
+    <t>REM PLAYERS TURNS</t>
+  </si>
+  <si>
+    <t>REM DEALERS TURNS</t>
+  </si>
+  <si>
+    <t>REM RENDER CARD FACE</t>
+  </si>
+  <si>
+    <t>IF CVAL&gt;10 THEN IF CVAL=14 THEN CVAL=1 ELSE CVAL=10</t>
+  </si>
+  <si>
+    <t>FOR J=3 TO 5</t>
+  </si>
+  <si>
+    <t>NEXT J</t>
+  </si>
+  <si>
+    <t>DIM DECK(9)</t>
+  </si>
+  <si>
+    <t>CHECKDUP</t>
+  </si>
+  <si>
+    <t>DUP=0</t>
+  </si>
+  <si>
+    <t>FOR I=0 TO 9</t>
+  </si>
+  <si>
+    <t>FOR H=0 TO 9</t>
+  </si>
+  <si>
+    <t>DRAWLOOP</t>
+  </si>
+  <si>
+    <t>FOR H=0 TO 4</t>
+  </si>
+  <si>
+    <t>X=INT(RND*4)+1</t>
+  </si>
+  <si>
+    <t>X=X*16</t>
+  </si>
+  <si>
+    <t>X=X+INT(RND*13)+2</t>
+  </si>
+  <si>
+    <t>DECK(H)=X</t>
+  </si>
+  <si>
+    <t>IF DECK(I)=X THEN DUP=1 :: RETURN</t>
+  </si>
+  <si>
+    <t>HANDS(0,H,1)=INT(DECK(H)/16)</t>
+  </si>
+  <si>
+    <t>HANDS(0,H,0)=DECK(H)-HANDS(0,H,1)*16</t>
+  </si>
+  <si>
+    <t>HANDS(1,H,1)=INT(DECK(H+5)/16)</t>
+  </si>
+  <si>
+    <t>HANDS(1,H,0)=DECK(H+5)-HANDS(1,H,1)*16</t>
+  </si>
+  <si>
+    <t>DISPLAY AT (22,2) BEEP: "DO YOU WISH TO PLAY AGAIN?"</t>
+  </si>
+  <si>
+    <t>DISPLAY AT (22,2): "DO YOU WANT ANOTHER CARD?"</t>
+  </si>
+  <si>
+    <t>DISPLAY AT (22,2): "                         " :: DISPLAY AT (23,14): " "</t>
+  </si>
+  <si>
+    <t>IF BUSTED=1 THEN DISPLAY AT (12,4) BEEP: "YOU BUSTED. YOU LOSE."</t>
+  </si>
+  <si>
+    <t>IF BUSTED=1 THEN DISPLAY AT (12,3) BEEP: "DEALER BUSTED. YOU WIN."</t>
+  </si>
+  <si>
+    <t>IF PSCORE=SCORE THEN DISPLAY AT (12,11): "TIE GAME"</t>
+  </si>
+  <si>
+    <t>IF PSCORE&gt;SCORE THEN DISPLAY AT (12,11): "YOU WIN!"</t>
+  </si>
+  <si>
+    <t>IF PSCORE&lt;SCORE THEN DISPLAY AT (12,11): "YOU LOSE"</t>
+  </si>
+  <si>
+    <t>FOR I=1 TO 5 :: CALL CLEAR :: DISPLAY AT (12,7) BEEP: "GAME TERMINATED" :: FOR J=1 TO 100 :: NEXT J :: NEXT I</t>
+  </si>
+  <si>
+    <t>DISPLAY AT(12,6): "SHUFFLING THE DECK"</t>
+  </si>
+  <si>
+    <t>DISPLAY AT(12,6): "                  "</t>
+  </si>
+  <si>
+    <t>REM DISPLAY AT (1,24): "P:"&amp;STR$(PSCORE)</t>
+  </si>
+  <si>
+    <t>REM DISPLAY AT (2,24):"D:"&amp;STR$(DSCORE)</t>
+  </si>
+  <si>
+    <t>SHUFFLE</t>
   </si>
 </sst>
 </file>
@@ -3078,7 +3108,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AB3D0CF-00CA-1047-A168-192C0697CE9E}">
-  <dimension ref="A1:D290"/>
+  <dimension ref="A1:D305"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -3086,7 +3116,7 @@
   <cols>
     <col min="1" max="1" width="18.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="108.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="100.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3101,7 +3131,7 @@
         <v>500</v>
       </c>
       <c r="D1" s="25" t="s">
-        <v>766</v>
+        <v>759</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -3137,7 +3167,7 @@
         <v>120</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>754</v>
+        <v>747</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -3146,7 +3176,7 @@
         <v>130</v>
       </c>
       <c r="C5" t="s">
-        <v>752</v>
+        <v>745</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -3155,7 +3185,7 @@
         <v>140</v>
       </c>
       <c r="C6" t="s">
-        <v>753</v>
+        <v>746</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -3197,14 +3227,14 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="27" t="s">
-        <v>763</v>
+        <v>756</v>
       </c>
       <c r="B10">
         <v>180</v>
       </c>
       <c r="C10" t="str">
-        <f>_xlfn.CONCAT("REM ***",A10,"***")</f>
-        <v>REM ***GAMELOOP***</v>
+        <f>_xlfn.CONCAT("REM LABEL ***",A10,"***")</f>
+        <v>REM LABEL ***GAMELOOP***</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -3214,10 +3244,10 @@
       </c>
       <c r="C11" t="str">
         <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D11,A:A,0),0)," :: REM CALL ",D11,"")</f>
-        <v>GOSUB 2320 :: REM CALL PLAY</v>
+        <v>GOSUB 2470 :: REM CALL PLAY</v>
       </c>
       <c r="D11" t="str">
-        <f>A224</f>
+        <f>A239</f>
         <v>PLAY</v>
       </c>
     </row>
@@ -3227,7 +3257,7 @@
         <v>200</v>
       </c>
       <c r="C12" t="s">
-        <v>430</v>
+        <v>815</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -3246,10 +3276,10 @@
       </c>
       <c r="C14" t="str" cm="1">
         <f t="array" ref="C14">CONCATENATE("IF A$=""N"" THEN GOSUB ",INDEX(B:B,MATCH(D14,A:A,0),0)," :: REM CALL ",D14,"")</f>
-        <v>IF A$="N" THEN GOSUB 2940 :: REM CALL TERMINATE</v>
+        <v>IF A$="N" THEN GOSUB 3090 :: REM CALL TERMINATE</v>
       </c>
       <c r="D14" t="str">
-        <f>A286</f>
+        <f>A301</f>
         <v>TERMINATE</v>
       </c>
     </row>
@@ -3312,7 +3342,7 @@
         <v>280</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>807</v>
+        <v>783</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -3321,7 +3351,7 @@
         <v>290</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>792</v>
+        <v>768</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -3330,7 +3360,7 @@
         <v>300</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>793</v>
+        <v>769</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -3339,7 +3369,7 @@
         <v>310</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>806</v>
+        <v>782</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -3348,7 +3378,7 @@
         <v>320</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>799</v>
+        <v>775</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -3357,7 +3387,7 @@
         <v>330</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>800</v>
+        <v>776</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -3366,7 +3396,7 @@
         <v>340</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>801</v>
+        <v>777</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -3375,7 +3405,7 @@
         <v>350</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>802</v>
+        <v>778</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -3384,7 +3414,7 @@
         <v>360</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>803</v>
+        <v>779</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -3393,7 +3423,7 @@
         <v>370</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>804</v>
+        <v>780</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -3402,7 +3432,7 @@
         <v>380</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>805</v>
+        <v>781</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -3411,7 +3441,7 @@
         <v>390</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>794</v>
+        <v>770</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
@@ -3420,7 +3450,7 @@
         <v>400</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>795</v>
+        <v>771</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
@@ -3429,7 +3459,7 @@
         <v>410</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>796</v>
+        <v>772</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
@@ -3438,7 +3468,7 @@
         <v>420</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>797</v>
+        <v>773</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
@@ -3447,7 +3477,7 @@
         <v>430</v>
       </c>
       <c r="C35" s="11" t="s">
-        <v>788</v>
+        <v>764</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
@@ -3465,7 +3495,7 @@
         <v>450</v>
       </c>
       <c r="C37" s="11" t="s">
-        <v>789</v>
+        <v>765</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
@@ -3474,7 +3504,7 @@
         <v>460</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>790</v>
+        <v>766</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
@@ -3483,7 +3513,7 @@
         <v>470</v>
       </c>
       <c r="C39" s="11" t="s">
-        <v>791</v>
+        <v>767</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
@@ -3492,7 +3522,7 @@
         <v>480</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>808</v>
+        <v>784</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
@@ -3501,7 +3531,7 @@
         <v>490</v>
       </c>
       <c r="C41" s="11" t="s">
-        <v>809</v>
+        <v>785</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
@@ -3510,7 +3540,7 @@
         <v>500</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>810</v>
+        <v>786</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
@@ -3519,7 +3549,7 @@
         <v>510</v>
       </c>
       <c r="C43" s="11" t="s">
-        <v>811</v>
+        <v>787</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
@@ -3528,7 +3558,7 @@
         <v>520</v>
       </c>
       <c r="C44" s="11" t="s">
-        <v>812</v>
+        <v>788</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
@@ -3537,7 +3567,7 @@
         <v>530</v>
       </c>
       <c r="C45" s="11" t="s">
-        <v>813</v>
+        <v>789</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
@@ -3546,7 +3576,7 @@
         <v>540</v>
       </c>
       <c r="C46" s="11" t="s">
-        <v>814</v>
+        <v>790</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
@@ -3555,7 +3585,7 @@
         <v>550</v>
       </c>
       <c r="C47" s="11" t="s">
-        <v>815</v>
+        <v>791</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
@@ -3564,7 +3594,7 @@
         <v>560</v>
       </c>
       <c r="C48" s="11" t="s">
-        <v>816</v>
+        <v>792</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
@@ -3573,7 +3603,7 @@
         <v>570</v>
       </c>
       <c r="C49" s="11" t="s">
-        <v>798</v>
+        <v>774</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
@@ -3582,7 +3612,7 @@
         <v>580</v>
       </c>
       <c r="C50" s="11" t="s">
-        <v>788</v>
+        <v>764</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
@@ -4141,7 +4171,7 @@
         <v>1150</v>
       </c>
       <c r="C107" s="11" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.2">
@@ -4213,7 +4243,7 @@
         <v>1230</v>
       </c>
       <c r="C115" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.2">
@@ -4231,7 +4261,7 @@
         <v>1250</v>
       </c>
       <c r="C117" t="s">
-        <v>740</v>
+        <v>737</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.2">
@@ -4240,7 +4270,7 @@
         <v>1260</v>
       </c>
       <c r="C118" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.2">
@@ -4249,7 +4279,7 @@
         <v>1270</v>
       </c>
       <c r="C119" t="s">
-        <v>742</v>
+        <v>739</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.2">
@@ -4258,7 +4288,7 @@
         <v>1280</v>
       </c>
       <c r="C120" t="s">
-        <v>743</v>
+        <v>740</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.2">
@@ -4276,7 +4306,7 @@
         <v>1300</v>
       </c>
       <c r="C122" t="s">
-        <v>744</v>
+        <v>741</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.2">
@@ -4285,7 +4315,7 @@
         <v>1310</v>
       </c>
       <c r="C123" t="s">
-        <v>745</v>
+        <v>742</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.2">
@@ -4294,7 +4324,7 @@
         <v>1320</v>
       </c>
       <c r="C124" t="s">
-        <v>746</v>
+        <v>743</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.2">
@@ -4303,7 +4333,7 @@
         <v>1330</v>
       </c>
       <c r="C125" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.2">
@@ -4312,7 +4342,7 @@
         <v>1340</v>
       </c>
       <c r="C126" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.2">
@@ -4321,7 +4351,7 @@
         <v>1350</v>
       </c>
       <c r="C127" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.2">
@@ -4330,7 +4360,7 @@
         <v>1360</v>
       </c>
       <c r="C128" t="s">
-        <v>716</v>
+        <v>795</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.2">
@@ -4956,7 +4986,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A193" s="26"/>
       <c r="B193">
         <v>2010</v>
@@ -4965,303 +4995,305 @@
         <v>662</v>
       </c>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A194" s="26" t="s">
         <v>589</v>
       </c>
       <c r="B194">
         <v>2020</v>
       </c>
-      <c r="C194" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C194" s="11" t="str">
+        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A194,"***")</f>
+        <v>REM SUBROUTINE ***RENDERACE***</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A195" s="26"/>
       <c r="B195">
         <v>2030</v>
       </c>
       <c r="C195" t="s">
-        <v>662</v>
-      </c>
-    </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A196" s="26" t="s">
-        <v>751</v>
-      </c>
+        <v>192</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A196" s="26"/>
       <c r="B196">
         <v>2040</v>
       </c>
-      <c r="C196" s="11" t="str">
-        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A196,"***")</f>
-        <v>REM SUBROUTINE ***DRAWHANDS***</v>
-      </c>
-    </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A197" s="26"/>
+      <c r="C196" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A197" s="26" t="s">
+        <v>828</v>
+      </c>
       <c r="B197">
         <v>2050</v>
       </c>
-      <c r="C197" s="11" t="s">
-        <v>747</v>
-      </c>
-    </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C197" s="11" t="str">
+        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A197,"***")</f>
+        <v>REM SUBROUTINE ***SHUFFLE***</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A198" s="26"/>
       <c r="B198">
         <v>2060</v>
       </c>
-      <c r="C198" s="11" t="s">
-        <v>748</v>
-      </c>
-    </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C198" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A199" s="26"/>
       <c r="B199">
         <v>2070</v>
       </c>
-      <c r="C199" s="11" t="s">
-        <v>772</v>
-      </c>
-    </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C199" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A200" s="26"/>
       <c r="B200">
         <v>2080</v>
       </c>
-      <c r="C200" s="11" t="s">
-        <v>749</v>
-      </c>
-    </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A201" s="26"/>
+      <c r="C200" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A201" s="26" t="s">
+        <v>804</v>
+      </c>
       <c r="B201">
         <v>2090</v>
       </c>
-      <c r="C201" s="11" t="s">
-        <v>781</v>
-      </c>
-    </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C201" t="str">
+        <f>_xlfn.CONCAT("REM LABEL ***",A201,"***")</f>
+        <v>REM LABEL ***DRAWLOOP***</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A202" s="26"/>
       <c r="B202">
         <v>2100</v>
       </c>
       <c r="C202" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.2">
+        <v>824</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A203" s="26"/>
       <c r="B203">
         <v>2110</v>
       </c>
-      <c r="C203" s="11" t="s">
-        <v>785</v>
-      </c>
-    </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C203" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A204" s="26"/>
       <c r="B204">
         <v>2120</v>
       </c>
-      <c r="C204" s="11" t="s">
-        <v>780</v>
-      </c>
-    </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C204" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A205" s="26"/>
       <c r="B205">
         <v>2130</v>
       </c>
-      <c r="C205" s="11" t="s">
-        <v>782</v>
-      </c>
-    </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C205" t="s">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A206" s="26"/>
       <c r="B206">
         <v>2140</v>
       </c>
-      <c r="C206" s="11" t="s">
-        <v>783</v>
-      </c>
-    </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C206" t="str">
+        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D206,A:A,0),0)," :: REM CALL ",D206,"")</f>
+        <v>GOSUB 2280 :: REM CALL CHECKDUP</v>
+      </c>
+      <c r="D206" t="str">
+        <f>A220</f>
+        <v>CHECKDUP</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A207" s="26"/>
       <c r="B207">
         <v>2150</v>
       </c>
-      <c r="C207" s="11" t="s">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C207" t="str">
+        <f>_xlfn.CONCAT("IF DUP=1 THEN ",INDEX(B:B,MATCH(D207,A:A,0),0)," :: REM GOTO ",D207,"")</f>
+        <v>IF DUP=1 THEN 2090 :: REM GOTO DRAWLOOP</v>
+      </c>
+      <c r="D207" t="str">
+        <f>A201</f>
+        <v>DRAWLOOP</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A208" s="26"/>
       <c r="B208">
         <v>2160</v>
       </c>
       <c r="C208" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.2">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A209" s="26"/>
       <c r="B209">
         <v>2170</v>
       </c>
-      <c r="C209" s="11" t="s">
-        <v>662</v>
-      </c>
-    </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A210" s="26" t="s">
-        <v>720</v>
-      </c>
+      <c r="C209" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A210" s="26"/>
       <c r="B210">
         <v>2180</v>
       </c>
-      <c r="C210" s="11" t="str">
-        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A210,"***")</f>
-        <v>REM SUBROUTINE ***CLEARTABLE***</v>
-      </c>
-    </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C210" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A211" s="26"/>
       <c r="B211">
         <v>2190</v>
       </c>
       <c r="C211" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.2">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A212" s="26"/>
       <c r="B212">
         <v>2200</v>
       </c>
       <c r="C212" t="s">
-        <v>786</v>
-      </c>
-    </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.2">
+        <v>812</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A213" s="26"/>
       <c r="B213">
         <v>2210</v>
       </c>
       <c r="C213" t="s">
-        <v>755</v>
-      </c>
-    </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.2">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A214" s="26"/>
       <c r="B214">
         <v>2220</v>
       </c>
       <c r="C214" t="s">
-        <v>662</v>
-      </c>
-    </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A215" s="26" t="s">
-        <v>721</v>
-      </c>
+        <v>805</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A215" s="26"/>
       <c r="B215">
         <v>2230</v>
       </c>
-      <c r="C215" s="11" t="str">
-        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A215,"***")</f>
-        <v>REM SUBROUTINE ***DEAL***</v>
-      </c>
-    </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C215" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A216" s="26"/>
       <c r="B216">
         <v>2240</v>
       </c>
-      <c r="C216" s="11" t="s">
-        <v>756</v>
-      </c>
-    </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C216" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A217" s="26"/>
       <c r="B217">
         <v>2250</v>
       </c>
-      <c r="C217" s="11" t="s">
-        <v>757</v>
-      </c>
-    </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C217" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A218" s="26"/>
       <c r="B218">
         <v>2260</v>
       </c>
-      <c r="C218" s="11" t="s">
-        <v>750</v>
-      </c>
-    </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C218" t="s">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A219" s="26"/>
       <c r="B219">
         <v>2270</v>
       </c>
-      <c r="C219" s="11" t="str">
-        <f>_xlfn.CONCAT("IF CVAL&lt;10 THEN ",B221)</f>
-        <v>IF CVAL&lt;10 THEN 2290</v>
-      </c>
-    </row>
-    <row r="220" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A220" s="26"/>
+      <c r="C219" s="11" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A220" s="26" t="s">
+        <v>800</v>
+      </c>
       <c r="B220">
         <v>2280</v>
       </c>
-      <c r="C220" s="11" t="s">
-        <v>734</v>
-      </c>
-    </row>
-    <row r="221" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C220" s="11" t="str">
+        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A220,"***")</f>
+        <v>REM SUBROUTINE ***CHECKDUP***</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A221" s="26"/>
       <c r="B221">
         <v>2290</v>
       </c>
       <c r="C221" s="11" t="s">
-        <v>758</v>
-      </c>
-    </row>
-    <row r="222" spans="1:4" x14ac:dyDescent="0.2">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A222" s="26"/>
       <c r="B222">
         <v>2300</v>
       </c>
-      <c r="C222" t="str">
-        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D222,A:A,0),0)," :: REM CALL ",D222,"")</f>
-        <v>GOSUB 1140 :: REM CALL RENDERCARD</v>
-      </c>
-      <c r="D222" t="str">
-        <f>A106</f>
-        <v>RENDERCARD</v>
-      </c>
-    </row>
-    <row r="223" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C222" s="11" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A223" s="26"/>
       <c r="B223">
         <v>2310</v>
       </c>
       <c r="C223" s="11" t="s">
-        <v>662</v>
-      </c>
-    </row>
-    <row r="224" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A224" s="26" t="s">
-        <v>722</v>
-      </c>
+        <v>810</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A224" s="26"/>
       <c r="B224">
         <v>2320</v>
       </c>
-      <c r="C224" s="11" t="str">
-        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A224,"***")</f>
-        <v>REM SUBROUTINE ***PLAY***</v>
+      <c r="C224" s="11" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.2">
@@ -5269,27 +5301,20 @@
       <c r="B225">
         <v>2330</v>
       </c>
-      <c r="C225" t="str">
-        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D225,A:A,0),0)," :: REM CALL ",D225,"")</f>
-        <v>GOSUB 2180 :: REM CALL CLEARTABLE</v>
-      </c>
-      <c r="D225" t="str">
-        <f>A210</f>
-        <v>CLEARTABLE</v>
+      <c r="C225" s="11" t="s">
+        <v>662</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A226" s="26"/>
+      <c r="A226" s="26" t="s">
+        <v>719</v>
+      </c>
       <c r="B226">
         <v>2340</v>
       </c>
-      <c r="C226" t="str">
-        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D226,A:A,0),0)," :: REM CALL ",D226,"")</f>
-        <v>GOSUB 2040 :: REM CALL DRAWHANDS</v>
-      </c>
-      <c r="D226" t="str">
-        <f>A196</f>
-        <v>DRAWHANDS</v>
+      <c r="C226" s="11" t="str">
+        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A226,"***")</f>
+        <v>REM SUBROUTINE ***CLEARTABLE***</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.2">
@@ -5298,7 +5323,7 @@
         <v>2350</v>
       </c>
       <c r="C227" t="s">
-        <v>725</v>
+        <v>7</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.2">
@@ -5306,13 +5331,8 @@
       <c r="B228">
         <v>2360</v>
       </c>
-      <c r="C228" t="str">
-        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D228,A:A,0),0)," :: REM CALL ",D228,"")</f>
-        <v>GOSUB 2230 :: REM CALL DEAL</v>
-      </c>
-      <c r="D228" t="str">
-        <f>A215</f>
-        <v>DEAL</v>
+      <c r="C228" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.2">
@@ -5320,13 +5340,8 @@
       <c r="B229">
         <v>2370</v>
       </c>
-      <c r="C229" t="str">
-        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D229,A:A,0),0)," :: REM CALL ",D229,"")</f>
-        <v>GOSUB 2230 :: REM CALL DEAL</v>
-      </c>
-      <c r="D229" t="str">
-        <f>A215</f>
-        <v>DEAL</v>
+      <c r="C229" t="s">
+        <v>748</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.2">
@@ -5335,21 +5350,19 @@
         <v>2380</v>
       </c>
       <c r="C230" t="s">
-        <v>726</v>
+        <v>662</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A231" s="26"/>
+      <c r="A231" s="26" t="s">
+        <v>720</v>
+      </c>
       <c r="B231">
         <v>2390</v>
       </c>
-      <c r="C231" t="str">
-        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D231,A:A,0),0)," :: REM CALL ",D231,"")</f>
-        <v>GOSUB 2230 :: REM CALL DEAL</v>
-      </c>
-      <c r="D231" t="str">
-        <f>A215</f>
-        <v>DEAL</v>
+      <c r="C231" s="11" t="str">
+        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A231,"***")</f>
+        <v>REM SUBROUTINE ***DEAL***</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.2">
@@ -5357,8 +5370,8 @@
       <c r="B232">
         <v>2400</v>
       </c>
-      <c r="C232" t="s">
-        <v>727</v>
+      <c r="C232" s="11" t="s">
+        <v>749</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.2">
@@ -5366,25 +5379,17 @@
       <c r="B233">
         <v>2410</v>
       </c>
-      <c r="C233" t="str">
-        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D233,A:A,0),0)," :: REM CALL ",D233,"")</f>
-        <v>GOSUB 2230 :: REM CALL DEAL</v>
-      </c>
-      <c r="D233" t="str">
-        <f>A215</f>
-        <v>DEAL</v>
+      <c r="C233" s="11" t="s">
+        <v>750</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A234" s="26" t="s">
-        <v>770</v>
-      </c>
+      <c r="A234" s="26"/>
       <c r="B234">
         <v>2420</v>
       </c>
-      <c r="C234" t="str">
-        <f>_xlfn.CONCAT("REM ***",A234,"***")</f>
-        <v>REM ***PLAYER***</v>
+      <c r="C234" s="11" t="s">
+        <v>744</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.2">
@@ -5392,8 +5397,8 @@
       <c r="B235">
         <v>2430</v>
       </c>
-      <c r="C235" t="s">
-        <v>739</v>
+      <c r="C235" s="11" t="s">
+        <v>796</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.2">
@@ -5401,8 +5406,8 @@
       <c r="B236">
         <v>2440</v>
       </c>
-      <c r="C236" t="s">
-        <v>729</v>
+      <c r="C236" s="11" t="s">
+        <v>751</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.2">
@@ -5410,8 +5415,13 @@
       <c r="B237">
         <v>2450</v>
       </c>
-      <c r="C237" s="1" t="s">
-        <v>769</v>
+      <c r="C237" t="str">
+        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D237,A:A,0),0)," :: REM CALL ",D237,"")</f>
+        <v>GOSUB 1140 :: REM CALL RENDERCARD</v>
+      </c>
+      <c r="D237" t="str">
+        <f>A106</f>
+        <v>RENDERCARD</v>
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.2">
@@ -5419,17 +5429,20 @@
       <c r="B238">
         <v>2460</v>
       </c>
-      <c r="C238" s="1" t="s">
-        <v>334</v>
+      <c r="C238" s="11" t="s">
+        <v>662</v>
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A239" s="26"/>
+      <c r="A239" s="26" t="s">
+        <v>721</v>
+      </c>
       <c r="B239">
         <v>2470</v>
       </c>
-      <c r="C239" s="1" t="s">
-        <v>778</v>
+      <c r="C239" s="11" t="str">
+        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A239,"***")</f>
+        <v>REM SUBROUTINE ***PLAY***</v>
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.2">
@@ -5437,13 +5450,13 @@
       <c r="B240">
         <v>2480</v>
       </c>
-      <c r="C240" s="1" t="str">
-        <f>_xlfn.CONCAT("IF A$=""N"" THEN ",INDEX(B:B,MATCH(D240,A:A,0),0)," :: REM GOTO ",D240,"")</f>
-        <v>IF A$="N" THEN 2550 :: REM GOTO REVEAL</v>
+      <c r="C240" t="str">
+        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D240,A:A,0),0)," :: REM CALL ",D240,"")</f>
+        <v>GOSUB 2340 :: REM CALL CLEARTABLE</v>
       </c>
       <c r="D240" t="str">
-        <f>A247</f>
-        <v>REVEAL</v>
+        <f>A226</f>
+        <v>CLEARTABLE</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.2">
@@ -5451,8 +5464,13 @@
       <c r="B241">
         <v>2490</v>
       </c>
-      <c r="C241" s="1" t="s">
-        <v>725</v>
+      <c r="C241" t="str">
+        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D241,A:A,0),0)," :: REM CALL ",D241,"")</f>
+        <v>GOSUB 2050 :: REM CALL SHUFFLE</v>
+      </c>
+      <c r="D241" t="str">
+        <f>A197</f>
+        <v>SHUFFLE</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.2">
@@ -5460,13 +5478,8 @@
       <c r="B242">
         <v>2500</v>
       </c>
-      <c r="C242" t="str">
-        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D242,A:A,0),0)," :: REM CALL ",D242,"")</f>
-        <v>GOSUB 2230 :: REM CALL DEAL</v>
-      </c>
-      <c r="D242" t="str">
-        <f>A215</f>
-        <v>DEAL</v>
+      <c r="C242" t="s">
+        <v>724</v>
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.2">
@@ -5474,8 +5487,13 @@
       <c r="B243">
         <v>2510</v>
       </c>
-      <c r="C243" s="1" t="s">
-        <v>762</v>
+      <c r="C243" t="str">
+        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D243,A:A,0),0)," :: REM CALL ",D243,"")</f>
+        <v>GOSUB 2390 :: REM CALL DEAL</v>
+      </c>
+      <c r="D243" t="str">
+        <f>A231</f>
+        <v>DEAL</v>
       </c>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.2">
@@ -5483,8 +5501,13 @@
       <c r="B244">
         <v>2520</v>
       </c>
-      <c r="C244" t="s">
-        <v>777</v>
+      <c r="C244" t="str">
+        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D244,A:A,0),0)," :: REM CALL ",D244,"")</f>
+        <v>GOSUB 2390 :: REM CALL DEAL</v>
+      </c>
+      <c r="D244" t="str">
+        <f>A231</f>
+        <v>DEAL</v>
       </c>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.2">
@@ -5492,13 +5515,8 @@
       <c r="B245">
         <v>2530</v>
       </c>
-      <c r="C245" s="1" t="str">
-        <f>_xlfn.CONCAT("IF BUSTED=1 THEN ",INDEX(B:B,MATCH(D245,A:A,0),0)," :: REM GOTO ",D245,"")</f>
-        <v>IF BUSTED=1 THEN 2550 :: REM GOTO REVEAL</v>
-      </c>
-      <c r="D245" t="str">
-        <f>A247</f>
-        <v>REVEAL</v>
+      <c r="C245" t="s">
+        <v>725</v>
       </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.2">
@@ -5506,20 +5524,22 @@
       <c r="B246">
         <v>2540</v>
       </c>
-      <c r="C246" s="1" t="s">
-        <v>728</v>
+      <c r="C246" t="str">
+        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D246,A:A,0),0)," :: REM CALL ",D246,"")</f>
+        <v>GOSUB 2390 :: REM CALL DEAL</v>
+      </c>
+      <c r="D246" t="str">
+        <f>A231</f>
+        <v>DEAL</v>
       </c>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A247" s="27" t="s">
-        <v>732</v>
-      </c>
+      <c r="A247" s="26"/>
       <c r="B247">
         <v>2550</v>
       </c>
-      <c r="C247" t="str">
-        <f>_xlfn.CONCAT("REM ***",A247,"***")</f>
-        <v>REM ***REVEAL***</v>
+      <c r="C247" t="s">
+        <v>726</v>
       </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.2">
@@ -5527,8 +5547,13 @@
       <c r="B248">
         <v>2560</v>
       </c>
-      <c r="C248" s="1" t="s">
-        <v>764</v>
+      <c r="C248" t="str">
+        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D248,A:A,0),0)," :: REM CALL ",D248,"")</f>
+        <v>GOSUB 2390 :: REM CALL DEAL</v>
+      </c>
+      <c r="D248" t="str">
+        <f>A231</f>
+        <v>DEAL</v>
       </c>
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.2">
@@ -5536,13 +5561,8 @@
       <c r="B249">
         <v>2570</v>
       </c>
-      <c r="C249" t="str">
-        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D249,A:A,0),0)," :: REM CALL ",D249,"")</f>
-        <v>GOSUB 1140 :: REM CALL RENDERCARD</v>
-      </c>
-      <c r="D249" t="str">
-        <f>A106</f>
-        <v>RENDERCARD</v>
+      <c r="C249" t="s">
+        <v>793</v>
       </c>
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.2">
@@ -5550,147 +5570,134 @@
       <c r="B250">
         <v>2580</v>
       </c>
-      <c r="C250" s="1" t="str">
-        <f>_xlfn.CONCAT("IF BUSTED=1 THEN ",INDEX(B:B,MATCH(D250,A:A,0),0)," :: REM GOTO ",D250,"")</f>
-        <v>IF BUSTED=1 THEN 2720 :: REM GOTO GAMEOVER</v>
-      </c>
-      <c r="D250" t="str">
-        <f>A264</f>
-        <v>GAMEOVER</v>
+      <c r="C250" t="s">
+        <v>736</v>
       </c>
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A251" s="27" t="s">
-        <v>767</v>
-      </c>
+      <c r="A251" s="26"/>
       <c r="B251">
         <v>2590</v>
       </c>
-      <c r="C251" t="str">
-        <f>_xlfn.CONCAT("REM ***",A251,"***")</f>
-        <v>REM ***DEALER***</v>
+      <c r="C251" t="s">
+        <v>797</v>
       </c>
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A252" s="27"/>
+      <c r="A252" s="26"/>
       <c r="B252">
         <v>2600</v>
       </c>
-      <c r="C252" t="s">
-        <v>739</v>
+      <c r="C252" s="1" t="s">
+        <v>816</v>
       </c>
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A253" s="27"/>
+      <c r="A253" s="26"/>
       <c r="B253">
         <v>2610</v>
       </c>
-      <c r="C253" t="s">
-        <v>729</v>
+      <c r="C253" s="1" t="s">
+        <v>334</v>
       </c>
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A254" s="27"/>
+      <c r="A254" s="26"/>
       <c r="B254">
         <v>2620</v>
       </c>
       <c r="C254" s="1" t="s">
-        <v>726</v>
+        <v>817</v>
       </c>
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A255" s="27"/>
+      <c r="A255" s="26"/>
       <c r="B255">
         <v>2630</v>
       </c>
-      <c r="C255" t="str">
-        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D255,A:A,0),0)," :: REM CALL ",D255,"")</f>
-        <v>GOSUB 2870 :: REM CALL CALCSCORE</v>
+      <c r="C255" s="1" t="str">
+        <f>_xlfn.CONCAT("IF A$=""N"" THEN ",INDEX(B:B,MATCH(D255,A:A,0),0)," :: REM GOTO ",D255,"")</f>
+        <v>IF A$="N" THEN 2700 :: REM GOTO REVEAL</v>
       </c>
       <c r="D255" t="str">
-        <f>A279</f>
-        <v>CALCSCORE</v>
+        <f>A262</f>
+        <v>REVEAL</v>
       </c>
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A256" s="27"/>
+      <c r="A256" s="26"/>
       <c r="B256">
         <v>2640</v>
       </c>
-      <c r="C256" t="str">
-        <f>_xlfn.CONCAT("IF SCORE&gt;=17 THEN ",,INDEX(B:B,MATCH(D256,A:A,0),0)," :: REM GOTO ",D256,"")</f>
-        <v>IF SCORE&gt;=17 THEN 2700 :: REM GOTO TALLY</v>
-      </c>
-      <c r="D256" t="str">
-        <f>A262</f>
-        <v>TALLY</v>
+      <c r="C256" s="1" t="s">
+        <v>724</v>
       </c>
     </row>
     <row r="257" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A257" s="27"/>
+      <c r="A257" s="26"/>
       <c r="B257">
         <v>2650</v>
       </c>
       <c r="C257" t="str">
         <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D257,A:A,0),0)," :: REM CALL ",D257,"")</f>
-        <v>GOSUB 2230 :: REM CALL DEAL</v>
+        <v>GOSUB 2390 :: REM CALL DEAL</v>
       </c>
       <c r="D257" t="str">
-        <f>A215</f>
+        <f>A231</f>
         <v>DEAL</v>
       </c>
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A258" s="27"/>
+      <c r="A258" s="26"/>
       <c r="B258">
         <v>2660</v>
       </c>
       <c r="C258" s="1" t="s">
-        <v>768</v>
+        <v>755</v>
       </c>
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A259" s="27"/>
+      <c r="A259" s="26"/>
       <c r="B259">
         <v>2670</v>
       </c>
       <c r="C259" t="s">
-        <v>776</v>
+        <v>818</v>
       </c>
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A260" s="27"/>
+      <c r="A260" s="26"/>
       <c r="B260">
         <v>2680</v>
       </c>
       <c r="C260" s="1" t="str">
         <f>_xlfn.CONCAT("IF BUSTED=1 THEN ",INDEX(B:B,MATCH(D260,A:A,0),0)," :: REM GOTO ",D260,"")</f>
-        <v>IF BUSTED=1 THEN 2720 :: REM GOTO GAMEOVER</v>
+        <v>IF BUSTED=1 THEN 2700 :: REM GOTO REVEAL</v>
       </c>
       <c r="D260" t="str">
-        <f>A264</f>
-        <v>GAMEOVER</v>
+        <f>A262</f>
+        <v>REVEAL</v>
       </c>
     </row>
     <row r="261" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A261" s="27"/>
+      <c r="A261" s="26"/>
       <c r="B261">
         <v>2690</v>
       </c>
       <c r="C261" s="1" t="s">
-        <v>728</v>
+        <v>798</v>
       </c>
     </row>
     <row r="262" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A262" s="27" t="s">
-        <v>771</v>
+        <v>730</v>
       </c>
       <c r="B262">
         <v>2700</v>
       </c>
       <c r="C262" t="str">
-        <f>_xlfn.CONCAT("REM ***",A262,"***")</f>
-        <v>REM ***TALLY***</v>
+        <f>_xlfn.CONCAT("REM LABEL ***",A262,"***")</f>
+        <v>REM LABEL ***REVEAL***</v>
       </c>
     </row>
     <row r="263" spans="1:4" x14ac:dyDescent="0.2">
@@ -5698,25 +5705,22 @@
       <c r="B263">
         <v>2710</v>
       </c>
-      <c r="C263" t="str">
-        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D263,A:A,0),0)," :: REM CALL ",D263,"")</f>
-        <v>GOSUB 2740 :: REM CALL WHOWON</v>
-      </c>
-      <c r="D263" t="str">
-        <f>A266</f>
-        <v>WHOWON</v>
+      <c r="C263" s="1" t="s">
+        <v>757</v>
       </c>
     </row>
     <row r="264" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A264" s="27" t="s">
-        <v>765</v>
-      </c>
+      <c r="A264" s="26"/>
       <c r="B264">
         <v>2720</v>
       </c>
       <c r="C264" t="str">
-        <f>_xlfn.CONCAT("REM ***",A264,"***")</f>
-        <v>REM ***GAMEOVER***</v>
+        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D264,A:A,0),0)," :: REM CALL ",D264,"")</f>
+        <v>GOSUB 1140 :: REM CALL RENDERCARD</v>
+      </c>
+      <c r="D264" t="str">
+        <f>A106</f>
+        <v>RENDERCARD</v>
       </c>
     </row>
     <row r="265" spans="1:4" x14ac:dyDescent="0.2">
@@ -5724,24 +5728,26 @@
       <c r="B265">
         <v>2730</v>
       </c>
-      <c r="C265" t="s">
-        <v>662</v>
+      <c r="C265" s="1" t="str">
+        <f>_xlfn.CONCAT("IF BUSTED=1 THEN ",INDEX(B:B,MATCH(D265,A:A,0),0)," :: REM GOTO ",D265,"")</f>
+        <v>IF BUSTED=1 THEN 2870 :: REM GOTO GAMEOVER</v>
+      </c>
+      <c r="D265" t="str">
+        <f>A279</f>
+        <v>GAMEOVER</v>
       </c>
     </row>
     <row r="266" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A266" s="26" t="s">
-        <v>614</v>
-      </c>
+      <c r="A266" s="27"/>
       <c r="B266">
         <v>2740</v>
       </c>
-      <c r="C266" s="11" t="str">
-        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A266,"***")</f>
-        <v>REM SUBROUTINE ***WHOWON***</v>
+      <c r="C266" t="s">
+        <v>794</v>
       </c>
     </row>
     <row r="267" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A267" s="26"/>
+      <c r="A267" s="27"/>
       <c r="B267">
         <v>2750</v>
       </c>
@@ -5750,208 +5756,236 @@
       </c>
     </row>
     <row r="268" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A268" s="26"/>
+      <c r="A268" s="27"/>
       <c r="B268">
         <v>2760</v>
       </c>
-      <c r="C268" t="str">
-        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D268,A:A,0),0)," :: REM CALL ",D268,"")</f>
-        <v>GOSUB 2870 :: REM CALL CALCSCORE</v>
-      </c>
-      <c r="D268" t="str">
-        <f>A279</f>
-        <v>CALCSCORE</v>
+      <c r="C268" t="s">
+        <v>797</v>
       </c>
     </row>
     <row r="269" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A269" s="26"/>
+      <c r="A269" s="27"/>
       <c r="B269">
         <v>2770</v>
       </c>
-      <c r="C269" t="s">
-        <v>737</v>
+      <c r="C269" s="1" t="s">
+        <v>725</v>
       </c>
     </row>
     <row r="270" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A270" s="26"/>
+      <c r="A270" s="27"/>
       <c r="B270">
         <v>2780</v>
       </c>
-      <c r="C270" t="s">
-        <v>817</v>
+      <c r="C270" t="str">
+        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D270,A:A,0),0)," :: REM CALL ",D270,"")</f>
+        <v>GOSUB 3020 :: REM CALL CALCSCORE</v>
+      </c>
+      <c r="D270" t="str">
+        <f>A294</f>
+        <v>CALCSCORE</v>
       </c>
     </row>
     <row r="271" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A271" s="26"/>
+      <c r="A271" s="27"/>
       <c r="B271">
         <v>2790</v>
       </c>
-      <c r="C271" t="s">
-        <v>733</v>
+      <c r="C271" t="str">
+        <f>_xlfn.CONCAT("IF SCORE&gt;=17 THEN ",,INDEX(B:B,MATCH(D271,A:A,0),0)," :: REM GOTO ",D271,"")</f>
+        <v>IF SCORE&gt;=17 THEN 2850 :: REM GOTO TALLY</v>
+      </c>
+      <c r="D271" t="str">
+        <f>A277</f>
+        <v>TALLY</v>
       </c>
     </row>
     <row r="272" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A272" s="26"/>
+      <c r="A272" s="27"/>
       <c r="B272">
         <v>2800</v>
       </c>
       <c r="C272" t="str">
         <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D272,A:A,0),0)," :: REM CALL ",D272,"")</f>
-        <v>GOSUB 2870 :: REM CALL CALCSCORE</v>
+        <v>GOSUB 2390 :: REM CALL DEAL</v>
       </c>
       <c r="D272" t="str">
-        <f>A279</f>
-        <v>CALCSCORE</v>
-      </c>
-    </row>
-    <row r="273" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A273" s="26"/>
+        <f>A231</f>
+        <v>DEAL</v>
+      </c>
+    </row>
+    <row r="273" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A273" s="27"/>
       <c r="B273">
         <v>2810</v>
       </c>
-      <c r="C273" t="s">
-        <v>738</v>
-      </c>
-    </row>
-    <row r="274" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A274" s="26"/>
+      <c r="C273" s="1" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="274" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A274" s="27"/>
       <c r="B274">
         <v>2820</v>
       </c>
       <c r="C274" t="s">
-        <v>818</v>
-      </c>
-    </row>
-    <row r="275" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A275" s="26"/>
+        <v>819</v>
+      </c>
+    </row>
+    <row r="275" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A275" s="27"/>
       <c r="B275">
         <v>2830</v>
       </c>
-      <c r="C275" t="s">
-        <v>773</v>
-      </c>
-    </row>
-    <row r="276" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A276" s="26"/>
+      <c r="C275" s="1" t="str">
+        <f>_xlfn.CONCAT("IF BUSTED=1 THEN ",INDEX(B:B,MATCH(D275,A:A,0),0)," :: REM GOTO ",D275,"")</f>
+        <v>IF BUSTED=1 THEN 2870 :: REM GOTO GAMEOVER</v>
+      </c>
+      <c r="D275" t="str">
+        <f>A279</f>
+        <v>GAMEOVER</v>
+      </c>
+    </row>
+    <row r="276" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A276" s="27"/>
       <c r="B276">
         <v>2840</v>
       </c>
-      <c r="C276" t="s">
-        <v>774</v>
-      </c>
-    </row>
-    <row r="277" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A277" s="26"/>
+      <c r="C276" s="1" t="s">
+        <v>798</v>
+      </c>
+    </row>
+    <row r="277" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A277" s="27" t="s">
+        <v>761</v>
+      </c>
       <c r="B277">
         <v>2850</v>
       </c>
-      <c r="C277" t="s">
-        <v>775</v>
-      </c>
-    </row>
-    <row r="278" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C277" t="str">
+        <f>_xlfn.CONCAT("REM LABEL ***",A277,"***")</f>
+        <v>REM LABEL ***TALLY***</v>
+      </c>
+    </row>
+    <row r="278" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A278" s="26"/>
       <c r="B278">
         <v>2860</v>
       </c>
-      <c r="C278" t="s">
-        <v>662</v>
-      </c>
-    </row>
-    <row r="279" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A279" s="26" t="s">
-        <v>735</v>
+      <c r="C278" t="str">
+        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D278,A:A,0),0)," :: REM CALL ",D278,"")</f>
+        <v>GOSUB 2890 :: REM CALL WHOWON</v>
+      </c>
+      <c r="D278" t="str">
+        <f>A281</f>
+        <v>WHOWON</v>
+      </c>
+    </row>
+    <row r="279" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A279" s="27" t="s">
+        <v>758</v>
       </c>
       <c r="B279">
         <v>2870</v>
       </c>
-      <c r="C279" s="11" t="str">
-        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A279,"***")</f>
-        <v>REM SUBROUTINE ***CALCSCORE***</v>
-      </c>
-    </row>
-    <row r="280" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C279" t="str">
+        <f>_xlfn.CONCAT("REM LABEL ***",A279,"***")</f>
+        <v>REM LABEL ***GAMEOVER***</v>
+      </c>
+    </row>
+    <row r="280" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A280" s="26"/>
       <c r="B280">
         <v>2880</v>
       </c>
       <c r="C280" t="s">
-        <v>759</v>
-      </c>
-    </row>
-    <row r="281" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A281" s="26"/>
+        <v>662</v>
+      </c>
+    </row>
+    <row r="281" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A281" s="26" t="s">
+        <v>614</v>
+      </c>
       <c r="B281">
         <v>2890</v>
       </c>
-      <c r="C281" t="s">
-        <v>761</v>
-      </c>
-    </row>
-    <row r="282" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C281" s="11" t="str">
+        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A281,"***")</f>
+        <v>REM SUBROUTINE ***WHOWON***</v>
+      </c>
+    </row>
+    <row r="282" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A282" s="26"/>
       <c r="B282">
         <v>2900</v>
       </c>
       <c r="C282" t="s">
-        <v>760</v>
-      </c>
-    </row>
-    <row r="283" spans="1:3" x14ac:dyDescent="0.2">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="283" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A283" s="26"/>
       <c r="B283">
         <v>2910</v>
       </c>
-      <c r="C283" s="11" t="s">
-        <v>779</v>
-      </c>
-    </row>
-    <row r="284" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C283" t="str">
+        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D283,A:A,0),0)," :: REM CALL ",D283,"")</f>
+        <v>GOSUB 3020 :: REM CALL CALCSCORE</v>
+      </c>
+      <c r="D283" t="str">
+        <f>A294</f>
+        <v>CALCSCORE</v>
+      </c>
+    </row>
+    <row r="284" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A284" s="26"/>
       <c r="B284">
         <v>2920</v>
       </c>
-      <c r="C284" s="11" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="285" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C284" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="285" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A285" s="26"/>
       <c r="B285">
         <v>2930</v>
       </c>
-      <c r="C285" s="11" t="s">
-        <v>662</v>
-      </c>
-    </row>
-    <row r="286" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A286" s="26" t="s">
-        <v>730</v>
-      </c>
+      <c r="C285" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="286" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A286" s="26"/>
       <c r="B286">
         <v>2940</v>
       </c>
-      <c r="C286" s="11" t="str">
-        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A286,"***")</f>
-        <v>REM SUBROUTINE ***TERMINATE***</v>
-      </c>
-    </row>
-    <row r="287" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C286" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="287" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A287" s="26"/>
       <c r="B287">
         <v>2950</v>
       </c>
-      <c r="C287" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="288" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C287" t="str">
+        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D287,A:A,0),0)," :: REM CALL ",D287,"")</f>
+        <v>GOSUB 3020 :: REM CALL CALCSCORE</v>
+      </c>
+      <c r="D287" t="str">
+        <f>A294</f>
+        <v>CALCSCORE</v>
+      </c>
+    </row>
+    <row r="288" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A288" s="26"/>
       <c r="B288">
         <v>2960</v>
       </c>
       <c r="C288" t="s">
-        <v>731</v>
+        <v>735</v>
       </c>
     </row>
     <row r="289" spans="1:3" x14ac:dyDescent="0.2">
@@ -5959,8 +5993,8 @@
       <c r="B289">
         <v>2970</v>
       </c>
-      <c r="C289" s="11" t="s">
-        <v>691</v>
+      <c r="C289" t="s">
+        <v>827</v>
       </c>
     </row>
     <row r="290" spans="1:3" x14ac:dyDescent="0.2">
@@ -5969,6 +6003,147 @@
         <v>2980</v>
       </c>
       <c r="C290" t="s">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="291" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A291" s="26"/>
+      <c r="B291">
+        <v>2990</v>
+      </c>
+      <c r="C291" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="292" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A292" s="26"/>
+      <c r="B292">
+        <v>3000</v>
+      </c>
+      <c r="C292" t="s">
+        <v>822</v>
+      </c>
+    </row>
+    <row r="293" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A293" s="26"/>
+      <c r="B293">
+        <v>3010</v>
+      </c>
+      <c r="C293" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="294" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A294" s="26" t="s">
+        <v>732</v>
+      </c>
+      <c r="B294">
+        <v>3020</v>
+      </c>
+      <c r="C294" s="11" t="str">
+        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A294,"***")</f>
+        <v>REM SUBROUTINE ***CALCSCORE***</v>
+      </c>
+    </row>
+    <row r="295" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A295" s="26"/>
+      <c r="B295">
+        <v>3030</v>
+      </c>
+      <c r="C295" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="296" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A296" s="26"/>
+      <c r="B296">
+        <v>3040</v>
+      </c>
+      <c r="C296" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="297" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A297" s="26"/>
+      <c r="B297">
+        <v>3050</v>
+      </c>
+      <c r="C297" t="s">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="298" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A298" s="26"/>
+      <c r="B298">
+        <v>3060</v>
+      </c>
+      <c r="C298" s="11" t="s">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="299" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A299" s="26"/>
+      <c r="B299">
+        <v>3070</v>
+      </c>
+      <c r="C299" s="11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="300" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A300" s="26"/>
+      <c r="B300">
+        <v>3080</v>
+      </c>
+      <c r="C300" s="11" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="301" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A301" s="26" t="s">
+        <v>728</v>
+      </c>
+      <c r="B301">
+        <v>3090</v>
+      </c>
+      <c r="C301" s="11" t="str">
+        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A301,"***")</f>
+        <v>REM SUBROUTINE ***TERMINATE***</v>
+      </c>
+    </row>
+    <row r="302" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A302" s="26"/>
+      <c r="B302">
+        <v>3100</v>
+      </c>
+      <c r="C302" t="s">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="303" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A303" s="26"/>
+      <c r="B303">
+        <v>3110</v>
+      </c>
+      <c r="C303" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="304" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A304" s="26"/>
+      <c r="B304">
+        <v>3120</v>
+      </c>
+      <c r="C304" s="11" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="305" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A305" s="26"/>
+      <c r="B305">
+        <v>3130</v>
+      </c>
+      <c r="C305" t="s">
         <v>662</v>
       </c>
     </row>
@@ -6033,7 +6208,7 @@
         <v>551</v>
       </c>
       <c r="G2" t="s">
-        <v>787</v>
+        <v>763</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
added .bas compact logic for getting game under 12K
</commit_message>
<xml_diff>
--- a/blackjack.xlsx
+++ b/blackjack.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seanwo/projects/ti994a/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F91DC8C-8071-654C-9008-1E070874D35E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2119038A-1E5B-D044-91FE-1447A055BB09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7620" yWindow="29560" windowWidth="34560" windowHeight="21580" xr2:uid="{F2DCDACA-2E8A-E041-BEAE-FEED980AFD9D}"/>
+    <workbookView xWindow="1700" yWindow="500" windowWidth="33000" windowHeight="28300" xr2:uid="{F2DCDACA-2E8A-E041-BEAE-FEED980AFD9D}"/>
   </bookViews>
   <sheets>
     <sheet name="REFACTORED" sheetId="4" r:id="rId1"/>
@@ -2863,7 +2863,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -2894,7 +2894,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3255,97 +3254,97 @@
         <v>718</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="30">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B2">
         <v>100</v>
       </c>
-      <c r="C2" s="30" t="s">
+      <c r="C2" t="s">
         <v>863</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="30">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B3">
         <v>110</v>
       </c>
-      <c r="C3" s="30" t="s">
+      <c r="C3" t="s">
         <v>870</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="30">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B4">
         <v>120</v>
       </c>
-      <c r="C4" s="30" t="s">
+      <c r="C4" t="s">
         <v>865</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="30">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B5">
         <v>130</v>
       </c>
-      <c r="C5" s="30" t="s">
+      <c r="C5" t="s">
         <v>866</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="30">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B6">
         <v>140</v>
       </c>
-      <c r="C6" s="30" t="s">
+      <c r="C6" t="s">
         <v>870</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="30">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B7">
         <v>150</v>
       </c>
-      <c r="C7" s="30" t="s">
+      <c r="C7" t="s">
         <v>867</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="30">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B8">
         <v>160</v>
       </c>
-      <c r="C8" s="30" t="s">
+      <c r="C8" t="s">
         <v>868</v>
       </c>
     </row>
-    <row r="9" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="30">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B9">
         <v>170</v>
       </c>
-      <c r="C9" s="30" t="s">
+      <c r="C9" t="s">
         <v>870</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="30">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B10">
         <v>180</v>
       </c>
-      <c r="C10" s="30" t="s">
+      <c r="C10" t="s">
         <v>869</v>
       </c>
     </row>
-    <row r="11" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="30">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B11">
         <v>190</v>
       </c>
-      <c r="C11" s="30" t="s">
+      <c r="C11" t="s">
         <v>864</v>
       </c>
     </row>
-    <row r="12" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="30">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B12">
         <v>200</v>
       </c>
-      <c r="C12" s="30" t="s">
+      <c r="C12" t="s">
         <v>870</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="26"/>
-      <c r="B13" s="30">
+      <c r="B13">
         <v>210</v>
       </c>
       <c r="C13" s="28" t="str">
@@ -3359,7 +3358,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="26"/>
-      <c r="B14" s="30">
+      <c r="B14">
         <v>220</v>
       </c>
       <c r="C14" s="28" t="str">
@@ -3373,7 +3372,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="26"/>
-      <c r="B15" s="30">
+      <c r="B15">
         <v>230</v>
       </c>
       <c r="C15" s="28" t="str">
@@ -3386,20 +3385,19 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="29" t="s">
+      <c r="B16">
+        <v>240</v>
+      </c>
+      <c r="C16" t="str">
+        <f>_xlfn.CONCAT("REM LABEL ***",A17,"***")</f>
+        <v>REM LABEL ***GAMELOOP***</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="29" t="s">
         <v>715</v>
       </c>
-      <c r="B16" s="30">
-        <v>240</v>
-      </c>
-      <c r="C16" t="str">
-        <f>_xlfn.CONCAT("REM LABEL ***",A16,"***")</f>
-        <v>REM LABEL ***GAMELOOP***</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="26"/>
-      <c r="B17" s="30">
+      <c r="B17">
         <v>250</v>
       </c>
       <c r="C17" s="28" t="str">
@@ -3412,21 +3410,20 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="29" t="s">
+      <c r="B18">
+        <v>260</v>
+      </c>
+      <c r="C18" t="str">
+        <f>_xlfn.CONCAT("REM LABEL ***",A19,"***")</f>
+        <v>REM LABEL ***ASKAGAIN***</v>
+      </c>
+      <c r="D18" s="28"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="29" t="s">
         <v>861</v>
       </c>
-      <c r="B18" s="30">
-        <v>260</v>
-      </c>
-      <c r="C18" t="str">
-        <f>_xlfn.CONCAT("REM LABEL ***",A18,"***")</f>
-        <v>REM LABEL ***ASKAGAIN***</v>
-      </c>
-      <c r="D18" s="28"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="26"/>
-      <c r="B19" s="30">
+      <c r="B19">
         <v>270</v>
       </c>
       <c r="C19" t="s">
@@ -3435,7 +3432,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="26"/>
-      <c r="B20" s="30">
+      <c r="B20">
         <v>280</v>
       </c>
       <c r="C20" t="s">
@@ -3444,21 +3441,21 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="26"/>
-      <c r="B21" s="30">
+      <c r="B21">
         <v>290</v>
       </c>
       <c r="C21" t="str">
         <f>_xlfn.CONCAT("IF A$="""" THEN ",INDEX(B:B,MATCH(D21,A:A,0),0)," :: REM GOTO ",D21,"")</f>
-        <v>IF A$="" THEN 260 :: REM GOTO ASKAGAIN</v>
+        <v>IF A$="" THEN 270 :: REM GOTO ASKAGAIN</v>
       </c>
       <c r="D21" s="29" t="str">
-        <f>A18</f>
+        <f>A19</f>
         <v>ASKAGAIN</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="26"/>
-      <c r="B22" s="30">
+      <c r="B22">
         <v>300</v>
       </c>
       <c r="C22" s="28" t="str">
@@ -3472,21 +3469,21 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="26"/>
-      <c r="B23" s="30">
+      <c r="B23">
         <v>310</v>
       </c>
       <c r="C23" t="str">
         <f>_xlfn.CONCAT("GOTO ",INDEX(B:B,MATCH(D23,A:A,0),0)," :: REM GOTO ",D23,"")</f>
-        <v>GOTO 240 :: REM GOTO GAMELOOP</v>
+        <v>GOTO 250 :: REM GOTO GAMELOOP</v>
       </c>
       <c r="D23" s="29" t="str">
-        <f>A16</f>
+        <f>A17</f>
         <v>GAMELOOP</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="26"/>
-      <c r="B24" s="30">
+      <c r="B24">
         <v>320</v>
       </c>
       <c r="C24" t="s">
@@ -3498,7 +3495,7 @@
       <c r="A25" s="28" t="s">
         <v>501</v>
       </c>
-      <c r="B25" s="30">
+      <c r="B25">
         <v>330</v>
       </c>
       <c r="C25" s="11" t="str">
@@ -3508,7 +3505,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="26"/>
-      <c r="B26" s="30">
+      <c r="B26">
         <v>340</v>
       </c>
       <c r="C26" s="11" t="str">
@@ -3518,7 +3515,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="26"/>
-      <c r="B27" s="30">
+      <c r="B27">
         <v>350</v>
       </c>
       <c r="C27" s="11" t="s">
@@ -3527,7 +3524,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="26"/>
-      <c r="B28" s="30">
+      <c r="B28">
         <v>360</v>
       </c>
       <c r="C28" s="11" t="s">
@@ -3536,7 +3533,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="26"/>
-      <c r="B29" s="30">
+      <c r="B29">
         <v>370</v>
       </c>
       <c r="C29" s="11" t="s">
@@ -3545,7 +3542,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="26"/>
-      <c r="B30" s="30">
+      <c r="B30">
         <v>380</v>
       </c>
       <c r="C30" s="11" t="s">
@@ -3554,7 +3551,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="26"/>
-      <c r="B31" s="30">
+      <c r="B31">
         <v>390</v>
       </c>
       <c r="C31" s="11" t="s">
@@ -3563,7 +3560,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="26"/>
-      <c r="B32" s="30">
+      <c r="B32">
         <v>400</v>
       </c>
       <c r="C32" s="11" t="s">
@@ -3572,7 +3569,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="26"/>
-      <c r="B33" s="30">
+      <c r="B33">
         <v>410</v>
       </c>
       <c r="C33" s="11" t="s">
@@ -3581,7 +3578,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="26"/>
-      <c r="B34" s="30">
+      <c r="B34">
         <v>420</v>
       </c>
       <c r="C34" s="11" t="s">
@@ -3590,7 +3587,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="26"/>
-      <c r="B35" s="30">
+      <c r="B35">
         <v>430</v>
       </c>
       <c r="C35" s="11" t="s">
@@ -3599,7 +3596,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="26"/>
-      <c r="B36" s="30">
+      <c r="B36">
         <v>440</v>
       </c>
       <c r="C36" s="11" t="s">
@@ -3608,7 +3605,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="26"/>
-      <c r="B37" s="30">
+      <c r="B37">
         <v>450</v>
       </c>
       <c r="C37" s="11" t="s">
@@ -3617,7 +3614,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="26"/>
-      <c r="B38" s="30">
+      <c r="B38">
         <v>460</v>
       </c>
       <c r="C38" s="11" t="s">
@@ -3626,7 +3623,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="26"/>
-      <c r="B39" s="30">
+      <c r="B39">
         <v>470</v>
       </c>
       <c r="C39" s="11" t="s">
@@ -3635,7 +3632,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="26"/>
-      <c r="B40" s="30">
+      <c r="B40">
         <v>480</v>
       </c>
       <c r="C40" s="11" t="s">
@@ -3644,7 +3641,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="26"/>
-      <c r="B41" s="30">
+      <c r="B41">
         <v>490</v>
       </c>
       <c r="C41" s="11" t="s">
@@ -3653,7 +3650,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="26"/>
-      <c r="B42" s="30">
+      <c r="B42">
         <v>500</v>
       </c>
       <c r="C42" s="11" t="s">
@@ -3662,7 +3659,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="26"/>
-      <c r="B43" s="30">
+      <c r="B43">
         <v>510</v>
       </c>
       <c r="C43" s="11" t="s">
@@ -3671,7 +3668,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="26"/>
-      <c r="B44" s="30">
+      <c r="B44">
         <v>520</v>
       </c>
       <c r="C44" s="11" t="s">
@@ -3680,7 +3677,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="26"/>
-      <c r="B45" s="30">
+      <c r="B45">
         <v>530</v>
       </c>
       <c r="C45" s="11" t="s">
@@ -3689,7 +3686,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="26"/>
-      <c r="B46" s="30">
+      <c r="B46">
         <v>540</v>
       </c>
       <c r="C46" s="11" t="s">
@@ -3698,7 +3695,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="26"/>
-      <c r="B47" s="30">
+      <c r="B47">
         <v>550</v>
       </c>
       <c r="C47" s="11" t="s">
@@ -3707,7 +3704,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="26"/>
-      <c r="B48" s="30">
+      <c r="B48">
         <v>560</v>
       </c>
       <c r="C48" s="11" t="s">
@@ -3716,7 +3713,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="26"/>
-      <c r="B49" s="30">
+      <c r="B49">
         <v>570</v>
       </c>
       <c r="C49" s="11" t="s">
@@ -3725,7 +3722,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="26"/>
-      <c r="B50" s="30">
+      <c r="B50">
         <v>580</v>
       </c>
       <c r="C50" s="11" t="s">
@@ -3734,7 +3731,7 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="26"/>
-      <c r="B51" s="30">
+      <c r="B51">
         <v>590</v>
       </c>
       <c r="C51" s="11" t="s">
@@ -3743,7 +3740,7 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="26"/>
-      <c r="B52" s="30">
+      <c r="B52">
         <v>600</v>
       </c>
       <c r="C52" s="11" t="s">
@@ -3752,7 +3749,7 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="26"/>
-      <c r="B53" s="30">
+      <c r="B53">
         <v>610</v>
       </c>
       <c r="C53" s="11" t="s">
@@ -3761,7 +3758,7 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="26"/>
-      <c r="B54" s="30">
+      <c r="B54">
         <v>620</v>
       </c>
       <c r="C54" s="11" t="s">
@@ -3770,7 +3767,7 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="26"/>
-      <c r="B55" s="30">
+      <c r="B55">
         <v>630</v>
       </c>
       <c r="C55" s="11" t="s">
@@ -3779,7 +3776,7 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="26"/>
-      <c r="B56" s="30">
+      <c r="B56">
         <v>640</v>
       </c>
       <c r="C56" s="11" t="s">
@@ -3788,7 +3785,7 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="26"/>
-      <c r="B57" s="30">
+      <c r="B57">
         <v>650</v>
       </c>
       <c r="C57" s="11" t="s">
@@ -3797,7 +3794,7 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="26"/>
-      <c r="B58" s="30">
+      <c r="B58">
         <v>660</v>
       </c>
       <c r="C58" s="11" t="s">
@@ -3806,7 +3803,7 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="26"/>
-      <c r="B59" s="30">
+      <c r="B59">
         <v>670</v>
       </c>
       <c r="C59" s="11" t="s">
@@ -3815,7 +3812,7 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="26"/>
-      <c r="B60" s="30">
+      <c r="B60">
         <v>680</v>
       </c>
       <c r="C60" s="11" t="s">
@@ -3824,7 +3821,7 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="26"/>
-      <c r="B61" s="30">
+      <c r="B61">
         <v>690</v>
       </c>
       <c r="C61" s="11" t="s">
@@ -3833,7 +3830,7 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" s="26"/>
-      <c r="B62" s="30">
+      <c r="B62">
         <v>700</v>
       </c>
       <c r="C62" s="11" t="s">
@@ -3844,7 +3841,7 @@
       <c r="A63" s="28" t="s">
         <v>662</v>
       </c>
-      <c r="B63" s="30">
+      <c r="B63">
         <v>710</v>
       </c>
       <c r="C63" s="11" t="str">
@@ -3854,7 +3851,7 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" s="26"/>
-      <c r="B64" s="30">
+      <c r="B64">
         <v>720</v>
       </c>
       <c r="C64" s="11" t="str">
@@ -3864,7 +3861,7 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="26"/>
-      <c r="B65" s="30">
+      <c r="B65">
         <v>730</v>
       </c>
       <c r="C65" s="28" t="str">
@@ -3878,7 +3875,7 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" s="26"/>
-      <c r="B66" s="30">
+      <c r="B66">
         <v>740</v>
       </c>
       <c r="C66" s="28" t="str">
@@ -3892,7 +3889,7 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" s="26"/>
-      <c r="B67" s="30">
+      <c r="B67">
         <v>750</v>
       </c>
       <c r="C67" s="28" t="str">
@@ -3906,7 +3903,7 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" s="26"/>
-      <c r="B68" s="30">
+      <c r="B68">
         <v>760</v>
       </c>
       <c r="C68" s="28" t="str">
@@ -3923,7 +3920,7 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" s="26"/>
-      <c r="B69" s="30">
+      <c r="B69">
         <v>770</v>
       </c>
       <c r="C69" t="s">
@@ -3932,7 +3929,7 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" s="26"/>
-      <c r="B70" s="30">
+      <c r="B70">
         <v>780</v>
       </c>
       <c r="C70" s="11" t="s">
@@ -3943,7 +3940,7 @@
       <c r="A71" s="28" t="s">
         <v>853</v>
       </c>
-      <c r="B71" s="30">
+      <c r="B71">
         <v>790</v>
       </c>
       <c r="C71" s="11" t="str">
@@ -3953,7 +3950,7 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" s="28"/>
-      <c r="B72" s="30">
+      <c r="B72">
         <v>800</v>
       </c>
       <c r="C72" s="11" t="str">
@@ -3963,7 +3960,7 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" s="26"/>
-      <c r="B73" s="30">
+      <c r="B73">
         <v>810</v>
       </c>
       <c r="C73" s="28" t="str">
@@ -3980,7 +3977,7 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" s="26"/>
-      <c r="B74" s="30">
+      <c r="B74">
         <v>820</v>
       </c>
       <c r="C74" t="s">
@@ -3989,7 +3986,7 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" s="26"/>
-      <c r="B75" s="30">
+      <c r="B75">
         <v>830</v>
       </c>
       <c r="C75" s="28" t="str">
@@ -4006,7 +4003,7 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" s="26"/>
-      <c r="B76" s="30">
+      <c r="B76">
         <v>840</v>
       </c>
       <c r="C76" t="s">
@@ -4015,7 +4012,7 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" s="26"/>
-      <c r="B77" s="30">
+      <c r="B77">
         <v>850</v>
       </c>
       <c r="C77" s="28" t="str">
@@ -4032,7 +4029,7 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" s="26"/>
-      <c r="B78" s="30">
+      <c r="B78">
         <v>860</v>
       </c>
       <c r="C78" s="28" t="str">
@@ -4049,7 +4046,7 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" s="26"/>
-      <c r="B79" s="30">
+      <c r="B79">
         <v>870</v>
       </c>
       <c r="C79" s="28" t="str">
@@ -4066,7 +4063,7 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" s="26"/>
-      <c r="B80" s="30">
+      <c r="B80">
         <v>880</v>
       </c>
       <c r="C80" t="s">
@@ -4075,7 +4072,7 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" s="26"/>
-      <c r="B81" s="30">
+      <c r="B81">
         <v>890</v>
       </c>
       <c r="C81" s="11" t="s">
@@ -4086,7 +4083,7 @@
       <c r="A82" s="28" t="s">
         <v>854</v>
       </c>
-      <c r="B82" s="30">
+      <c r="B82">
         <v>900</v>
       </c>
       <c r="C82" s="11" t="str">
@@ -4096,7 +4093,7 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" s="28"/>
-      <c r="B83" s="30">
+      <c r="B83">
         <v>910</v>
       </c>
       <c r="C83" s="11" t="str">
@@ -4106,7 +4103,7 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" s="26"/>
-      <c r="B84" s="30">
+      <c r="B84">
         <v>920</v>
       </c>
       <c r="C84" s="28" t="str">
@@ -4123,7 +4120,7 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" s="26"/>
-      <c r="B85" s="30">
+      <c r="B85">
         <v>930</v>
       </c>
       <c r="C85" t="s">
@@ -4132,7 +4129,7 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" s="26"/>
-      <c r="B86" s="30">
+      <c r="B86">
         <v>940</v>
       </c>
       <c r="C86" s="28" t="str">
@@ -4149,7 +4146,7 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" s="26"/>
-      <c r="B87" s="30">
+      <c r="B87">
         <v>950</v>
       </c>
       <c r="C87" t="s">
@@ -4158,7 +4155,7 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" s="26"/>
-      <c r="B88" s="30">
+      <c r="B88">
         <v>960</v>
       </c>
       <c r="C88" s="28" t="str">
@@ -4175,7 +4172,7 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" s="26"/>
-      <c r="B89" s="30">
+      <c r="B89">
         <v>970</v>
       </c>
       <c r="C89" s="28" t="str">
@@ -4192,7 +4189,7 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" s="26"/>
-      <c r="B90" s="30">
+      <c r="B90">
         <v>980</v>
       </c>
       <c r="C90" s="11" t="s">
@@ -4203,7 +4200,7 @@
       <c r="A91" s="28" t="s">
         <v>664</v>
       </c>
-      <c r="B91" s="30">
+      <c r="B91">
         <v>990</v>
       </c>
       <c r="C91" s="11" t="str">
@@ -4213,7 +4210,7 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" s="26"/>
-      <c r="B92" s="30">
+      <c r="B92">
         <v>1000</v>
       </c>
       <c r="C92" s="11" t="str">
@@ -4226,7 +4223,7 @@
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" s="26"/>
-      <c r="B93" s="30">
+      <c r="B93">
         <v>1010</v>
       </c>
       <c r="C93" s="11" t="s">
@@ -4235,7 +4232,7 @@
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" s="26"/>
-      <c r="B94" s="30">
+      <c r="B94">
         <v>1020</v>
       </c>
       <c r="C94" t="s">
@@ -4244,7 +4241,7 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" s="26"/>
-      <c r="B95" s="30">
+      <c r="B95">
         <v>1030</v>
       </c>
       <c r="C95" t="s">
@@ -4253,7 +4250,7 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" s="26"/>
-      <c r="B96" s="30">
+      <c r="B96">
         <v>1040</v>
       </c>
       <c r="C96" t="s">
@@ -4262,7 +4259,7 @@
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" s="26"/>
-      <c r="B97" s="30">
+      <c r="B97">
         <v>1050</v>
       </c>
       <c r="C97" t="s">
@@ -4271,7 +4268,7 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" s="26"/>
-      <c r="B98" s="30">
+      <c r="B98">
         <v>1060</v>
       </c>
       <c r="C98" t="s">
@@ -4280,7 +4277,7 @@
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" s="26"/>
-      <c r="B99" s="30">
+      <c r="B99">
         <v>1070</v>
       </c>
       <c r="C99" t="s">
@@ -4289,7 +4286,7 @@
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" s="26"/>
-      <c r="B100" s="30">
+      <c r="B100">
         <v>1080</v>
       </c>
       <c r="C100" t="s">
@@ -4298,7 +4295,7 @@
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" s="26"/>
-      <c r="B101" s="30">
+      <c r="B101">
         <v>1090</v>
       </c>
       <c r="C101" t="s">
@@ -4307,7 +4304,7 @@
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102" s="26"/>
-      <c r="B102" s="30">
+      <c r="B102">
         <v>1100</v>
       </c>
       <c r="C102" t="s">
@@ -4316,7 +4313,7 @@
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103" s="26"/>
-      <c r="B103" s="30">
+      <c r="B103">
         <v>1110</v>
       </c>
       <c r="C103" t="s">
@@ -4325,7 +4322,7 @@
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104" s="26"/>
-      <c r="B104" s="30">
+      <c r="B104">
         <v>1120</v>
       </c>
       <c r="C104" t="s">
@@ -4334,7 +4331,7 @@
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105" s="26"/>
-      <c r="B105" s="30">
+      <c r="B105">
         <v>1130</v>
       </c>
       <c r="C105" t="s">
@@ -4343,7 +4340,7 @@
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A106" s="26"/>
-      <c r="B106" s="30">
+      <c r="B106">
         <v>1140</v>
       </c>
       <c r="C106" t="s">
@@ -4352,7 +4349,7 @@
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A107" s="26"/>
-      <c r="B107" s="30">
+      <c r="B107">
         <v>1150</v>
       </c>
       <c r="C107" s="11" t="s">
@@ -4363,7 +4360,7 @@
       <c r="A108" s="28" t="s">
         <v>678</v>
       </c>
-      <c r="B108" s="30">
+      <c r="B108">
         <v>1160</v>
       </c>
       <c r="C108" s="11" t="str">
@@ -4373,7 +4370,7 @@
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A109" s="26"/>
-      <c r="B109" s="30">
+      <c r="B109">
         <v>1170</v>
       </c>
       <c r="C109" s="11" t="str">
@@ -4383,7 +4380,7 @@
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A110" s="26"/>
-      <c r="B110" s="30">
+      <c r="B110">
         <v>1180</v>
       </c>
       <c r="C110" s="28" t="str">
@@ -4400,7 +4397,7 @@
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A111" s="26"/>
-      <c r="B111" s="30">
+      <c r="B111">
         <v>1190</v>
       </c>
       <c r="C111" t="s">
@@ -4409,7 +4406,7 @@
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A112" s="26"/>
-      <c r="B112" s="30">
+      <c r="B112">
         <v>1200</v>
       </c>
       <c r="C112" s="28" t="str">
@@ -4426,7 +4423,7 @@
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A113" s="26"/>
-      <c r="B113" s="30">
+      <c r="B113">
         <v>1210</v>
       </c>
       <c r="C113" t="s">
@@ -4435,7 +4432,7 @@
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A114" s="26"/>
-      <c r="B114" s="30">
+      <c r="B114">
         <v>1220</v>
       </c>
       <c r="C114" s="11" t="s">
@@ -4446,7 +4443,7 @@
       <c r="A115" s="28" t="s">
         <v>681</v>
       </c>
-      <c r="B115" s="30">
+      <c r="B115">
         <v>1230</v>
       </c>
       <c r="C115" s="11" t="str">
@@ -4456,7 +4453,7 @@
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A116" s="26"/>
-      <c r="B116" s="30">
+      <c r="B116">
         <v>1240</v>
       </c>
       <c r="C116" s="11" t="str">
@@ -4466,7 +4463,7 @@
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A117" s="26"/>
-      <c r="B117" s="30">
+      <c r="B117">
         <v>1250</v>
       </c>
       <c r="C117" s="11" t="s">
@@ -4475,7 +4472,7 @@
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A118" s="26"/>
-      <c r="B118" s="30">
+      <c r="B118">
         <v>1260</v>
       </c>
       <c r="C118" s="11" t="s">
@@ -4484,7 +4481,7 @@
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A119" s="26"/>
-      <c r="B119" s="30">
+      <c r="B119">
         <v>1270</v>
       </c>
       <c r="C119" s="11" t="s">
@@ -4493,7 +4490,7 @@
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A120" s="26"/>
-      <c r="B120" s="30">
+      <c r="B120">
         <v>1280</v>
       </c>
       <c r="C120" s="11" t="s">
@@ -4502,7 +4499,7 @@
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A121" s="26"/>
-      <c r="B121" s="30">
+      <c r="B121">
         <v>1290</v>
       </c>
       <c r="C121" s="11" t="s">
@@ -4511,7 +4508,7 @@
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A122" s="26"/>
-      <c r="B122" s="30">
+      <c r="B122">
         <v>1300</v>
       </c>
       <c r="C122" s="11" t="s">
@@ -4520,7 +4517,7 @@
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A123" s="26"/>
-      <c r="B123" s="30">
+      <c r="B123">
         <v>1310</v>
       </c>
       <c r="C123" s="11" t="s">
@@ -4529,7 +4526,7 @@
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A124" s="26"/>
-      <c r="B124" s="30">
+      <c r="B124">
         <v>1320</v>
       </c>
       <c r="C124" s="11" t="s">
@@ -4540,7 +4537,7 @@
       <c r="A125" s="28" t="s">
         <v>577</v>
       </c>
-      <c r="B125" s="30">
+      <c r="B125">
         <v>1330</v>
       </c>
       <c r="C125" s="11" t="str">
@@ -4550,7 +4547,7 @@
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A126" s="26"/>
-      <c r="B126" s="30">
+      <c r="B126">
         <v>1340</v>
       </c>
       <c r="C126" s="11" t="str">
@@ -4563,7 +4560,7 @@
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A127" s="26"/>
-      <c r="B127" s="30">
+      <c r="B127">
         <v>1350</v>
       </c>
       <c r="C127" s="28" t="str">
@@ -4584,7 +4581,7 @@
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A128" s="26"/>
-      <c r="B128" s="30">
+      <c r="B128">
         <v>1360</v>
       </c>
       <c r="C128" s="11" t="s">
@@ -4593,7 +4590,7 @@
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A129" s="26"/>
-      <c r="B129" s="30">
+      <c r="B129">
         <v>1370</v>
       </c>
       <c r="C129" s="11" t="s">
@@ -4602,7 +4599,7 @@
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A130" s="26"/>
-      <c r="B130" s="30">
+      <c r="B130">
         <v>1380</v>
       </c>
       <c r="C130" t="s">
@@ -4611,7 +4608,7 @@
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A131" s="26"/>
-      <c r="B131" s="30">
+      <c r="B131">
         <v>1390</v>
       </c>
       <c r="C131" t="s">
@@ -4620,7 +4617,7 @@
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A132" s="26"/>
-      <c r="B132" s="30">
+      <c r="B132">
         <v>1400</v>
       </c>
       <c r="C132" t="s">
@@ -4629,7 +4626,7 @@
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A133" s="26"/>
-      <c r="B133" s="30">
+      <c r="B133">
         <v>1410</v>
       </c>
       <c r="C133" s="28" t="str">
@@ -4646,7 +4643,7 @@
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A134" s="26"/>
-      <c r="B134" s="30">
+      <c r="B134">
         <v>1420</v>
       </c>
       <c r="C134" s="28" t="str">
@@ -4663,7 +4660,7 @@
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A135" s="26"/>
-      <c r="B135" s="30">
+      <c r="B135">
         <v>1430</v>
       </c>
       <c r="C135" t="s">
@@ -4672,7 +4669,7 @@
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A136" s="26"/>
-      <c r="B136" s="30">
+      <c r="B136">
         <v>1440</v>
       </c>
       <c r="C136" t="s">
@@ -4681,7 +4678,7 @@
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A137" s="26"/>
-      <c r="B137" s="30">
+      <c r="B137">
         <v>1450</v>
       </c>
       <c r="C137" t="str">
@@ -4695,7 +4692,7 @@
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A138" s="26"/>
-      <c r="B138" s="30">
+      <c r="B138">
         <v>1460</v>
       </c>
       <c r="C138" t="s">
@@ -4704,7 +4701,7 @@
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A139" s="26"/>
-      <c r="B139" s="30">
+      <c r="B139">
         <v>1470</v>
       </c>
       <c r="C139" s="28" t="str">
@@ -4721,7 +4718,7 @@
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A140" s="26"/>
-      <c r="B140" s="30">
+      <c r="B140">
         <v>1480</v>
       </c>
       <c r="C140" s="28" t="str">
@@ -4738,7 +4735,7 @@
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A141" s="26"/>
-      <c r="B141" s="30">
+      <c r="B141">
         <v>1490</v>
       </c>
       <c r="C141" s="28" t="str">
@@ -4755,7 +4752,7 @@
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A142" s="26"/>
-      <c r="B142" s="30">
+      <c r="B142">
         <v>1500</v>
       </c>
       <c r="C142" s="28" t="str">
@@ -4772,7 +4769,7 @@
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A143" s="26"/>
-      <c r="B143" s="30">
+      <c r="B143">
         <v>1510</v>
       </c>
       <c r="C143" t="s">
@@ -4781,7 +4778,7 @@
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A144" s="26"/>
-      <c r="B144" s="30">
+      <c r="B144">
         <v>1520</v>
       </c>
       <c r="C144" s="28" t="str">
@@ -4798,7 +4795,7 @@
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A145" s="26"/>
-      <c r="B145" s="30">
+      <c r="B145">
         <v>1530</v>
       </c>
       <c r="C145" s="28" t="str">
@@ -4815,7 +4812,7 @@
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A146" s="26"/>
-      <c r="B146" s="30">
+      <c r="B146">
         <v>1540</v>
       </c>
       <c r="C146" t="s">
@@ -4824,7 +4821,7 @@
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A147" s="26"/>
-      <c r="B147" s="30">
+      <c r="B147">
         <v>1550</v>
       </c>
       <c r="C147" t="s">
@@ -4833,7 +4830,7 @@
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A148" s="26"/>
-      <c r="B148" s="30">
+      <c r="B148">
         <v>1560</v>
       </c>
       <c r="C148" t="s">
@@ -4842,7 +4839,7 @@
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A149" s="26"/>
-      <c r="B149" s="30">
+      <c r="B149">
         <v>1570</v>
       </c>
       <c r="C149" t="s">
@@ -4851,7 +4848,7 @@
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A150" s="26"/>
-      <c r="B150" s="30">
+      <c r="B150">
         <v>1580</v>
       </c>
       <c r="C150" t="s">
@@ -4860,7 +4857,7 @@
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A151" s="26"/>
-      <c r="B151" s="30">
+      <c r="B151">
         <v>1590</v>
       </c>
       <c r="C151" s="28" t="str">
@@ -4881,7 +4878,7 @@
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A152" s="26"/>
-      <c r="B152" s="30">
+      <c r="B152">
         <v>1600</v>
       </c>
       <c r="C152" s="28" t="str">
@@ -4902,7 +4899,7 @@
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A153" s="26"/>
-      <c r="B153" s="30">
+      <c r="B153">
         <v>1610</v>
       </c>
       <c r="C153" s="28" t="str">
@@ -4923,7 +4920,7 @@
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A154" s="26"/>
-      <c r="B154" s="30">
+      <c r="B154">
         <v>1620</v>
       </c>
       <c r="C154" s="28" t="str">
@@ -4944,7 +4941,7 @@
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A155" s="26"/>
-      <c r="B155" s="30">
+      <c r="B155">
         <v>1630</v>
       </c>
       <c r="C155" s="28" t="str">
@@ -4965,7 +4962,7 @@
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A156" s="26"/>
-      <c r="B156" s="30">
+      <c r="B156">
         <v>1640</v>
       </c>
       <c r="C156" s="28" t="str">
@@ -4986,7 +4983,7 @@
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A157" s="26"/>
-      <c r="B157" s="30">
+      <c r="B157">
         <v>1650</v>
       </c>
       <c r="C157" s="28" t="str">
@@ -5007,7 +5004,7 @@
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A158" s="26"/>
-      <c r="B158" s="30">
+      <c r="B158">
         <v>1660</v>
       </c>
       <c r="C158" s="28" t="str">
@@ -5028,7 +5025,7 @@
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A159" s="26"/>
-      <c r="B159" s="30">
+      <c r="B159">
         <v>1670</v>
       </c>
       <c r="C159" s="28" t="str">
@@ -5049,7 +5046,7 @@
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A160" s="26"/>
-      <c r="B160" s="30">
+      <c r="B160">
         <v>1680</v>
       </c>
       <c r="C160" s="28" t="str">
@@ -5070,7 +5067,7 @@
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A161" s="26"/>
-      <c r="B161" s="30">
+      <c r="B161">
         <v>1690</v>
       </c>
       <c r="C161" s="28" t="str">
@@ -5091,7 +5088,7 @@
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A162" s="26"/>
-      <c r="B162" s="30">
+      <c r="B162">
         <v>1700</v>
       </c>
       <c r="C162" s="28" t="str">
@@ -5112,7 +5109,7 @@
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A163" s="26"/>
-      <c r="B163" s="30">
+      <c r="B163">
         <v>1710</v>
       </c>
       <c r="C163" s="28" t="str">
@@ -5136,7 +5133,7 @@
         <f>_xlfn.CONCAT(A125,".SUBEND")</f>
         <v>RENDERCARD.SUBEND</v>
       </c>
-      <c r="B164" s="30">
+      <c r="B164">
         <v>1720</v>
       </c>
       <c r="C164" s="11" t="s">
@@ -5147,7 +5144,7 @@
       <c r="A165" s="28" t="s">
         <v>689</v>
       </c>
-      <c r="B165" s="30">
+      <c r="B165">
         <v>1730</v>
       </c>
       <c r="C165" s="11" t="str">
@@ -5157,7 +5154,7 @@
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A166" s="26"/>
-      <c r="B166" s="30">
+      <c r="B166">
         <v>1740</v>
       </c>
       <c r="C166" s="11" t="str">
@@ -5170,7 +5167,7 @@
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A167" s="26"/>
-      <c r="B167" s="30">
+      <c r="B167">
         <v>1750</v>
       </c>
       <c r="C167" t="s">
@@ -5179,7 +5176,7 @@
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A168" s="26"/>
-      <c r="B168" s="30">
+      <c r="B168">
         <v>1760</v>
       </c>
       <c r="C168" t="s">
@@ -5188,7 +5185,7 @@
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A169" s="26"/>
-      <c r="B169" s="30">
+      <c r="B169">
         <v>1770</v>
       </c>
       <c r="C169" s="11" t="s">
@@ -5199,7 +5196,7 @@
       <c r="A170" s="28" t="s">
         <v>578</v>
       </c>
-      <c r="B170" s="30">
+      <c r="B170">
         <v>1780</v>
       </c>
       <c r="C170" s="11" t="str">
@@ -5209,7 +5206,7 @@
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A171" s="26"/>
-      <c r="B171" s="30">
+      <c r="B171">
         <v>1790</v>
       </c>
       <c r="C171" s="11" t="str">
@@ -5222,7 +5219,7 @@
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A172" s="26"/>
-      <c r="B172" s="30">
+      <c r="B172">
         <v>1800</v>
       </c>
       <c r="C172" t="s">
@@ -5231,7 +5228,7 @@
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A173" s="26"/>
-      <c r="B173" s="30">
+      <c r="B173">
         <v>1810</v>
       </c>
       <c r="C173" s="11" t="s">
@@ -5242,7 +5239,7 @@
       <c r="A174" s="28" t="s">
         <v>579</v>
       </c>
-      <c r="B174" s="30">
+      <c r="B174">
         <v>1820</v>
       </c>
       <c r="C174" s="11" t="str">
@@ -5252,7 +5249,7 @@
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A175" s="26"/>
-      <c r="B175" s="30">
+      <c r="B175">
         <v>1830</v>
       </c>
       <c r="C175" s="11" t="str">
@@ -5265,7 +5262,7 @@
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A176" s="26"/>
-      <c r="B176" s="30">
+      <c r="B176">
         <v>1840</v>
       </c>
       <c r="C176" t="s">
@@ -5274,7 +5271,7 @@
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A177" s="26"/>
-      <c r="B177" s="30">
+      <c r="B177">
         <v>1850</v>
       </c>
       <c r="C177" t="s">
@@ -5283,7 +5280,7 @@
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A178" s="26"/>
-      <c r="B178" s="30">
+      <c r="B178">
         <v>1860</v>
       </c>
       <c r="C178" t="s">
@@ -5292,7 +5289,7 @@
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A179" s="26"/>
-      <c r="B179" s="30">
+      <c r="B179">
         <v>1870</v>
       </c>
       <c r="C179" t="s">
@@ -5301,7 +5298,7 @@
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A180" s="26"/>
-      <c r="B180" s="30">
+      <c r="B180">
         <v>1880</v>
       </c>
       <c r="C180" s="11" t="s">
@@ -5312,7 +5309,7 @@
       <c r="A181" s="28" t="s">
         <v>580</v>
       </c>
-      <c r="B181" s="30">
+      <c r="B181">
         <v>1890</v>
       </c>
       <c r="C181" s="11" t="str">
@@ -5322,7 +5319,7 @@
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A182" s="26"/>
-      <c r="B182" s="30">
+      <c r="B182">
         <v>1900</v>
       </c>
       <c r="C182" s="11" t="str">
@@ -5335,7 +5332,7 @@
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A183" s="26"/>
-      <c r="B183" s="30">
+      <c r="B183">
         <v>1910</v>
       </c>
       <c r="C183" s="28" t="str">
@@ -5352,7 +5349,7 @@
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A184" s="26"/>
-      <c r="B184" s="30">
+      <c r="B184">
         <v>1920</v>
       </c>
       <c r="C184" t="s">
@@ -5361,7 +5358,7 @@
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A185" s="26"/>
-      <c r="B185" s="30">
+      <c r="B185">
         <v>1930</v>
       </c>
       <c r="C185" s="11" t="s">
@@ -5372,7 +5369,7 @@
       <c r="A186" s="28" t="s">
         <v>581</v>
       </c>
-      <c r="B186" s="30">
+      <c r="B186">
         <v>1940</v>
       </c>
       <c r="C186" s="11" t="str">
@@ -5382,7 +5379,7 @@
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A187" s="26"/>
-      <c r="B187" s="30">
+      <c r="B187">
         <v>1950</v>
       </c>
       <c r="C187" s="11" t="str">
@@ -5395,7 +5392,7 @@
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A188" s="26"/>
-      <c r="B188" s="30">
+      <c r="B188">
         <v>1960</v>
       </c>
       <c r="C188" t="s">
@@ -5404,7 +5401,7 @@
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A189" s="26"/>
-      <c r="B189" s="30">
+      <c r="B189">
         <v>1970</v>
       </c>
       <c r="C189" t="s">
@@ -5413,7 +5410,7 @@
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A190" s="26"/>
-      <c r="B190" s="30">
+      <c r="B190">
         <v>1980</v>
       </c>
       <c r="C190" s="11" t="s">
@@ -5424,7 +5421,7 @@
       <c r="A191" s="28" t="s">
         <v>582</v>
       </c>
-      <c r="B191" s="30">
+      <c r="B191">
         <v>1990</v>
       </c>
       <c r="C191" s="11" t="str">
@@ -5434,7 +5431,7 @@
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A192" s="26"/>
-      <c r="B192" s="30">
+      <c r="B192">
         <v>2000</v>
       </c>
       <c r="C192" s="11" t="str">
@@ -5447,7 +5444,7 @@
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A193" s="26"/>
-      <c r="B193" s="30">
+      <c r="B193">
         <v>2010</v>
       </c>
       <c r="C193" s="28" t="str">
@@ -5464,7 +5461,7 @@
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A194" s="26"/>
-      <c r="B194" s="30">
+      <c r="B194">
         <v>2020</v>
       </c>
       <c r="C194" t="s">
@@ -5473,7 +5470,7 @@
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A195" s="26"/>
-      <c r="B195" s="30">
+      <c r="B195">
         <v>2030</v>
       </c>
       <c r="C195" s="11" t="s">
@@ -5484,7 +5481,7 @@
       <c r="A196" s="28" t="s">
         <v>583</v>
       </c>
-      <c r="B196" s="30">
+      <c r="B196">
         <v>2040</v>
       </c>
       <c r="C196" s="11" t="str">
@@ -5494,7 +5491,7 @@
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A197" s="26"/>
-      <c r="B197" s="30">
+      <c r="B197">
         <v>2050</v>
       </c>
       <c r="C197" s="11" t="str">
@@ -5507,7 +5504,7 @@
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A198" s="26"/>
-      <c r="B198" s="30">
+      <c r="B198">
         <v>2060</v>
       </c>
       <c r="C198" t="s">
@@ -5516,7 +5513,7 @@
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A199" s="26"/>
-      <c r="B199" s="30">
+      <c r="B199">
         <v>2070</v>
       </c>
       <c r="C199" t="s">
@@ -5525,7 +5522,7 @@
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A200" s="26"/>
-      <c r="B200" s="30">
+      <c r="B200">
         <v>2080</v>
       </c>
       <c r="C200" t="s">
@@ -5534,7 +5531,7 @@
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A201" s="26"/>
-      <c r="B201" s="30">
+      <c r="B201">
         <v>2090</v>
       </c>
       <c r="C201" t="s">
@@ -5543,7 +5540,7 @@
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A202" s="26"/>
-      <c r="B202" s="30">
+      <c r="B202">
         <v>2100</v>
       </c>
       <c r="C202" t="s">
@@ -5552,7 +5549,7 @@
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A203" s="26"/>
-      <c r="B203" s="30">
+      <c r="B203">
         <v>2110</v>
       </c>
       <c r="C203" t="s">
@@ -5561,7 +5558,7 @@
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A204" s="26"/>
-      <c r="B204" s="30">
+      <c r="B204">
         <v>2120</v>
       </c>
       <c r="C204" t="s">
@@ -5570,7 +5567,7 @@
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A205" s="26"/>
-      <c r="B205" s="30">
+      <c r="B205">
         <v>2130</v>
       </c>
       <c r="C205" t="s">
@@ -5579,7 +5576,7 @@
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A206" s="26"/>
-      <c r="B206" s="30">
+      <c r="B206">
         <v>2140</v>
       </c>
       <c r="C206" s="11" t="s">
@@ -5590,7 +5587,7 @@
       <c r="A207" s="28" t="s">
         <v>584</v>
       </c>
-      <c r="B207" s="30">
+      <c r="B207">
         <v>2150</v>
       </c>
       <c r="C207" s="11" t="str">
@@ -5600,7 +5597,7 @@
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A208" s="26"/>
-      <c r="B208" s="30">
+      <c r="B208">
         <v>2160</v>
       </c>
       <c r="C208" s="11" t="str">
@@ -5613,7 +5610,7 @@
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A209" s="26"/>
-      <c r="B209" s="30">
+      <c r="B209">
         <v>2170</v>
       </c>
       <c r="C209" t="s">
@@ -5622,7 +5619,7 @@
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A210" s="26"/>
-      <c r="B210" s="30">
+      <c r="B210">
         <v>2180</v>
       </c>
       <c r="C210" t="s">
@@ -5631,7 +5628,7 @@
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A211" s="26"/>
-      <c r="B211" s="30">
+      <c r="B211">
         <v>2190</v>
       </c>
       <c r="C211" t="s">
@@ -5640,7 +5637,7 @@
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A212" s="26"/>
-      <c r="B212" s="30">
+      <c r="B212">
         <v>2200</v>
       </c>
       <c r="C212" t="s">
@@ -5649,7 +5646,7 @@
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A213" s="26"/>
-      <c r="B213" s="30">
+      <c r="B213">
         <v>2210</v>
       </c>
       <c r="C213" t="s">
@@ -5658,7 +5655,7 @@
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A214" s="26"/>
-      <c r="B214" s="30">
+      <c r="B214">
         <v>2220</v>
       </c>
       <c r="C214" s="11" t="s">
@@ -5669,7 +5666,7 @@
       <c r="A215" s="28" t="s">
         <v>585</v>
       </c>
-      <c r="B215" s="30">
+      <c r="B215">
         <v>2230</v>
       </c>
       <c r="C215" s="11" t="str">
@@ -5679,7 +5676,7 @@
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A216" s="26"/>
-      <c r="B216" s="30">
+      <c r="B216">
         <v>2240</v>
       </c>
       <c r="C216" s="11" t="str">
@@ -5692,7 +5689,7 @@
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A217" s="26"/>
-      <c r="B217" s="30">
+      <c r="B217">
         <v>2250</v>
       </c>
       <c r="C217" t="s">
@@ -5701,7 +5698,7 @@
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A218" s="26"/>
-      <c r="B218" s="30">
+      <c r="B218">
         <v>2260</v>
       </c>
       <c r="C218" t="s">
@@ -5710,7 +5707,7 @@
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A219" s="26"/>
-      <c r="B219" s="30">
+      <c r="B219">
         <v>2270</v>
       </c>
       <c r="C219" s="11" t="s">
@@ -5721,7 +5718,7 @@
       <c r="A220" s="28" t="s">
         <v>586</v>
       </c>
-      <c r="B220" s="30">
+      <c r="B220">
         <v>2280</v>
       </c>
       <c r="C220" s="11" t="str">
@@ -5731,7 +5728,7 @@
     </row>
     <row r="221" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A221" s="26"/>
-      <c r="B221" s="30">
+      <c r="B221">
         <v>2290</v>
       </c>
       <c r="C221" s="11" t="str">
@@ -5744,7 +5741,7 @@
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A222" s="26"/>
-      <c r="B222" s="30">
+      <c r="B222">
         <v>2300</v>
       </c>
       <c r="C222" t="s">
@@ -5753,7 +5750,7 @@
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A223" s="26"/>
-      <c r="B223" s="30">
+      <c r="B223">
         <v>2310</v>
       </c>
       <c r="C223" t="s">
@@ -5762,7 +5759,7 @@
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A224" s="26"/>
-      <c r="B224" s="30">
+      <c r="B224">
         <v>2320</v>
       </c>
       <c r="C224" t="s">
@@ -5771,7 +5768,7 @@
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A225" s="26"/>
-      <c r="B225" s="30">
+      <c r="B225">
         <v>2330</v>
       </c>
       <c r="C225" s="11" t="s">
@@ -5782,7 +5779,7 @@
       <c r="A226" s="28" t="s">
         <v>587</v>
       </c>
-      <c r="B226" s="30">
+      <c r="B226">
         <v>2340</v>
       </c>
       <c r="C226" s="11" t="str">
@@ -5792,7 +5789,7 @@
     </row>
     <row r="227" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A227" s="26"/>
-      <c r="B227" s="30">
+      <c r="B227">
         <v>2350</v>
       </c>
       <c r="C227" s="11" t="str">
@@ -5805,7 +5802,7 @@
     </row>
     <row r="228" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A228" s="26"/>
-      <c r="B228" s="30">
+      <c r="B228">
         <v>2360</v>
       </c>
       <c r="C228" t="s">
@@ -5814,7 +5811,7 @@
     </row>
     <row r="229" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A229" s="26"/>
-      <c r="B229" s="30">
+      <c r="B229">
         <v>2370</v>
       </c>
       <c r="C229" t="s">
@@ -5823,7 +5820,7 @@
     </row>
     <row r="230" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A230" s="26"/>
-      <c r="B230" s="30">
+      <c r="B230">
         <v>2380</v>
       </c>
       <c r="C230" t="s">
@@ -5832,7 +5829,7 @@
     </row>
     <row r="231" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A231" s="26"/>
-      <c r="B231" s="30">
+      <c r="B231">
         <v>2390</v>
       </c>
       <c r="C231" t="s">
@@ -5841,7 +5838,7 @@
     </row>
     <row r="232" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A232" s="26"/>
-      <c r="B232" s="30">
+      <c r="B232">
         <v>2400</v>
       </c>
       <c r="C232" s="11" t="s">
@@ -5852,7 +5849,7 @@
       <c r="A233" s="28" t="s">
         <v>588</v>
       </c>
-      <c r="B233" s="30">
+      <c r="B233">
         <v>2410</v>
       </c>
       <c r="C233" s="11" t="str">
@@ -5862,7 +5859,7 @@
     </row>
     <row r="234" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A234" s="26"/>
-      <c r="B234" s="30">
+      <c r="B234">
         <v>2420</v>
       </c>
       <c r="C234" s="11" t="str">
@@ -5875,7 +5872,7 @@
     </row>
     <row r="235" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A235" s="26"/>
-      <c r="B235" s="30">
+      <c r="B235">
         <v>2430</v>
       </c>
       <c r="C235" t="s">
@@ -5884,7 +5881,7 @@
     </row>
     <row r="236" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A236" s="26"/>
-      <c r="B236" s="30">
+      <c r="B236">
         <v>2440</v>
       </c>
       <c r="C236" t="s">
@@ -5893,7 +5890,7 @@
     </row>
     <row r="237" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A237" s="26"/>
-      <c r="B237" s="30">
+      <c r="B237">
         <v>2450</v>
       </c>
       <c r="C237" t="s">
@@ -5902,7 +5899,7 @@
     </row>
     <row r="238" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A238" s="26"/>
-      <c r="B238" s="30">
+      <c r="B238">
         <v>2460</v>
       </c>
       <c r="C238" t="s">
@@ -5911,7 +5908,7 @@
     </row>
     <row r="239" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A239" s="26"/>
-      <c r="B239" s="30">
+      <c r="B239">
         <v>2470</v>
       </c>
       <c r="C239" s="11" t="s">
@@ -5922,7 +5919,7 @@
       <c r="A240" s="28" t="s">
         <v>589</v>
       </c>
-      <c r="B240" s="30">
+      <c r="B240">
         <v>2480</v>
       </c>
       <c r="C240" s="11" t="str">
@@ -5932,7 +5929,7 @@
     </row>
     <row r="241" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A241" s="26"/>
-      <c r="B241" s="30">
+      <c r="B241">
         <v>2490</v>
       </c>
       <c r="C241" s="11" t="str">
@@ -5945,7 +5942,7 @@
     </row>
     <row r="242" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A242" s="26"/>
-      <c r="B242" s="30">
+      <c r="B242">
         <v>2500</v>
       </c>
       <c r="C242" t="s">
@@ -5954,7 +5951,7 @@
     </row>
     <row r="243" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A243" s="26"/>
-      <c r="B243" s="30">
+      <c r="B243">
         <v>2510</v>
       </c>
       <c r="C243" s="11" t="s">
@@ -5962,10 +5959,10 @@
       </c>
     </row>
     <row r="244" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A244" s="26" t="s">
+      <c r="A244" s="28" t="s">
         <v>695</v>
       </c>
-      <c r="B244" s="30">
+      <c r="B244">
         <v>2520</v>
       </c>
       <c r="C244" s="11" t="str">
@@ -5975,7 +5972,7 @@
     </row>
     <row r="245" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A245" s="26"/>
-      <c r="B245" s="30">
+      <c r="B245">
         <v>2530</v>
       </c>
       <c r="C245" s="11" t="str">
@@ -5985,7 +5982,7 @@
     </row>
     <row r="246" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A246" s="26"/>
-      <c r="B246" s="30">
+      <c r="B246">
         <v>2540</v>
       </c>
       <c r="C246" s="11" t="s">
@@ -5994,7 +5991,7 @@
     </row>
     <row r="247" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A247" s="26"/>
-      <c r="B247" s="30">
+      <c r="B247">
         <v>2550</v>
       </c>
       <c r="C247" t="s">
@@ -6003,7 +6000,7 @@
     </row>
     <row r="248" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A248" s="26"/>
-      <c r="B248" s="30">
+      <c r="B248">
         <v>2560</v>
       </c>
       <c r="C248" t="s">
@@ -6012,7 +6009,7 @@
     </row>
     <row r="249" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A249" s="26"/>
-      <c r="B249" s="30">
+      <c r="B249">
         <v>2570</v>
       </c>
       <c r="C249" s="28" t="str">
@@ -6029,7 +6026,7 @@
     </row>
     <row r="250" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A250" s="26"/>
-      <c r="B250" s="30">
+      <c r="B250">
         <v>2580</v>
       </c>
       <c r="C250" s="28" t="str">
@@ -6046,7 +6043,7 @@
     </row>
     <row r="251" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A251" s="26"/>
-      <c r="B251" s="30">
+      <c r="B251">
         <v>2590</v>
       </c>
       <c r="C251" t="s">
@@ -6055,7 +6052,7 @@
     </row>
     <row r="252" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A252" s="26"/>
-      <c r="B252" s="30">
+      <c r="B252">
         <v>2600</v>
       </c>
       <c r="C252" s="28" t="str">
@@ -6072,7 +6069,7 @@
     </row>
     <row r="253" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A253" s="26"/>
-      <c r="B253" s="30">
+      <c r="B253">
         <v>2610</v>
       </c>
       <c r="C253" s="28" t="str">
@@ -6089,7 +6086,7 @@
     </row>
     <row r="254" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A254" s="26"/>
-      <c r="B254" s="30">
+      <c r="B254">
         <v>2620</v>
       </c>
       <c r="C254" t="s">
@@ -6098,7 +6095,7 @@
     </row>
     <row r="255" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A255" s="26"/>
-      <c r="B255" s="30">
+      <c r="B255">
         <v>2630</v>
       </c>
       <c r="C255" s="28" t="str">
@@ -6115,7 +6112,7 @@
     </row>
     <row r="256" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A256" s="26"/>
-      <c r="B256" s="30">
+      <c r="B256">
         <v>2640</v>
       </c>
       <c r="C256" t="s">
@@ -6124,7 +6121,7 @@
     </row>
     <row r="257" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A257" s="26"/>
-      <c r="B257" s="30">
+      <c r="B257">
         <v>2650</v>
       </c>
       <c r="C257" s="28" t="str">
@@ -6141,7 +6138,7 @@
     </row>
     <row r="258" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A258" s="26"/>
-      <c r="B258" s="30">
+      <c r="B258">
         <v>2660</v>
       </c>
       <c r="C258" t="s">
@@ -6150,7 +6147,7 @@
     </row>
     <row r="259" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A259" s="26"/>
-      <c r="B259" s="30">
+      <c r="B259">
         <v>2670</v>
       </c>
       <c r="C259" t="s">
@@ -6159,7 +6156,7 @@
     </row>
     <row r="260" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A260" s="26"/>
-      <c r="B260" s="30">
+      <c r="B260">
         <v>2680</v>
       </c>
       <c r="C260" t="s">
@@ -6168,7 +6165,7 @@
     </row>
     <row r="261" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A261" s="26"/>
-      <c r="B261" s="30">
+      <c r="B261">
         <v>2690</v>
       </c>
       <c r="C261" s="1" t="s">
@@ -6176,20 +6173,19 @@
       </c>
     </row>
     <row r="262" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A262" s="29" t="s">
+      <c r="B262">
+        <v>2700</v>
+      </c>
+      <c r="C262" t="str">
+        <f>_xlfn.CONCAT("REM LABEL ***",A263,"***")</f>
+        <v>REM LABEL ***ASKANOTHER***</v>
+      </c>
+    </row>
+    <row r="263" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A263" s="29" t="s">
         <v>862</v>
       </c>
-      <c r="B262" s="30">
-        <v>2700</v>
-      </c>
-      <c r="C262" t="str">
-        <f>_xlfn.CONCAT("REM LABEL ***",A262,"***")</f>
-        <v>REM LABEL ***ASKANOTHER***</v>
-      </c>
-    </row>
-    <row r="263" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A263" s="26"/>
-      <c r="B263" s="30">
+      <c r="B263">
         <v>2710</v>
       </c>
       <c r="C263" s="1" t="s">
@@ -6198,21 +6194,21 @@
     </row>
     <row r="264" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A264" s="26"/>
-      <c r="B264" s="30">
+      <c r="B264">
         <v>2720</v>
       </c>
       <c r="C264" t="str">
         <f>_xlfn.CONCAT("IF A$="""" THEN ",INDEX(B:B,MATCH(D264,A:A,0),0)," :: REM GOTO ",D264,"")</f>
-        <v>IF A$="" THEN 2700 :: REM GOTO ASKANOTHER</v>
+        <v>IF A$="" THEN 2710 :: REM GOTO ASKANOTHER</v>
       </c>
       <c r="D264" s="29" t="str">
-        <f>A262</f>
+        <f>A263</f>
         <v>ASKANOTHER</v>
       </c>
     </row>
     <row r="265" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A265" s="26"/>
-      <c r="B265" s="30">
+      <c r="B265">
         <v>2730</v>
       </c>
       <c r="C265" s="1" t="s">
@@ -6221,21 +6217,21 @@
     </row>
     <row r="266" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A266" s="26"/>
-      <c r="B266" s="30">
+      <c r="B266">
         <v>2740</v>
       </c>
       <c r="C266" s="1" t="str">
         <f>_xlfn.CONCAT("IF A$=""N"" THEN ",INDEX(B:B,MATCH(D266,A:A,0),0)," :: REM GOTO ",D266,"")</f>
-        <v>IF A$="N" THEN 2810 :: REM GOTO REVEAL</v>
+        <v>IF A$="N" THEN 2820 :: REM GOTO REVEAL</v>
       </c>
       <c r="D266" s="29" t="str">
-        <f>A273</f>
+        <f>A274</f>
         <v>REVEAL</v>
       </c>
     </row>
     <row r="267" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A267" s="26"/>
-      <c r="B267" s="30">
+      <c r="B267">
         <v>2750</v>
       </c>
       <c r="C267" s="1" t="s">
@@ -6244,7 +6240,7 @@
     </row>
     <row r="268" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A268" s="26"/>
-      <c r="B268" s="30">
+      <c r="B268">
         <v>2760</v>
       </c>
       <c r="C268" s="28" t="str">
@@ -6261,7 +6257,7 @@
     </row>
     <row r="269" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A269" s="26"/>
-      <c r="B269" s="30">
+      <c r="B269">
         <v>2770</v>
       </c>
       <c r="C269" s="1" t="s">
@@ -6270,7 +6266,7 @@
     </row>
     <row r="270" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A270" s="26"/>
-      <c r="B270" s="30">
+      <c r="B270">
         <v>2780</v>
       </c>
       <c r="C270" t="s">
@@ -6279,21 +6275,21 @@
     </row>
     <row r="271" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A271" s="26"/>
-      <c r="B271" s="30">
+      <c r="B271">
         <v>2790</v>
       </c>
       <c r="C271" s="1" t="str">
         <f>_xlfn.CONCAT("IF BUSTED=1 THEN ",INDEX(B:B,MATCH(D271,A:A,0),0)," :: REM GOTO ",D271,"")</f>
-        <v>IF BUSTED=1 THEN 2810 :: REM GOTO REVEAL</v>
+        <v>IF BUSTED=1 THEN 2820 :: REM GOTO REVEAL</v>
       </c>
       <c r="D271" s="29" t="str">
-        <f>A273</f>
+        <f>A274</f>
         <v>REVEAL</v>
       </c>
     </row>
     <row r="272" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A272" s="26"/>
-      <c r="B272" s="30">
+      <c r="B272">
         <v>2800</v>
       </c>
       <c r="C272" s="1" t="s">
@@ -6301,20 +6297,19 @@
       </c>
     </row>
     <row r="273" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A273" s="27" t="s">
+      <c r="B273">
+        <v>2810</v>
+      </c>
+      <c r="C273" t="str">
+        <f>_xlfn.CONCAT("REM LABEL ***",A274,"***")</f>
+        <v>REM LABEL ***REVEAL***</v>
+      </c>
+    </row>
+    <row r="274" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A274" s="27" t="s">
         <v>702</v>
       </c>
-      <c r="B273" s="30">
-        <v>2810</v>
-      </c>
-      <c r="C273" t="str">
-        <f>_xlfn.CONCAT("REM LABEL ***",A273,"***")</f>
-        <v>REM LABEL ***REVEAL***</v>
-      </c>
-    </row>
-    <row r="274" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A274" s="26"/>
-      <c r="B274" s="30">
+      <c r="B274">
         <v>2820</v>
       </c>
       <c r="C274" s="1" t="s">
@@ -6323,7 +6318,7 @@
     </row>
     <row r="275" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A275" s="26"/>
-      <c r="B275" s="30">
+      <c r="B275">
         <v>2830</v>
       </c>
       <c r="C275" s="28" t="str">
@@ -6340,21 +6335,21 @@
     </row>
     <row r="276" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A276" s="26"/>
-      <c r="B276" s="30">
+      <c r="B276">
         <v>2840</v>
       </c>
       <c r="C276" s="1" t="str">
         <f>_xlfn.CONCAT("IF BUSTED=1 THEN ",INDEX(B:B,MATCH(D276,A:A,0),0)," :: REM GOTO ",D276,"")</f>
-        <v>IF BUSTED=1 THEN 2980 :: REM GOTO GAMEOVER</v>
+        <v>IF BUSTED=1 THEN 2990 :: REM GOTO GAMEOVER</v>
       </c>
       <c r="D276" s="29" t="str">
-        <f>A290</f>
+        <f>A291</f>
         <v>GAMEOVER</v>
       </c>
     </row>
     <row r="277" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A277" s="27"/>
-      <c r="B277" s="30">
+      <c r="B277">
         <v>2850</v>
       </c>
       <c r="C277" t="s">
@@ -6363,7 +6358,7 @@
     </row>
     <row r="278" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A278" s="27"/>
-      <c r="B278" s="30">
+      <c r="B278">
         <v>2860</v>
       </c>
       <c r="C278" t="s">
@@ -6372,7 +6367,7 @@
     </row>
     <row r="279" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A279" s="27"/>
-      <c r="B279" s="30">
+      <c r="B279">
         <v>2870</v>
       </c>
       <c r="C279" t="s">
@@ -6381,7 +6376,7 @@
     </row>
     <row r="280" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A280" s="27"/>
-      <c r="B280" s="30">
+      <c r="B280">
         <v>2880</v>
       </c>
       <c r="C280" s="1" t="s">
@@ -6390,7 +6385,7 @@
     </row>
     <row r="281" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A281" s="27"/>
-      <c r="B281" s="30">
+      <c r="B281">
         <v>2890</v>
       </c>
       <c r="C281" s="28" t="str">
@@ -6407,21 +6402,21 @@
     </row>
     <row r="282" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A282" s="27"/>
-      <c r="B282" s="30">
+      <c r="B282">
         <v>2900</v>
       </c>
       <c r="C282" t="str">
         <f>_xlfn.CONCAT("IF SCORE&gt;=17 THEN ",,INDEX(B:B,MATCH(D282,A:A,0),0)," :: REM GOTO ",D282,"")</f>
-        <v>IF SCORE&gt;=17 THEN 2960 :: REM GOTO TALLY</v>
+        <v>IF SCORE&gt;=17 THEN 2970 :: REM GOTO TALLY</v>
       </c>
       <c r="D282" s="29" t="str">
-        <f>A288</f>
+        <f>A289</f>
         <v>TALLY</v>
       </c>
     </row>
     <row r="283" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A283" s="27"/>
-      <c r="B283" s="30">
+      <c r="B283">
         <v>2910</v>
       </c>
       <c r="C283" s="28" t="str">
@@ -6438,7 +6433,7 @@
     </row>
     <row r="284" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A284" s="27"/>
-      <c r="B284" s="30">
+      <c r="B284">
         <v>2920</v>
       </c>
       <c r="C284" s="1" t="s">
@@ -6447,7 +6442,7 @@
     </row>
     <row r="285" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A285" s="27"/>
-      <c r="B285" s="30">
+      <c r="B285">
         <v>2930</v>
       </c>
       <c r="C285" t="s">
@@ -6456,21 +6451,21 @@
     </row>
     <row r="286" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A286" s="27"/>
-      <c r="B286" s="30">
+      <c r="B286">
         <v>2940</v>
       </c>
       <c r="C286" s="1" t="str">
         <f>_xlfn.CONCAT("IF BUSTED=1 THEN ",INDEX(B:B,MATCH(D286,A:A,0),0)," :: REM GOTO ",D286,"")</f>
-        <v>IF BUSTED=1 THEN 2980 :: REM GOTO GAMEOVER</v>
+        <v>IF BUSTED=1 THEN 2990 :: REM GOTO GAMEOVER</v>
       </c>
       <c r="D286" s="29" t="str">
-        <f>A290</f>
+        <f>A291</f>
         <v>GAMEOVER</v>
       </c>
     </row>
     <row r="287" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A287" s="27"/>
-      <c r="B287" s="30">
+      <c r="B287">
         <v>2950</v>
       </c>
       <c r="C287" s="1" t="s">
@@ -6478,20 +6473,19 @@
       </c>
     </row>
     <row r="288" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A288" s="27" t="s">
+      <c r="B288">
+        <v>2960</v>
+      </c>
+      <c r="C288" t="str">
+        <f>_xlfn.CONCAT("REM LABEL ***",A289,"***")</f>
+        <v>REM LABEL ***TALLY***</v>
+      </c>
+    </row>
+    <row r="289" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A289" s="27" t="s">
         <v>719</v>
       </c>
-      <c r="B288" s="30">
-        <v>2960</v>
-      </c>
-      <c r="C288" t="str">
-        <f>_xlfn.CONCAT("REM LABEL ***",A288,"***")</f>
-        <v>REM LABEL ***TALLY***</v>
-      </c>
-    </row>
-    <row r="289" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A289" s="26"/>
-      <c r="B289" s="30">
+      <c r="B289">
         <v>2970</v>
       </c>
       <c r="C289" s="28" t="str">
@@ -6507,20 +6501,19 @@
       </c>
     </row>
     <row r="290" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A290" s="27" t="s">
+      <c r="B290">
+        <v>2980</v>
+      </c>
+      <c r="C290" t="str">
+        <f>_xlfn.CONCAT("REM LABEL ***",A291,"***")</f>
+        <v>REM LABEL ***GAMEOVER***</v>
+      </c>
+    </row>
+    <row r="291" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A291" s="27" t="s">
         <v>717</v>
       </c>
-      <c r="B290" s="30">
-        <v>2980</v>
-      </c>
-      <c r="C290" t="str">
-        <f>_xlfn.CONCAT("REM LABEL ***",A290,"***")</f>
-        <v>REM LABEL ***GAMEOVER***</v>
-      </c>
-    </row>
-    <row r="291" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A291" s="26"/>
-      <c r="B291" s="30">
+      <c r="B291">
         <v>2990</v>
       </c>
       <c r="C291" t="s">
@@ -6531,7 +6524,7 @@
       <c r="A292" s="28" t="s">
         <v>693</v>
       </c>
-      <c r="B292" s="30">
+      <c r="B292">
         <v>3000</v>
       </c>
       <c r="C292" s="11" t="str">
@@ -6541,7 +6534,7 @@
     </row>
     <row r="293" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A293" s="26"/>
-      <c r="B293" s="30">
+      <c r="B293">
         <v>3010</v>
       </c>
       <c r="C293" s="11" t="str">
@@ -6554,7 +6547,7 @@
     </row>
     <row r="294" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A294" s="26"/>
-      <c r="B294" s="30">
+      <c r="B294">
         <v>3020</v>
       </c>
       <c r="C294" t="s">
@@ -6563,7 +6556,7 @@
     </row>
     <row r="295" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A295" s="26"/>
-      <c r="B295" s="30">
+      <c r="B295">
         <v>3030</v>
       </c>
       <c r="C295" t="s">
@@ -6572,7 +6565,7 @@
     </row>
     <row r="296" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A296" s="26"/>
-      <c r="B296" s="30">
+      <c r="B296">
         <v>3040</v>
       </c>
       <c r="C296" t="s">
@@ -6581,7 +6574,7 @@
     </row>
     <row r="297" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A297" s="26"/>
-      <c r="B297" s="30">
+      <c r="B297">
         <v>3050</v>
       </c>
       <c r="C297" t="s">
@@ -6590,7 +6583,7 @@
     </row>
     <row r="298" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A298" s="26"/>
-      <c r="B298" s="30">
+      <c r="B298">
         <v>3060</v>
       </c>
       <c r="C298" t="s">
@@ -6601,7 +6594,7 @@
       <c r="A299" s="28" t="s">
         <v>780</v>
       </c>
-      <c r="B299" s="30">
+      <c r="B299">
         <v>3070</v>
       </c>
       <c r="C299" s="11" t="str">
@@ -6611,7 +6604,7 @@
     </row>
     <row r="300" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A300" s="26"/>
-      <c r="B300" s="30">
+      <c r="B300">
         <v>3080</v>
       </c>
       <c r="C300" s="11" t="str">
@@ -6624,7 +6617,7 @@
     </row>
     <row r="301" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A301" s="26"/>
-      <c r="B301" s="30">
+      <c r="B301">
         <v>3090</v>
       </c>
       <c r="C301" t="s">
@@ -6633,7 +6626,7 @@
     </row>
     <row r="302" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A302" s="26"/>
-      <c r="B302" s="30">
+      <c r="B302">
         <v>3100</v>
       </c>
       <c r="C302" t="s">
@@ -6642,7 +6635,7 @@
     </row>
     <row r="303" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A303" s="26"/>
-      <c r="B303" s="30">
+      <c r="B303">
         <v>3110</v>
       </c>
       <c r="C303" t="s">
@@ -6650,20 +6643,19 @@
       </c>
     </row>
     <row r="304" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A304" s="29" t="s">
+      <c r="B304">
+        <v>3120</v>
+      </c>
+      <c r="C304" t="str">
+        <f>_xlfn.CONCAT("REM LABEL ***",A305,"***")</f>
+        <v>REM LABEL ***DRAWLOOP***</v>
+      </c>
+    </row>
+    <row r="305" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A305" s="29" t="s">
         <v>760</v>
       </c>
-      <c r="B304" s="30">
-        <v>3120</v>
-      </c>
-      <c r="C304" t="str">
-        <f>_xlfn.CONCAT("REM LABEL ***",A304,"***")</f>
-        <v>REM LABEL ***DRAWLOOP***</v>
-      </c>
-    </row>
-    <row r="305" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A305" s="26"/>
-      <c r="B305" s="30">
+      <c r="B305">
         <v>3130</v>
       </c>
       <c r="C305" t="s">
@@ -6672,7 +6664,7 @@
     </row>
     <row r="306" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A306" s="26"/>
-      <c r="B306" s="30">
+      <c r="B306">
         <v>3140</v>
       </c>
       <c r="C306" t="s">
@@ -6681,7 +6673,7 @@
     </row>
     <row r="307" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A307" s="26"/>
-      <c r="B307" s="30">
+      <c r="B307">
         <v>3150</v>
       </c>
       <c r="C307" t="s">
@@ -6690,7 +6682,7 @@
     </row>
     <row r="308" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A308" s="26"/>
-      <c r="B308" s="30">
+      <c r="B308">
         <v>3160</v>
       </c>
       <c r="C308" t="s">
@@ -6699,7 +6691,7 @@
     </row>
     <row r="309" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A309" s="26"/>
-      <c r="B309" s="30">
+      <c r="B309">
         <v>3170</v>
       </c>
       <c r="C309" t="s">
@@ -6708,7 +6700,7 @@
     </row>
     <row r="310" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A310" s="26"/>
-      <c r="B310" s="30">
+      <c r="B310">
         <v>3180</v>
       </c>
       <c r="C310" s="28" t="str">
@@ -6725,21 +6717,21 @@
     </row>
     <row r="311" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A311" s="26"/>
-      <c r="B311" s="30">
+      <c r="B311">
         <v>3190</v>
       </c>
       <c r="C311" t="str">
         <f>_xlfn.CONCAT("IF DUP=1 THEN ",INDEX(B:B,MATCH(D311,A:A,0),0)," :: REM GOTO ",D311,"")</f>
-        <v>IF DUP=1 THEN 3120 :: REM GOTO DRAWLOOP</v>
+        <v>IF DUP=1 THEN 3130 :: REM GOTO DRAWLOOP</v>
       </c>
       <c r="D311" s="29" t="str">
-        <f>A304</f>
+        <f>A305</f>
         <v>DRAWLOOP</v>
       </c>
     </row>
     <row r="312" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A312" s="26"/>
-      <c r="B312" s="30">
+      <c r="B312">
         <v>3200</v>
       </c>
       <c r="C312" t="s">
@@ -6748,7 +6740,7 @@
     </row>
     <row r="313" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A313" s="26"/>
-      <c r="B313" s="30">
+      <c r="B313">
         <v>3210</v>
       </c>
       <c r="C313" t="s">
@@ -6757,7 +6749,7 @@
     </row>
     <row r="314" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A314" s="26"/>
-      <c r="B314" s="30">
+      <c r="B314">
         <v>3220</v>
       </c>
       <c r="C314" t="s">
@@ -6766,7 +6758,7 @@
     </row>
     <row r="315" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A315" s="26"/>
-      <c r="B315" s="30">
+      <c r="B315">
         <v>3230</v>
       </c>
       <c r="C315" t="s">
@@ -6775,7 +6767,7 @@
     </row>
     <row r="316" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A316" s="26"/>
-      <c r="B316" s="30">
+      <c r="B316">
         <v>3240</v>
       </c>
       <c r="C316" t="s">
@@ -6784,7 +6776,7 @@
     </row>
     <row r="317" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A317" s="26"/>
-      <c r="B317" s="30">
+      <c r="B317">
         <v>3250</v>
       </c>
       <c r="C317" t="s">
@@ -6793,7 +6785,7 @@
     </row>
     <row r="318" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A318" s="26"/>
-      <c r="B318" s="30">
+      <c r="B318">
         <v>3260</v>
       </c>
       <c r="C318" t="s">
@@ -6802,7 +6794,7 @@
     </row>
     <row r="319" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A319" s="26"/>
-      <c r="B319" s="30">
+      <c r="B319">
         <v>3270</v>
       </c>
       <c r="C319" t="s">
@@ -6811,7 +6803,7 @@
     </row>
     <row r="320" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A320" s="26"/>
-      <c r="B320" s="30">
+      <c r="B320">
         <v>3280</v>
       </c>
       <c r="C320" t="s">
@@ -6820,7 +6812,7 @@
     </row>
     <row r="321" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A321" s="26"/>
-      <c r="B321" s="30">
+      <c r="B321">
         <v>3290</v>
       </c>
       <c r="C321" t="s">
@@ -6829,7 +6821,7 @@
     </row>
     <row r="322" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A322" s="26"/>
-      <c r="B322" s="30">
+      <c r="B322">
         <v>3300</v>
       </c>
       <c r="C322" t="s">
@@ -6838,7 +6830,7 @@
     </row>
     <row r="323" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A323" s="26"/>
-      <c r="B323" s="30">
+      <c r="B323">
         <v>3310</v>
       </c>
       <c r="C323" s="11" t="s">
@@ -6849,7 +6841,7 @@
       <c r="A324" s="28" t="s">
         <v>756</v>
       </c>
-      <c r="B324" s="30">
+      <c r="B324">
         <v>3320</v>
       </c>
       <c r="C324" s="11" t="str">
@@ -6859,7 +6851,7 @@
     </row>
     <row r="325" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A325" s="26"/>
-      <c r="B325" s="30">
+      <c r="B325">
         <v>3330</v>
       </c>
       <c r="C325" s="11" t="str">
@@ -6872,7 +6864,7 @@
     </row>
     <row r="326" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A326" s="26"/>
-      <c r="B326" s="30">
+      <c r="B326">
         <v>3340</v>
       </c>
       <c r="C326" s="11" t="s">
@@ -6881,7 +6873,7 @@
     </row>
     <row r="327" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A327" s="26"/>
-      <c r="B327" s="30">
+      <c r="B327">
         <v>3350</v>
       </c>
       <c r="C327" s="11" t="s">
@@ -6890,7 +6882,7 @@
     </row>
     <row r="328" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A328" s="26"/>
-      <c r="B328" s="30">
+      <c r="B328">
         <v>3360</v>
       </c>
       <c r="C328" s="11" t="str">
@@ -6904,7 +6896,7 @@
     </row>
     <row r="329" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A329" s="26"/>
-      <c r="B329" s="30">
+      <c r="B329">
         <v>3370</v>
       </c>
       <c r="C329" s="11" t="s">
@@ -6916,7 +6908,7 @@
         <f>_xlfn.CONCAT(A324,".SUBEND")</f>
         <v>CHECKDUP.SUBEND</v>
       </c>
-      <c r="B330" s="30">
+      <c r="B330">
         <v>3380</v>
       </c>
       <c r="C330" s="11" t="s">
@@ -6927,7 +6919,7 @@
       <c r="A331" s="28" t="s">
         <v>694</v>
       </c>
-      <c r="B331" s="30">
+      <c r="B331">
         <v>3390</v>
       </c>
       <c r="C331" s="11" t="str">
@@ -6937,7 +6929,7 @@
     </row>
     <row r="332" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A332" s="26"/>
-      <c r="B332" s="30">
+      <c r="B332">
         <v>3400</v>
       </c>
       <c r="C332" s="11" t="str">
@@ -6950,7 +6942,7 @@
     </row>
     <row r="333" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A333" s="26"/>
-      <c r="B333" s="30">
+      <c r="B333">
         <v>3410</v>
       </c>
       <c r="C333" s="11" t="s">
@@ -6959,7 +6951,7 @@
     </row>
     <row r="334" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A334" s="26"/>
-      <c r="B334" s="30">
+      <c r="B334">
         <v>3420</v>
       </c>
       <c r="C334" s="11" t="s">
@@ -6968,7 +6960,7 @@
     </row>
     <row r="335" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A335" s="26"/>
-      <c r="B335" s="30">
+      <c r="B335">
         <v>3430</v>
       </c>
       <c r="C335" s="11" t="s">
@@ -6977,7 +6969,7 @@
     </row>
     <row r="336" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A336" s="26"/>
-      <c r="B336" s="30">
+      <c r="B336">
         <v>3440</v>
       </c>
       <c r="C336" s="11" t="s">
@@ -6986,7 +6978,7 @@
     </row>
     <row r="337" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A337" s="26"/>
-      <c r="B337" s="30">
+      <c r="B337">
         <v>3450</v>
       </c>
       <c r="C337" s="11" t="s">
@@ -6995,7 +6987,7 @@
     </row>
     <row r="338" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A338" s="26"/>
-      <c r="B338" s="30">
+      <c r="B338">
         <v>3460</v>
       </c>
       <c r="C338" s="28" t="str">
@@ -7012,7 +7004,7 @@
     </row>
     <row r="339" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A339" s="26"/>
-      <c r="B339" s="30">
+      <c r="B339">
         <v>3470</v>
       </c>
       <c r="C339" s="11" t="s">
@@ -7023,7 +7015,7 @@
       <c r="A340" s="28" t="s">
         <v>703</v>
       </c>
-      <c r="B340" s="30">
+      <c r="B340">
         <v>3480</v>
       </c>
       <c r="C340" s="11" t="str">
@@ -7033,7 +7025,7 @@
     </row>
     <row r="341" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A341" s="26"/>
-      <c r="B341" s="30">
+      <c r="B341">
         <v>3490</v>
       </c>
       <c r="C341" s="11" t="str">
@@ -7046,7 +7038,7 @@
     </row>
     <row r="342" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A342" s="26"/>
-      <c r="B342" s="30">
+      <c r="B342">
         <v>3500</v>
       </c>
       <c r="C342" t="s">
@@ -7055,7 +7047,7 @@
     </row>
     <row r="343" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A343" s="26"/>
-      <c r="B343" s="30">
+      <c r="B343">
         <v>3510</v>
       </c>
       <c r="C343" t="str">
@@ -7069,7 +7061,7 @@
     </row>
     <row r="344" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A344" s="26"/>
-      <c r="B344" s="30">
+      <c r="B344">
         <v>3520</v>
       </c>
       <c r="C344" t="s">
@@ -7078,7 +7070,7 @@
     </row>
     <row r="345" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A345" s="26"/>
-      <c r="B345" s="30">
+      <c r="B345">
         <v>3530</v>
       </c>
       <c r="C345" t="str">
@@ -7092,7 +7084,7 @@
     </row>
     <row r="346" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A346" s="26"/>
-      <c r="B346" s="30">
+      <c r="B346">
         <v>3540</v>
       </c>
       <c r="C346" s="11" t="s">
@@ -7104,7 +7096,7 @@
         <f>_xlfn.CONCAT(A340,".SUBEND")</f>
         <v>CALCSCORE.SUBEND</v>
       </c>
-      <c r="B347" s="30">
+      <c r="B347">
         <v>3550</v>
       </c>
       <c r="C347" s="11" t="s">
@@ -7115,7 +7107,7 @@
       <c r="A348" s="28" t="s">
         <v>614</v>
       </c>
-      <c r="B348" s="30">
+      <c r="B348">
         <v>3560</v>
       </c>
       <c r="C348" s="11" t="str">
@@ -7125,7 +7117,7 @@
     </row>
     <row r="349" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A349" s="26"/>
-      <c r="B349" s="30">
+      <c r="B349">
         <v>3570</v>
       </c>
       <c r="C349" s="11" t="str">
@@ -7138,7 +7130,7 @@
     </row>
     <row r="350" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A350" s="26"/>
-      <c r="B350" s="30">
+      <c r="B350">
         <v>3580</v>
       </c>
       <c r="C350" t="s">
@@ -7147,7 +7139,7 @@
     </row>
     <row r="351" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A351" s="26"/>
-      <c r="B351" s="30">
+      <c r="B351">
         <v>3590</v>
       </c>
       <c r="C351" t="str">
@@ -7164,7 +7156,7 @@
     </row>
     <row r="352" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A352" s="26"/>
-      <c r="B352" s="30">
+      <c r="B352">
         <v>3600</v>
       </c>
       <c r="C352" t="s">
@@ -7173,7 +7165,7 @@
     </row>
     <row r="353" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A353" s="26"/>
-      <c r="B353" s="30">
+      <c r="B353">
         <v>3610</v>
       </c>
       <c r="C353" t="s">
@@ -7182,7 +7174,7 @@
     </row>
     <row r="354" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A354" s="26"/>
-      <c r="B354" s="30">
+      <c r="B354">
         <v>3620</v>
       </c>
       <c r="C354" t="str">
@@ -7199,7 +7191,7 @@
     </row>
     <row r="355" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A355" s="26"/>
-      <c r="B355" s="30">
+      <c r="B355">
         <v>3630</v>
       </c>
       <c r="C355" t="s">
@@ -7208,7 +7200,7 @@
     </row>
     <row r="356" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A356" s="26"/>
-      <c r="B356" s="30">
+      <c r="B356">
         <v>3640</v>
       </c>
       <c r="C356" t="s">
@@ -7217,7 +7209,7 @@
     </row>
     <row r="357" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A357" s="26"/>
-      <c r="B357" s="30">
+      <c r="B357">
         <v>3650</v>
       </c>
       <c r="C357" t="s">
@@ -7226,7 +7218,7 @@
     </row>
     <row r="358" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A358" s="26"/>
-      <c r="B358" s="30">
+      <c r="B358">
         <v>3660</v>
       </c>
       <c r="C358" t="s">
@@ -7235,7 +7227,7 @@
     </row>
     <row r="359" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A359" s="26"/>
-      <c r="B359" s="30">
+      <c r="B359">
         <v>3670</v>
       </c>
       <c r="C359" t="s">
@@ -7246,7 +7238,7 @@
       <c r="A360" s="28" t="s">
         <v>700</v>
       </c>
-      <c r="B360" s="30">
+      <c r="B360">
         <v>3680</v>
       </c>
       <c r="C360" s="11" t="str">
@@ -7256,7 +7248,7 @@
     </row>
     <row r="361" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A361" s="26"/>
-      <c r="B361" s="30">
+      <c r="B361">
         <v>3690</v>
       </c>
       <c r="C361" s="11" t="str">
@@ -7266,7 +7258,7 @@
     </row>
     <row r="362" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A362" s="26"/>
-      <c r="B362" s="30">
+      <c r="B362">
         <v>3700</v>
       </c>
       <c r="C362" t="s">
@@ -7275,7 +7267,7 @@
     </row>
     <row r="363" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A363" s="26"/>
-      <c r="B363" s="30">
+      <c r="B363">
         <v>3710</v>
       </c>
       <c r="C363" t="s">
@@ -7284,7 +7276,7 @@
     </row>
     <row r="364" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A364" s="26"/>
-      <c r="B364" s="30">
+      <c r="B364">
         <v>3720</v>
       </c>
       <c r="C364" s="11" t="s">
@@ -7293,7 +7285,7 @@
     </row>
     <row r="365" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A365" s="26"/>
-      <c r="B365" s="30">
+      <c r="B365">
         <v>3730</v>
       </c>
       <c r="C365" t="s">
@@ -7304,7 +7296,7 @@
       <c r="A366" s="28" t="s">
         <v>809</v>
       </c>
-      <c r="B366" s="30">
+      <c r="B366">
         <v>3740</v>
       </c>
       <c r="C366" t="str">
@@ -7313,7 +7305,7 @@
       </c>
     </row>
     <row r="367" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B367" s="30">
+      <c r="B367">
         <v>3750</v>
       </c>
       <c r="C367" t="str">
@@ -7325,7 +7317,7 @@
       </c>
     </row>
     <row r="368" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B368" s="30">
+      <c r="B368">
         <v>3760</v>
       </c>
       <c r="C368" s="11" t="s">
@@ -7333,7 +7325,7 @@
       </c>
     </row>
     <row r="369" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B369" s="30">
+      <c r="B369">
         <v>3770</v>
       </c>
       <c r="C369" s="11" t="s">
@@ -7344,7 +7336,7 @@
       <c r="A370" s="28" t="s">
         <v>808</v>
       </c>
-      <c r="B370" s="30">
+      <c r="B370">
         <v>3780</v>
       </c>
       <c r="C370" t="str">
@@ -7353,7 +7345,7 @@
       </c>
     </row>
     <row r="371" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B371" s="30">
+      <c r="B371">
         <v>3790</v>
       </c>
       <c r="C371" t="str">
@@ -7365,7 +7357,7 @@
       </c>
     </row>
     <row r="372" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B372" s="30">
+      <c r="B372">
         <v>3800</v>
       </c>
       <c r="C372" s="11" t="s">
@@ -7373,7 +7365,7 @@
       </c>
     </row>
     <row r="373" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B373" s="30">
+      <c r="B373">
         <v>3810</v>
       </c>
       <c r="C373" s="11" t="s">
@@ -7384,7 +7376,7 @@
       <c r="A374" s="28" t="s">
         <v>807</v>
       </c>
-      <c r="B374" s="30">
+      <c r="B374">
         <v>3820</v>
       </c>
       <c r="C374" t="str">
@@ -7393,7 +7385,7 @@
       </c>
     </row>
     <row r="375" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B375" s="30">
+      <c r="B375">
         <v>3830</v>
       </c>
       <c r="C375" t="str">
@@ -7405,7 +7397,7 @@
       </c>
     </row>
     <row r="376" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B376" s="30">
+      <c r="B376">
         <v>3840</v>
       </c>
       <c r="C376" s="11" t="s">
@@ -7413,7 +7405,7 @@
       </c>
     </row>
     <row r="377" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B377" s="30">
+      <c r="B377">
         <v>3850</v>
       </c>
       <c r="C377" s="11" t="s">
@@ -7424,7 +7416,7 @@
       <c r="A378" s="28" t="s">
         <v>806</v>
       </c>
-      <c r="B378" s="30">
+      <c r="B378">
         <v>3860</v>
       </c>
       <c r="C378" t="str">
@@ -7433,7 +7425,7 @@
       </c>
     </row>
     <row r="379" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B379" s="30">
+      <c r="B379">
         <v>3870</v>
       </c>
       <c r="C379" t="str">
@@ -7445,7 +7437,7 @@
       </c>
     </row>
     <row r="380" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B380" s="30">
+      <c r="B380">
         <v>3880</v>
       </c>
       <c r="C380" s="11" t="s">
@@ -7453,7 +7445,7 @@
       </c>
     </row>
     <row r="381" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B381" s="30">
+      <c r="B381">
         <v>3890</v>
       </c>
       <c r="C381" s="11" t="s">
@@ -7464,7 +7456,7 @@
       <c r="A382" s="28" t="s">
         <v>805</v>
       </c>
-      <c r="B382" s="30">
+      <c r="B382">
         <v>3900</v>
       </c>
       <c r="C382" t="str">
@@ -7473,7 +7465,7 @@
       </c>
     </row>
     <row r="383" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B383" s="30">
+      <c r="B383">
         <v>3910</v>
       </c>
       <c r="C383" t="str">
@@ -7485,7 +7477,7 @@
       </c>
     </row>
     <row r="384" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B384" s="30">
+      <c r="B384">
         <v>3920</v>
       </c>
       <c r="C384" s="11" t="s">
@@ -7493,7 +7485,7 @@
       </c>
     </row>
     <row r="385" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B385" s="30">
+      <c r="B385">
         <v>3930</v>
       </c>
       <c r="C385" s="11" t="s">
@@ -7504,7 +7496,7 @@
       <c r="A386" s="28" t="s">
         <v>804</v>
       </c>
-      <c r="B386" s="30">
+      <c r="B386">
         <v>3940</v>
       </c>
       <c r="C386" t="str">
@@ -7513,7 +7505,7 @@
       </c>
     </row>
     <row r="387" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B387" s="30">
+      <c r="B387">
         <v>3950</v>
       </c>
       <c r="C387" t="str">
@@ -7525,7 +7517,7 @@
       </c>
     </row>
     <row r="388" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B388" s="30">
+      <c r="B388">
         <v>3960</v>
       </c>
       <c r="C388" s="11" t="s">
@@ -7533,7 +7525,7 @@
       </c>
     </row>
     <row r="389" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B389" s="30">
+      <c r="B389">
         <v>3970</v>
       </c>
       <c r="C389" s="11" t="s">
@@ -7544,7 +7536,7 @@
       <c r="A390" s="28" t="s">
         <v>801</v>
       </c>
-      <c r="B390" s="30">
+      <c r="B390">
         <v>3980</v>
       </c>
       <c r="C390" t="str">
@@ -7553,7 +7545,7 @@
       </c>
     </row>
     <row r="391" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B391" s="30">
+      <c r="B391">
         <v>3990</v>
       </c>
       <c r="C391" t="str">
@@ -7565,7 +7557,7 @@
       </c>
     </row>
     <row r="392" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B392" s="30">
+      <c r="B392">
         <v>4000</v>
       </c>
       <c r="C392" s="11" t="s">
@@ -7573,7 +7565,7 @@
       </c>
     </row>
     <row r="393" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B393" s="30">
+      <c r="B393">
         <v>4010</v>
       </c>
       <c r="C393" s="11" t="s">
@@ -7584,7 +7576,7 @@
       <c r="A394" s="28" t="s">
         <v>802</v>
       </c>
-      <c r="B394" s="30">
+      <c r="B394">
         <v>4020</v>
       </c>
       <c r="C394" t="str">
@@ -7593,7 +7585,7 @@
       </c>
     </row>
     <row r="395" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B395" s="30">
+      <c r="B395">
         <v>4030</v>
       </c>
       <c r="C395" t="str">
@@ -7605,7 +7597,7 @@
       </c>
     </row>
     <row r="396" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B396" s="30">
+      <c r="B396">
         <v>4040</v>
       </c>
       <c r="C396" s="11" t="s">
@@ -7613,7 +7605,7 @@
       </c>
     </row>
     <row r="397" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B397" s="30">
+      <c r="B397">
         <v>4050</v>
       </c>
       <c r="C397" s="11" t="s">
@@ -7624,7 +7616,7 @@
       <c r="A398" s="28" t="s">
         <v>803</v>
       </c>
-      <c r="B398" s="30">
+      <c r="B398">
         <v>4060</v>
       </c>
       <c r="C398" t="str">
@@ -7633,7 +7625,7 @@
       </c>
     </row>
     <row r="399" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B399" s="30">
+      <c r="B399">
         <v>4070</v>
       </c>
       <c r="C399" t="str">
@@ -7645,7 +7637,7 @@
       </c>
     </row>
     <row r="400" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B400" s="30">
+      <c r="B400">
         <v>4080</v>
       </c>
       <c r="C400" s="11" t="s">
@@ -7653,7 +7645,7 @@
       </c>
     </row>
     <row r="401" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B401" s="30">
+      <c r="B401">
         <v>4090</v>
       </c>
       <c r="C401" s="11" t="s">
@@ -7664,7 +7656,7 @@
       <c r="A402" s="28" t="s">
         <v>811</v>
       </c>
-      <c r="B402" s="30">
+      <c r="B402">
         <v>4100</v>
       </c>
       <c r="C402" t="str">
@@ -7673,7 +7665,7 @@
       </c>
     </row>
     <row r="403" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B403" s="30">
+      <c r="B403">
         <v>4110</v>
       </c>
       <c r="C403" t="str">
@@ -7685,7 +7677,7 @@
       </c>
     </row>
     <row r="404" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B404" s="30">
+      <c r="B404">
         <v>4120</v>
       </c>
       <c r="C404" s="11" t="s">
@@ -7693,7 +7685,7 @@
       </c>
     </row>
     <row r="405" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B405" s="30">
+      <c r="B405">
         <v>4130</v>
       </c>
       <c r="C405" s="11" t="s">

</xml_diff>